<commit_message>
Started refactoring type tests and test suite
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -62,9 +62,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>type-name-codeSimpleType-invalid</t>
-  </si>
-  <si>
     <t>Code simple types</t>
   </si>
   <si>
@@ -224,21 +221,12 @@
     <t>List types</t>
   </si>
   <si>
-    <t>type-name-codeType-invalid</t>
-  </si>
-  <si>
-    <t>A type with a name that ends with "CodeType" must have a base type with a name that ends with "CodeSimpleType".</t>
-  </si>
-  <si>
     <t>Code types</t>
   </si>
   <si>
     <t>10-18</t>
   </si>
   <si>
-    <t>type-name-codeType-inconsistent</t>
-  </si>
-  <si>
     <t>A CSC type with a "CodeSimpleType" base should be named similarly, with the name ending in "CodeType".</t>
   </si>
   <si>
@@ -263,9 +251,6 @@
     <t>10-49</t>
   </si>
   <si>
-    <t>type-name-term-defined</t>
-  </si>
-  <si>
     <t>A term in a type name that does not exist in the dictionary must be defined as "Local Terminology".</t>
   </si>
   <si>
@@ -519,13 +504,28 @@
   </si>
   <si>
     <t>type-name-repTerm-complex</t>
+  </si>
+  <si>
+    <t>type-name-repTerm-codeSimpleType</t>
+  </si>
+  <si>
+    <t>type-name-repTerm-codeType</t>
+  </si>
+  <si>
+    <t>type-name-inconsistent-codeType</t>
+  </si>
+  <si>
+    <t>type-name-term-undefined</t>
+  </si>
+  <si>
+    <t>A complex type with a name that ends with "CodeType" must have a base type with a name that ends with "CodeSimpleType".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,8 +553,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,6 +584,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -587,12 +599,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,10 +629,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -1031,7 +1048,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,46 +1084,46 @@
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="N1"/>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1119,19 +1136,19 @@
     </row>
     <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1144,19 +1161,19 @@
     </row>
     <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1169,19 +1186,19 @@
     </row>
     <row r="5" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1194,44 +1211,44 @@
     </row>
     <row r="6" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1244,19 +1261,19 @@
     </row>
     <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1269,19 +1286,19 @@
     </row>
     <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1294,44 +1311,44 @@
     </row>
     <row r="10" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1344,19 +1361,19 @@
     </row>
     <row r="12" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1369,19 +1386,19 @@
     </row>
     <row r="13" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -1394,19 +1411,19 @@
     </row>
     <row r="14" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
@@ -1419,22 +1436,22 @@
     </row>
     <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1447,22 +1464,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1471,30 +1488,30 @@
         <v>3</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1503,50 +1520,50 @@
         <v>3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
@@ -1555,10 +1572,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -1567,18 +1584,18 @@
         <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>163</v>
+      <c r="A20" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -1587,30 +1604,30 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>164</v>
+      <c r="A21" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
@@ -1619,10 +1636,10 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -1634,11 +1651,11 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>12</v>
+      <c r="A22" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
@@ -1647,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -1659,15 +1676,15 @@
         <v>3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
@@ -1676,10 +1693,10 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -1692,7 +1709,7 @@
     </row>
     <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
@@ -1701,10 +1718,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -1717,7 +1734,7 @@
     </row>
     <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
@@ -1726,10 +1743,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -1742,7 +1759,7 @@
     </row>
     <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
@@ -1751,10 +1768,10 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -1765,84 +1782,84 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -1855,50 +1872,50 @@
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -1907,30 +1924,30 @@
         <v>3</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -1943,22 +1960,22 @@
     </row>
     <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -1970,27 +1987,27 @@
         <v>6</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2002,7 +2019,7 @@
         <v>6</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K34"/>
       <c r="L34"/>
@@ -2011,114 +2028,114 @@
     </row>
     <row r="35" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I36" t="s">
         <v>6</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -2131,22 +2148,22 @@
     </row>
     <row r="39" spans="1:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -2159,19 +2176,19 @@
     </row>
     <row r="40" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2184,19 +2201,19 @@
     </row>
     <row r="41" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2209,19 +2226,19 @@
     </row>
     <row r="42" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2234,22 +2251,22 @@
     </row>
     <row r="43" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -2262,22 +2279,22 @@
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2290,22 +2307,22 @@
     </row>
     <row r="45" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2318,22 +2335,22 @@
     </row>
     <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2346,19 +2363,19 @@
     </row>
     <row r="47" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2371,19 +2388,19 @@
     </row>
     <row r="48" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2396,19 +2413,19 @@
     </row>
     <row r="49" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -2421,19 +2438,19 @@
     </row>
     <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -2446,22 +2463,22 @@
     </row>
     <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D51" t="s">
-        <v>104</v>
-      </c>
-      <c r="E51" t="s">
-        <v>23</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -2474,22 +2491,22 @@
     </row>
     <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -2502,22 +2519,22 @@
     </row>
     <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D53" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -2530,22 +2547,22 @@
     </row>
     <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -2558,22 +2575,22 @@
     </row>
     <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -2586,22 +2603,22 @@
     </row>
     <row r="56" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -2613,27 +2630,27 @@
         <v>6</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>99</v>
+      </c>
+      <c r="E57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D57" t="s">
-        <v>104</v>
-      </c>
-      <c r="E57" t="s">
-        <v>105</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -2646,50 +2663,50 @@
     </row>
     <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E58" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
     </row>
     <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -2701,55 +2718,55 @@
         <v>6</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E61" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Refactored reference tests into unit tests; made all async.
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,15 +176,9 @@
     <t>A type must have a valid namespace prefix.</t>
   </si>
   <si>
-    <t>A type name must use valid characters.</t>
-  </si>
-  <si>
     <t>10-45</t>
   </si>
   <si>
-    <t>A type name must end with the representation term "Type".</t>
-  </si>
-  <si>
     <t>11-1</t>
   </si>
   <si>
@@ -197,27 +191,15 @@
     <t>Complex types</t>
   </si>
   <si>
-    <t>An augmentation type name must end with the representation term "AugmentationType".</t>
-  </si>
-  <si>
     <t>Augmentation types</t>
   </si>
   <si>
-    <t>An association type name must end with the representation term "AssociationType".</t>
-  </si>
-  <si>
     <t>Association types</t>
   </si>
   <si>
-    <t>A metadata type name must end with the representation term "MetadataType".</t>
-  </si>
-  <si>
     <t>Metadata types</t>
   </si>
   <si>
-    <t>A simple list type name must end with the representation term "ListSimpleType".</t>
-  </si>
-  <si>
     <t>List types</t>
   </si>
   <si>
@@ -227,33 +209,9 @@
     <t>10-18</t>
   </si>
   <si>
-    <t>A CSC type with a "CodeSimpleType" base should be named similarly, with the name ending in "CodeType".</t>
-  </si>
-  <si>
-    <t>type-name-all-duplicate</t>
-  </si>
-  <si>
-    <t>A type name cannot be duplicated in the given namespace.</t>
-  </si>
-  <si>
-    <t>type-name-term-type</t>
-  </si>
-  <si>
-    <t>A type name should not use the term "Type" other than as its final representation term.</t>
-  </si>
-  <si>
-    <t>type-name-all-camelCase</t>
-  </si>
-  <si>
-    <t>A type name must begin with an upper case letter.</t>
-  </si>
-  <si>
     <t>10-49</t>
   </si>
   <si>
-    <t>A term in a type name that does not exist in the dictionary must be defined as "Local Terminology".</t>
-  </si>
-  <si>
     <t>type-def-term-defined</t>
   </si>
   <si>
@@ -404,12 +362,6 @@
     <t>A facet must have a valid style (e.g., enumeration, pattern, etc.).</t>
   </si>
   <si>
-    <t>A simple type must have a name.</t>
-  </si>
-  <si>
-    <t>A complex type must have a name.</t>
-  </si>
-  <si>
     <t>9-25</t>
   </si>
   <si>
@@ -464,15 +416,6 @@
     <t>A term in a property definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
   </si>
   <si>
-    <t>A simple type name must end with the representation term "SimpleType".</t>
-  </si>
-  <si>
-    <t>A complex type name must not end with the representation term "SimpleType".</t>
-  </si>
-  <si>
-    <t>A simple type with a name that ends with "CodeSimpleType" must declare enumerations.</t>
-  </si>
-  <si>
     <t>A term in a type definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
   </si>
   <si>
@@ -485,47 +428,104 @@
     <t>NDR 4.0</t>
   </si>
   <si>
-    <t>type-name-missing-simple</t>
-  </si>
-  <si>
-    <t>type-name-missing-complex</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>type-name-invalidChar</t>
-  </si>
-  <si>
-    <t>type-name-repTerm</t>
-  </si>
-  <si>
-    <t>type-name-repTerm-simple</t>
-  </si>
-  <si>
-    <t>type-name-repTerm-complex</t>
-  </si>
-  <si>
-    <t>type-name-repTerm-codeSimpleType</t>
-  </si>
-  <si>
-    <t>type-name-repTerm-codeType</t>
-  </si>
-  <si>
-    <t>type-name-inconsistent-codeType</t>
-  </si>
-  <si>
-    <t>type-name-term-undefined</t>
-  </si>
-  <si>
-    <t>A complex type with a name that ends with "CodeType" must have a base type with a name that ends with "CodeSimpleType".</t>
+    <t>Simple types must have a name.</t>
+  </si>
+  <si>
+    <t>Complex types must have a name.</t>
+  </si>
+  <si>
+    <t>Type names must use valid characters.</t>
+  </si>
+  <si>
+    <t>Type names must end with the representation term "Type".</t>
+  </si>
+  <si>
+    <t>Simple type names must end with the representation term "SimpleType".</t>
+  </si>
+  <si>
+    <t>Complex type names must not end with the representation term "SimpleType".</t>
+  </si>
+  <si>
+    <t>Simple types that use the representation term "CodeSimpleType" must declare codes.</t>
+  </si>
+  <si>
+    <t>Augmentation type names must end with the representation term "AugmentationType".</t>
+  </si>
+  <si>
+    <t>Association type names must end with the representation term "AssociationType".</t>
+  </si>
+  <si>
+    <t>Metadata type names must end with the representation term "MetadataType".</t>
+  </si>
+  <si>
+    <t>Simple list type names must end with the representation term "ListSimpleType".</t>
+  </si>
+  <si>
+    <t>Complex types that use the representation term "CodeType" must have a base type that uses the representation term "CodeSimpleType".</t>
+  </si>
+  <si>
+    <t>Complex types that use the representation term "CodeType" should be named similarly to their base type.</t>
+  </si>
+  <si>
+    <t>Type names must not overlap in a namespace.</t>
+  </si>
+  <si>
+    <t>Type names should not use the term "Type" in the name other than as the final representation term.</t>
+  </si>
+  <si>
+    <t>type_name_missing_simple</t>
+  </si>
+  <si>
+    <t>type_name_missing_complex</t>
+  </si>
+  <si>
+    <t>type_name_invalidChar</t>
+  </si>
+  <si>
+    <t>type_name_repTerm</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_simple</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_complex</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_codeSimpleType</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_codeType</t>
+  </si>
+  <si>
+    <t>type_name_inconsistent_codeType</t>
+  </si>
+  <si>
+    <t>type_name_duplicate</t>
+  </si>
+  <si>
+    <t>type_name_camelCase</t>
+  </si>
+  <si>
+    <t>type_name_term_undefined</t>
+  </si>
+  <si>
+    <t>type_name_reservedTerm_type</t>
+  </si>
+  <si>
+    <t>Type names must begin with an upper case letter.</t>
+  </si>
+  <si>
+    <t>Type names must use terms that either have standard dictionary entries or are custom defined as Local Terminology.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,15 +553,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,11 +577,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -599,13 +587,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,14 +616,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -1047,8 +1030,8 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,13 +1088,13 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="N1"/>
     </row>
     <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -1311,7 +1294,7 @@
     </row>
     <row r="10" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
@@ -1464,10 +1447,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1479,7 +1462,7 @@
         <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1488,18 +1471,18 @@
         <v>3</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1511,7 +1494,7 @@
         <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1520,18 +1503,18 @@
         <v>3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
@@ -1552,18 +1535,18 @@
         <v>3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
@@ -1584,18 +1567,18 @@
         <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -1607,7 +1590,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -1616,18 +1599,18 @@
         <v>3</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
@@ -1639,7 +1622,7 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -1651,11 +1634,11 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>160</v>
+      <c r="A22" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
@@ -1676,15 +1659,15 @@
         <v>3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
@@ -1696,7 +1679,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -1709,7 +1692,7 @@
     </row>
     <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
@@ -1721,7 +1704,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -1734,7 +1717,7 @@
     </row>
     <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
@@ -1746,7 +1729,7 @@
         <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -1759,7 +1742,7 @@
     </row>
     <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
@@ -1771,7 +1754,7 @@
         <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -1784,10 +1767,10 @@
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>7</v>
@@ -1799,7 +1782,7 @@
         <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -1808,18 +1791,18 @@
         <v>35</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>162</v>
+      <c r="A28" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>20</v>
@@ -1831,7 +1814,7 @@
         <v>23</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -1844,10 +1827,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>68</v>
+        <v>159</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1872,10 +1855,10 @@
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>70</v>
+        <v>162</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -1900,10 +1883,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -1924,18 +1907,18 @@
         <v>3</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -1960,10 +1943,10 @@
     </row>
     <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>18</v>
@@ -1975,7 +1958,7 @@
         <v>24</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -1987,15 +1970,15 @@
         <v>6</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
@@ -2007,7 +1990,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2019,7 +2002,7 @@
         <v>6</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="K34"/>
       <c r="L34"/>
@@ -2028,10 +2011,10 @@
     </row>
     <row r="35" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>45</v>
@@ -2043,7 +2026,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2055,15 +2038,15 @@
         <v>6</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>45</v>
@@ -2075,7 +2058,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2087,15 +2070,15 @@
         <v>6</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>20</v>
@@ -2120,10 +2103,10 @@
     </row>
     <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>18</v>
@@ -2148,10 +2131,10 @@
     </row>
     <row r="39" spans="1:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>20</v>
@@ -2176,7 +2159,7 @@
     </row>
     <row r="40" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>20</v>
@@ -2188,7 +2171,7 @@
         <v>46</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2201,7 +2184,7 @@
     </row>
     <row r="41" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>20</v>
@@ -2213,7 +2196,7 @@
         <v>46</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2226,7 +2209,7 @@
     </row>
     <row r="42" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>20</v>
@@ -2238,7 +2221,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2251,10 +2234,10 @@
     </row>
     <row r="43" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>18</v>
@@ -2266,7 +2249,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -2279,10 +2262,10 @@
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>20</v>
@@ -2294,7 +2277,7 @@
         <v>47</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2307,10 +2290,10 @@
     </row>
     <row r="45" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>20</v>
@@ -2322,7 +2305,7 @@
         <v>47</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2335,10 +2318,10 @@
     </row>
     <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>39</v>
@@ -2363,7 +2346,7 @@
     </row>
     <row r="47" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>20</v>
@@ -2375,7 +2358,7 @@
         <v>47</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2388,7 +2371,7 @@
     </row>
     <row r="48" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>20</v>
@@ -2400,7 +2383,7 @@
         <v>47</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2413,7 +2396,7 @@
     </row>
     <row r="49" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
@@ -2425,7 +2408,7 @@
         <v>47</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -2438,7 +2421,7 @@
     </row>
     <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>20</v>
@@ -2450,7 +2433,7 @@
         <v>47</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -2463,16 +2446,16 @@
     </row>
     <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E51" t="s">
         <v>22</v>
@@ -2491,16 +2474,16 @@
     </row>
     <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E52" t="s">
         <v>22</v>
@@ -2519,16 +2502,16 @@
     </row>
     <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E53" t="s">
         <v>23</v>
@@ -2547,16 +2530,16 @@
     </row>
     <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E54" t="s">
         <v>23</v>
@@ -2575,16 +2558,16 @@
     </row>
     <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E55" t="s">
         <v>23</v>
@@ -2603,22 +2586,22 @@
     </row>
     <row r="56" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E56" t="s">
         <v>23</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -2630,24 +2613,24 @@
         <v>6</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>19</v>
@@ -2663,19 +2646,19 @@
     </row>
     <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>19</v>
@@ -2691,22 +2674,22 @@
     </row>
     <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E59" t="s">
         <v>24</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -2718,52 +2701,52 @@
         <v>6</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated niem-test-suite dependency and moved JSDoc examples to test spreadsheet for better reuse
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="179">
   <si>
     <t>Field</t>
   </si>
@@ -470,9 +470,6 @@
     <t>Complex types that use the representation term "CodeType" should be named similarly to their base type.</t>
   </si>
   <si>
-    <t>Type names must not overlap in a namespace.</t>
-  </si>
-  <si>
     <t>Type names should not use the term "Type" in the name other than as the final representation term.</t>
   </si>
   <si>
@@ -485,9 +482,6 @@
     <t>type_name_invalidChar</t>
   </si>
   <si>
-    <t>type_name_repTerm</t>
-  </si>
-  <si>
     <t>type_name_repTerm_simple</t>
   </si>
   <si>
@@ -519,13 +513,61 @@
   </si>
   <si>
     <t>Type names must use terms that either have standard dictionary entries or are custom defined as Local Terminology.</t>
+  </si>
+  <si>
+    <t>Type name 'HairColorCodeType' is valid with base type 'HairColorCodeSimpleType'.</t>
+  </si>
+  <si>
+    <t>Type name 'HairColorCodeType' is not recommended with base type 'EyeColorCodeSimpleType'.</t>
+  </si>
+  <si>
+    <t>Type name "PersonType" uses valid characters.</t>
+  </si>
+  <si>
+    <t>Type name "ID#Type" does not use valid characters.</t>
+  </si>
+  <si>
+    <t>Type name 'WeekdayCodeSimpleType' is valid if the type declares codes.</t>
+  </si>
+  <si>
+    <t>Type name 'WeekdayCodeSimpleType' is not valid if the type does not declare codes.</t>
+  </si>
+  <si>
+    <t>Type name 'WeekdayCodeType' is not valid with base type 'string'</t>
+  </si>
+  <si>
+    <t>Type name 'IDSimpleType' is valid if the type is simple.</t>
+  </si>
+  <si>
+    <t>Type name 'IDSimpleType' is not valid if the type is complex.</t>
+  </si>
+  <si>
+    <t>Type name 'IDType' is not valid if the type is simple.</t>
+  </si>
+  <si>
+    <t>Type name 'PersonType' is valid.</t>
+  </si>
+  <si>
+    <t>Type name 'Person' is not valid.</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_type</t>
+  </si>
+  <si>
+    <t>Valid Example</t>
+  </si>
+  <si>
+    <t>Invalid Example</t>
+  </si>
+  <si>
+    <t>Type names must not occur more than once in a single namespace.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,8 +595,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,6 +626,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -587,12 +641,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,57 +671,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -718,6 +749,54 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -732,8 +811,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M61" totalsRowShown="0">
-  <autoFilter ref="A1:M61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O61" totalsRowShown="0">
+  <autoFilter ref="A1:O61">
     <filterColumn colId="3">
       <filters>
         <filter val="Type"/>
@@ -745,20 +824,22 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="13">
-    <tableColumn id="1" name="ID" dataDxfId="8" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="7"/>
-    <tableColumn id="17" name="Category" dataDxfId="6"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="14"/>
+    <tableColumn id="17" name="Category" dataDxfId="13"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="5"/>
+    <tableColumn id="14" name="Scope" dataDxfId="12"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="4"/>
-    <tableColumn id="18" name="Rules" dataDxfId="3"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" name="Notes" dataDxfId="0"/>
+    <tableColumn id="21" name="Spec" dataDxfId="11"/>
+    <tableColumn id="18" name="Rules" dataDxfId="10"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="1"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="0"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="9"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="8"/>
+    <tableColumn id="19" name="Notes" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1027,11 +1108,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,13 +1127,14 @@
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="9" width="11.88671875" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" style="7" customWidth="1"/>
-    <col min="11" max="12" width="26.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1"/>
-    <col min="15" max="15" width="31.5546875" customWidth="1"/>
+    <col min="11" max="12" width="34.77734375" style="7" customWidth="1"/>
+    <col min="13" max="14" width="26.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1081,18 +1165,24 @@
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>134</v>
       </c>
-      <c r="N1"/>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="P1"/>
+    </row>
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>128</v>
       </c>
@@ -1116,8 +1206,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1141,8 +1233,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1166,8 +1260,10 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1191,8 +1287,10 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1216,8 +1314,10 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1241,8 +1341,10 @@
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
@@ -1266,8 +1368,10 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1291,8 +1395,10 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>129</v>
       </c>
@@ -1316,8 +1422,10 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
@@ -1341,8 +1449,10 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1366,8 +1476,10 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1391,8 +1503,10 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1416,8 +1530,10 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>48</v>
       </c>
@@ -1444,10 +1560,12 @@
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>135</v>
@@ -1476,10 +1594,12 @@
       <c r="J16" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>136</v>
@@ -1508,10 +1628,12 @@
       <c r="J17" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>137</v>
@@ -1540,10 +1662,16 @@
       <c r="J18" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>138</v>
@@ -1572,10 +1700,16 @@
       <c r="J19" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K19" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>139</v>
@@ -1604,10 +1738,16 @@
       <c r="J20" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K20" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>140</v>
@@ -1632,10 +1772,16 @@
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>141</v>
@@ -1664,8 +1810,14 @@
       <c r="J22" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>142</v>
       </c>
@@ -1689,8 +1841,10 @@
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>143</v>
       </c>
@@ -1714,8 +1868,10 @@
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>144</v>
       </c>
@@ -1739,8 +1895,10 @@
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>145</v>
       </c>
@@ -1764,10 +1922,12 @@
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>146</v>
@@ -1796,10 +1956,16 @@
       <c r="J27" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>147</v>
@@ -1824,13 +1990,19 @@
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>159</v>
+      <c r="K28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1852,13 +2024,15 @@
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -1880,13 +2054,15 @@
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -1912,13 +2088,15 @@
       <c r="J31" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -1940,8 +2118,10 @@
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>117</v>
       </c>
@@ -1972,8 +2152,10 @@
       <c r="J33" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>118</v>
       </c>
@@ -2004,12 +2186,12 @@
       <c r="J34" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="K34"/>
-      <c r="L34"/>
       <c r="M34"/>
       <c r="N34"/>
-    </row>
-    <row r="35" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O34"/>
+      <c r="P34"/>
+    </row>
+    <row r="35" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>124</v>
       </c>
@@ -2040,8 +2222,10 @@
       <c r="J35" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>125</v>
       </c>
@@ -2072,8 +2256,10 @@
       <c r="J36" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>62</v>
       </c>
@@ -2100,8 +2286,10 @@
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>63</v>
       </c>
@@ -2128,8 +2316,10 @@
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>65</v>
       </c>
@@ -2156,8 +2346,10 @@
       </c>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+    </row>
+    <row r="40" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>67</v>
       </c>
@@ -2181,8 +2373,10 @@
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>68</v>
       </c>
@@ -2206,8 +2400,10 @@
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>69</v>
       </c>
@@ -2231,8 +2427,10 @@
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>70</v>
       </c>
@@ -2259,8 +2457,10 @@
       </c>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>73</v>
       </c>
@@ -2287,8 +2487,10 @@
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>76</v>
       </c>
@@ -2315,8 +2517,10 @@
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>78</v>
       </c>
@@ -2343,8 +2547,10 @@
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>80</v>
       </c>
@@ -2368,8 +2574,10 @@
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>81</v>
       </c>
@@ -2393,8 +2601,10 @@
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>82</v>
       </c>
@@ -2418,8 +2628,10 @@
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>83</v>
       </c>
@@ -2443,8 +2655,10 @@
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>88</v>
       </c>
@@ -2471,8 +2685,10 @@
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>90</v>
       </c>
@@ -2499,8 +2715,10 @@
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>92</v>
       </c>
@@ -2527,8 +2745,10 @@
       </c>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+    </row>
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>94</v>
       </c>
@@ -2555,8 +2775,10 @@
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+    </row>
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>96</v>
       </c>
@@ -2583,8 +2805,10 @@
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-    </row>
-    <row r="56" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+    </row>
+    <row r="56" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>98</v>
       </c>
@@ -2615,8 +2839,10 @@
       <c r="J56" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
@@ -2643,8 +2869,10 @@
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-    </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+    </row>
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>102</v>
       </c>
@@ -2671,8 +2899,10 @@
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>104</v>
       </c>
@@ -2703,8 +2933,10 @@
       <c r="J59" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>107</v>
       </c>
@@ -2731,8 +2963,10 @@
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+    </row>
+    <row r="61" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>110</v>
       </c>
@@ -2759,24 +2993,26 @@
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K62:M1048576 N35:N1048576 N2:N33">
-    <cfRule type="cellIs" dxfId="13" priority="50" operator="equal">
+  <conditionalFormatting sqref="M62:O1048576 P35:P1048576 P2:P33">
+    <cfRule type="cellIs" dxfId="6" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62:M1048576 N35:N1048576 N2:N33">
-    <cfRule type="cellIs" dxfId="9" priority="25" operator="equal">
+  <conditionalFormatting sqref="M62:O1048576 P35:P1048576 P2:P33">
+    <cfRule type="cellIs" dxfId="2" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added type name tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="183">
   <si>
     <t>Field</t>
   </si>
@@ -473,6 +473,12 @@
     <t>Type names should not use the term "Type" in the name other than as the final representation term.</t>
   </si>
   <si>
+    <t>type_name_repTerm_aug</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_assn</t>
+  </si>
+  <si>
     <t>type_name_missing_simple</t>
   </si>
   <si>
@@ -561,13 +567,19 @@
   </si>
   <si>
     <t>Type names must not occur more than once in a single namespace.</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_metadata</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,15 +607,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,11 +631,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -641,13 +641,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,14 +670,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -1111,10 +1106,10 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,10 +1161,10 @@
         <v>17</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1565,7 +1560,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>135</v>
@@ -1599,7 +1594,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>136</v>
@@ -1633,7 +1628,7 @@
     </row>
     <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>137</v>
@@ -1663,15 +1658,15 @@
         <v>50</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>138</v>
@@ -1701,15 +1696,15 @@
         <v>51</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>139</v>
@@ -1739,15 +1734,15 @@
         <v>53</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>140</v>
@@ -1773,15 +1768,15 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>141</v>
@@ -1811,13 +1806,16 @@
         <v>115</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>142</v>
       </c>
@@ -1845,6 +1843,9 @@
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>143</v>
       </c>
@@ -1872,6 +1873,9 @@
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>144</v>
       </c>
@@ -1899,6 +1903,9 @@
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>145</v>
       </c>
@@ -1927,7 +1934,7 @@
     </row>
     <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>146</v>
@@ -1957,15 +1964,15 @@
         <v>60</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>147</v>
@@ -1991,18 +1998,18 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>157</v>
+      <c r="A29" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -2028,8 +2035,8 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>160</v>
+      <c r="A30" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>148</v>
@@ -2058,11 +2065,11 @@
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>158</v>
+      <c r="A31" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -2093,10 +2100,10 @@
     </row>
     <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added type name spellcheck test
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -509,9 +509,6 @@
     <t>type_name_camelCase</t>
   </si>
   <si>
-    <t>type_name_term_undefined</t>
-  </si>
-  <si>
     <t>type_name_reservedTerm_type</t>
   </si>
   <si>
@@ -573,6 +570,9 @@
   </si>
   <si>
     <t>type_name_repTerm_list</t>
+  </si>
+  <si>
+    <t>type_name_spellcheck</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1109,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,10 +1161,10 @@
         <v>17</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1658,15 +1658,15 @@
         <v>50</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>138</v>
@@ -1696,10 +1696,10 @@
         <v>51</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1734,10 +1734,10 @@
         <v>53</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1768,10 +1768,10 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1806,10 +1806,10 @@
         <v>115</v>
       </c>
       <c r="K22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1874,7 +1874,7 @@
     </row>
     <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>144</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>145</v>
@@ -1964,10 +1964,10 @@
         <v>60</v>
       </c>
       <c r="K27" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1998,10 +1998,10 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -2009,7 +2009,7 @@
         <v>159</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>148</v>
@@ -2069,7 +2069,7 @@
         <v>160</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -2099,11 +2099,11 @@
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>161</v>
+      <c r="A32" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added Type definition tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="218">
   <si>
     <t>Field</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Base</t>
   </si>
   <si>
-    <t>type-prefix-all-invalid</t>
-  </si>
-  <si>
-    <t>A type must have a valid namespace prefix.</t>
-  </si>
-  <si>
     <t>10-45</t>
   </si>
   <si>
@@ -212,72 +206,12 @@
     <t>10-49</t>
   </si>
   <si>
-    <t>type-def-term-defined</t>
-  </si>
-  <si>
-    <t>type-style-all-missing</t>
-  </si>
-  <si>
-    <t>A type must have a style.</t>
-  </si>
-  <si>
-    <t>type-style-all-invalid</t>
-  </si>
-  <si>
-    <t>A type style should be one of the following: object, adapter, association, augmentation, CSC, simple, list, union, or blank (defaults to "object").</t>
-  </si>
-  <si>
-    <t>A type with a name that ends with "AugmentationType" must have style "augmentation".</t>
-  </si>
-  <si>
-    <t>A type with a name that ends with "AssociationType" must have style "association".</t>
-  </si>
-  <si>
-    <t>A type with a name that ends with "MetadataType" must have style "metadata".</t>
-  </si>
-  <si>
-    <t>type-base-simpleContent-missing</t>
-  </si>
-  <si>
-    <t>A CSC or simple type must declare a base type.</t>
-  </si>
-  <si>
     <t>Simple content types</t>
   </si>
   <si>
-    <t>type-base-csc-invalid</t>
-  </si>
-  <si>
-    <t>A CSC type must have a simple or CSC base type.</t>
-  </si>
-  <si>
     <t>CSC types</t>
   </si>
   <si>
-    <t>type-base-simple-invalid</t>
-  </si>
-  <si>
-    <t>A simple type must use a XML schema simple type as its base type.</t>
-  </si>
-  <si>
-    <t>type-base-all-invalid</t>
-  </si>
-  <si>
-    <t>A type's base type must exist.</t>
-  </si>
-  <si>
-    <t>An augmentation type must extend structures:AugmentationType.</t>
-  </si>
-  <si>
-    <t>An association type must extend another association type.</t>
-  </si>
-  <si>
-    <t>A metadata type must extend structures:MetadataType</t>
-  </si>
-  <si>
-    <t>A simple union type must not have a base type</t>
-  </si>
-  <si>
     <t>Union types</t>
   </si>
   <si>
@@ -374,18 +308,6 @@
     <t>11-8</t>
   </si>
   <si>
-    <t>A simple type must have a definition.</t>
-  </si>
-  <si>
-    <t>type-def-simple-missing</t>
-  </si>
-  <si>
-    <t>type-def-complex-missing</t>
-  </si>
-  <si>
-    <t>A complex type must have a definition.</t>
-  </si>
-  <si>
     <t>9-12</t>
   </si>
   <si>
@@ -398,27 +320,12 @@
     <t>11-45</t>
   </si>
   <si>
-    <t>type-def-complex-phrase</t>
-  </si>
-  <si>
-    <t>type-def-simple-phrase</t>
-  </si>
-  <si>
-    <t>A complex type definition must begin with the standard opening phrase "A data type".</t>
-  </si>
-  <si>
-    <t>A simple type definition must begin with the standard opening phrase "A data type".</t>
-  </si>
-  <si>
     <t>A property must have a unique name in its namespace.</t>
   </si>
   <si>
     <t>A term in a property definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
   </si>
   <si>
-    <t>A term in a type definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
-  </si>
-  <si>
     <t>An enumeration must belong to type with a name that ends in "CodeSimpleType"</t>
   </si>
   <si>
@@ -573,6 +480,204 @@
   </si>
   <si>
     <t>type_name_spellcheck</t>
+  </si>
+  <si>
+    <t>type_def_missing_simple</t>
+  </si>
+  <si>
+    <t>type_def_missing_complex</t>
+  </si>
+  <si>
+    <t>type_def_phrase_complex</t>
+  </si>
+  <si>
+    <t>type_def_phrase_simple</t>
+  </si>
+  <si>
+    <t>Type namespace prefixes must be defined.</t>
+  </si>
+  <si>
+    <t>Simple types must have a definition.</t>
+  </si>
+  <si>
+    <t>Complex types must have a definition.</t>
+  </si>
+  <si>
+    <t>Complex type definitions must begin with the standard opening phrase "A data type".</t>
+  </si>
+  <si>
+    <t>Simple type definitions must begin with the standard opening phrase "A data type".</t>
+  </si>
+  <si>
+    <t>Type definitions should use words and terms that are either defined in the dictionary or as "Local Terminology".</t>
+  </si>
+  <si>
+    <t>Types must have a style.</t>
+  </si>
+  <si>
+    <t>Type styles should be one of the following: object, adapter, association, augmentation, CSC, simple, list, union, or blank (defaults to "object").</t>
+  </si>
+  <si>
+    <t>Types with names that end with "AugmentationType" must have style "augmentation".</t>
+  </si>
+  <si>
+    <t>Types with names that end with "AssociationType" must have style "association".</t>
+  </si>
+  <si>
+    <t>Types with names that end with "MetadataType" must have style "metadata".</t>
+  </si>
+  <si>
+    <t>type_def_spellcheck</t>
+  </si>
+  <si>
+    <t>type_style_missing</t>
+  </si>
+  <si>
+    <t>type_style_unknown</t>
+  </si>
+  <si>
+    <t>type_prefix_unknown</t>
+  </si>
+  <si>
+    <t>type_base_unknown</t>
+  </si>
+  <si>
+    <t>type_style_aug</t>
+  </si>
+  <si>
+    <t>type_style_assn</t>
+  </si>
+  <si>
+    <t>type_style_metadata</t>
+  </si>
+  <si>
+    <t>type_base_missing_simpleContent</t>
+  </si>
+  <si>
+    <t>Types that represent a value (simple content) must declare a base type.</t>
+  </si>
+  <si>
+    <t>type_base_invalid_csc</t>
+  </si>
+  <si>
+    <t>Complex types with simple content (CSC) must have a simple or CSC base type.</t>
+  </si>
+  <si>
+    <t>type_base_invalid_simple</t>
+  </si>
+  <si>
+    <t>Simple types must use a XML schema simple type as its base type.</t>
+  </si>
+  <si>
+    <t>Types must have bases that are defined.</t>
+  </si>
+  <si>
+    <t>type_base_aug</t>
+  </si>
+  <si>
+    <t>type_base_assn</t>
+  </si>
+  <si>
+    <t>type_base_metadata</t>
+  </si>
+  <si>
+    <t>type_base_union</t>
+  </si>
+  <si>
+    <t>Augmentation types must extend structures:AugmentationType.</t>
+  </si>
+  <si>
+    <t>Association types must extend another association type.</t>
+  </si>
+  <si>
+    <t>Metadata types must extend structures:MetadataType</t>
+  </si>
+  <si>
+    <t>Simple union types must not have a base type</t>
+  </si>
+  <si>
+    <t>Type name 'PersonAugmentationType' is a valid augmentation type name.</t>
+  </si>
+  <si>
+    <t>Type name 'PersonType' is not a valid augmentation type name.</t>
+  </si>
+  <si>
+    <t>Type name 'PersonLocationAssociationType' is a valid association type name.</t>
+  </si>
+  <si>
+    <t>Type name 'PersonLocationType' is not a valid association type name.</t>
+  </si>
+  <si>
+    <t>Type name 'SourceType' is not a valid metadata type name.</t>
+  </si>
+  <si>
+    <t>Type name 'SourceMetadataType' is a valid metadata type name.</t>
+  </si>
+  <si>
+    <t>Type name 'DecimalListSimpleType' is a valid list type name.</t>
+  </si>
+  <si>
+    <t>Type name 'DecimalValuesSimpleType' is not a valid list type name.</t>
+  </si>
+  <si>
+    <t>Types 'justice:CaseType' and 'logistics:CaseType' are valid because even though they use the same name, they are defined in different namespaces.</t>
+  </si>
+  <si>
+    <t>Type name 'CaseType' cannot be defined twice in the same namespace.</t>
+  </si>
+  <si>
+    <t>Type name 'IDCategoryCodeType' is valid because the term 'Type' only appears at the end of the name.</t>
+  </si>
+  <si>
+    <t>Type name 'IDTypeCodeType' is not valid because the term 'Type' is used in the middle of the name.</t>
+  </si>
+  <si>
+    <t>Type name 'PersonType' is valid because it begins with an upper case letter.</t>
+  </si>
+  <si>
+    <t>Type name 'personType' is not valid because it begins with a lower case letter.</t>
+  </si>
+  <si>
+    <t>Type name 'ncic:VMOCodeType' is valid if the ncic namespace defines the meaning of 'VMO' in its Local Terminology section.</t>
+  </si>
+  <si>
+    <t>Type name 'ncic:VMOCodeType' is not valid if the ncic namespace does not defined 'VMO' in its Local Terminology section.</t>
+  </si>
+  <si>
+    <t>10-34</t>
+  </si>
+  <si>
+    <t>10-21</t>
+  </si>
+  <si>
+    <t>10-35</t>
+  </si>
+  <si>
+    <t>10-39</t>
+  </si>
+  <si>
+    <t>10-44</t>
+  </si>
+  <si>
+    <t>NDR rule does not mention local terminology.</t>
+  </si>
+  <si>
+    <t>Definition 'A data type for a human being' is valid for type 'PersonType'.</t>
+  </si>
+  <si>
+    <t>Definition 'A human being' is not valid for type 'PersonType'.</t>
+  </si>
+  <si>
+    <t>Definition 'A data type for United States state codes' is valid for type usps:StateCodeSimpleType.</t>
+  </si>
+  <si>
+    <t>Definition 'United States state codes' is not valid for type usps:StateCodeSimpleType.</t>
+  </si>
+  <si>
+    <t>Definition 'A data type for FIPS state codes" is valid if the term 'FIPS' is defined as Local Terminology in that namespace.</t>
+  </si>
+  <si>
+    <t>Definition 'A data type for FIPS state codes" is not recommended if the term 'FIPS' is not defined as Local Terminology in that namespace.</t>
   </si>
 </sst>
 </file>
@@ -646,7 +751,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,6 +773,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,7 +926,7 @@
     </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="Name"/>
+        <filter val="Definition"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1106,10 +1217,10 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1235,7 @@
     <col min="10" max="10" width="10.77734375" style="7" customWidth="1"/>
     <col min="11" max="12" width="34.77734375" style="7" customWidth="1"/>
     <col min="13" max="14" width="26.77734375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="27.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" style="9" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" style="1"/>
     <col min="17" max="17" width="31.5546875" customWidth="1"/>
   </cols>
@@ -1161,10 +1272,10 @@
         <v>17</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1172,14 +1283,14 @@
       <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
-        <v>134</v>
+      <c r="O1" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -1203,6 +1314,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -1230,6 +1342,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -1257,6 +1370,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -1284,6 +1398,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
+      <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -1311,6 +1426,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -1338,6 +1454,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -1365,6 +1482,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -1392,10 +1510,11 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
@@ -1419,6 +1538,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -1446,6 +1566,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -1473,6 +1594,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -1500,6 +1622,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -1527,13 +1650,14 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>48</v>
+      <c r="A15" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1557,13 +1681,14 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1575,7 +1700,7 @@
         <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1584,20 +1709,20 @@
         <v>3</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1609,7 +1734,7 @@
         <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1618,20 +1743,20 @@
         <v>3</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
@@ -1652,24 +1777,24 @@
         <v>3</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
@@ -1690,24 +1815,24 @@
         <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
@@ -1719,7 +1844,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -1728,24 +1853,24 @@
         <v>3</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
@@ -1757,7 +1882,7 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -1768,18 +1893,18 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="3" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
@@ -1800,24 +1925,24 @@
         <v>3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
@@ -1829,7 +1954,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -1837,17 +1962,25 @@
       <c r="H23" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
@@ -1859,7 +1992,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -1867,17 +2000,21 @@
       <c r="H24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
@@ -1889,7 +2026,7 @@
         <v>23</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -1897,17 +2034,21 @@
       <c r="H25" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
@@ -1919,7 +2060,7 @@
         <v>23</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -1927,17 +2068,21 @@
       <c r="H26" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>7</v>
@@ -1949,7 +2094,7 @@
         <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -1958,24 +2103,24 @@
         <v>35</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>20</v>
@@ -1987,7 +2132,7 @@
         <v>23</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -1998,18 +2143,18 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="3" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -2031,15 +2176,19 @@
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K29" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -2061,15 +2210,19 @@
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K30" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -2090,20 +2243,24 @@
         <v>3</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -2123,17 +2280,28 @@
       <c r="H32" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>117</v>
+      <c r="I32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>18</v>
@@ -2145,7 +2313,7 @@
         <v>24</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2157,17 +2325,17 @@
         <v>6</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>118</v>
+        <v>94</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
@@ -2179,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2191,19 +2359,20 @@
         <v>6</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>121</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
       <c r="M34"/>
       <c r="N34"/>
-      <c r="O34"/>
       <c r="P34"/>
     </row>
-    <row r="35" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>124</v>
+    <row r="35" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>45</v>
@@ -2215,7 +2384,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2227,17 +2396,21 @@
         <v>6</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>125</v>
+        <v>96</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>45</v>
@@ -2249,7 +2422,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2261,17 +2434,21 @@
         <v>6</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>20</v>
@@ -2291,17 +2468,21 @@
       <c r="H37" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>63</v>
+      <c r="A38" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>18</v>
@@ -2325,13 +2506,14 @@
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
+      <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>65</v>
+      <c r="A39" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>20</v>
@@ -2355,10 +2537,14 @@
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
+      <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>20</v>
@@ -2370,7 +2556,7 @@
         <v>46</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2382,10 +2568,14 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
+      <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>20</v>
@@ -2397,7 +2587,7 @@
         <v>46</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2409,10 +2599,14 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
+      <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>20</v>
@@ -2424,7 +2618,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2436,13 +2630,14 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
+      <c r="O42" s="1"/>
     </row>
     <row r="43" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>70</v>
+      <c r="A43" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>18</v>
@@ -2454,7 +2649,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -2464,15 +2659,15 @@
       </c>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>73</v>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>20</v>
@@ -2484,7 +2679,7 @@
         <v>47</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2494,15 +2689,15 @@
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>76</v>
+      <c r="A45" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>20</v>
@@ -2514,7 +2709,7 @@
         <v>47</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2524,15 +2719,15 @@
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>78</v>
+      <c r="A46" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>39</v>
@@ -2554,12 +2749,15 @@
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>20</v>
@@ -2571,7 +2769,7 @@
         <v>47</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2579,14 +2777,21 @@
       <c r="H47" t="s">
         <v>3</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="B48" s="2" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>20</v>
@@ -2598,7 +2803,7 @@
         <v>47</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2606,14 +2811,21 @@
       <c r="H48" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
@@ -2625,7 +2837,7 @@
         <v>47</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -2633,14 +2845,21 @@
       <c r="H49" t="s">
         <v>3</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>20</v>
@@ -2652,7 +2871,7 @@
         <v>47</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -2660,23 +2879,23 @@
       <c r="H50" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E51" t="s">
         <v>22</v>
@@ -2694,19 +2913,20 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E52" t="s">
         <v>22</v>
@@ -2724,19 +2944,20 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E53" t="s">
         <v>23</v>
@@ -2754,19 +2975,20 @@
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E54" t="s">
         <v>23</v>
@@ -2784,19 +3006,20 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
-    </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
         <v>23</v>
@@ -2814,25 +3037,26 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
-    </row>
-    <row r="56" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E56" t="s">
         <v>23</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -2844,26 +3068,27 @@
         <v>6</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
-    </row>
-    <row r="57" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>19</v>
@@ -2878,22 +3103,23 @@
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
-    </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E58" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>19</v>
@@ -2908,25 +3134,26 @@
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E59" t="s">
         <v>24</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -2938,56 +3165,58 @@
         <v>6</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
         <v>24</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
-    </row>
-    <row r="61" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>19</v>
@@ -3002,6 +3231,7 @@
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
+      <c r="O61" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M62:O1048576 P35:P1048576 P2:P33">

</xml_diff>

<commit_message>
Added Type base tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="226">
   <si>
     <t>Field</t>
   </si>
@@ -566,9 +566,6 @@
     <t>type_base_invalid_simple</t>
   </si>
   <si>
-    <t>Simple types must use a XML schema simple type as its base type.</t>
-  </si>
-  <si>
     <t>Types must have bases that are defined.</t>
   </si>
   <si>
@@ -678,6 +675,33 @@
   </si>
   <si>
     <t>Definition 'A data type for FIPS state codes" is not recommended if the term 'FIPS' is not defined as Local Terminology in that namespace.</t>
+  </si>
+  <si>
+    <t>Type HairColorCodeSimpleType needs a base type like xs:string or xs:token.</t>
+  </si>
+  <si>
+    <t>Type HairColorCodeSimpleType is not valid without a base type.</t>
+  </si>
+  <si>
+    <t>Simple content type HairColorCodeType can have a base type like HairColorCodeSimpleType (simple type).</t>
+  </si>
+  <si>
+    <t>Simple content type HairColorCodeType cannot have a type like nc:PersonType (complex object type).</t>
+  </si>
+  <si>
+    <t>Simple types should use a XML schema simple type as its base type.</t>
+  </si>
+  <si>
+    <t>Simple type ext:HairColorCodeSimpleType should not have base type ext:ColorCodeSimpleType.</t>
+  </si>
+  <si>
+    <t>Simple type ext:HairColorCodeSimpleType can have base type xs:token.</t>
+  </si>
+  <si>
+    <t>Type PersonType can extend type structures:ObjectType (this type exists).</t>
+  </si>
+  <si>
+    <t>Type PersonType cannot extend type structures:BogusType (this type does not exist).</t>
   </si>
 </sst>
 </file>
@@ -926,7 +950,7 @@
     </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="Definition"/>
+        <filter val="Base"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1217,10 +1241,10 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1966,13 +1990,13 @@
         <v>102</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K23" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2003,10 +2027,10 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2037,10 +2061,10 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2071,10 +2095,10 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2177,10 +2201,10 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2211,10 +2235,10 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2249,10 +2273,10 @@
         <v>59</v>
       </c>
       <c r="K31" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="L31" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2284,19 +2308,19 @@
         <v>102</v>
       </c>
       <c r="J32" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="O32" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>152</v>
       </c>
@@ -2330,7 +2354,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>153</v>
       </c>
@@ -2367,7 +2391,7 @@
       <c r="N34"/>
       <c r="P34"/>
     </row>
-    <row r="35" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>154</v>
       </c>
@@ -2399,13 +2423,13 @@
         <v>96</v>
       </c>
       <c r="K35" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="L35" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="L35" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>155</v>
       </c>
@@ -2437,14 +2461,14 @@
         <v>97</v>
       </c>
       <c r="K36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L36" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="L36" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+    </row>
+    <row r="37" spans="1:16" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2471,10 +2495,10 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="L37" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
@@ -2632,8 +2656,8 @@
       <c r="L42" s="3"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2659,11 +2683,15 @@
       </c>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="K43" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2689,15 +2717,19 @@
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="K44" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>179</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>20</v>
@@ -2715,19 +2747,23 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="K45" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>39</v>
@@ -2749,15 +2785,19 @@
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-    </row>
-    <row r="47" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K46" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>20</v>
@@ -2781,17 +2821,17 @@
         <v>102</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>20</v>
@@ -2815,17 +2855,17 @@
         <v>102</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
@@ -2849,17 +2889,17 @@
         <v>102</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added Type prefix tests.
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="252">
   <si>
     <t>Field</t>
   </si>
@@ -224,75 +224,42 @@
     <t>Kind</t>
   </si>
   <si>
-    <t>facet-prefix-all-missing</t>
-  </si>
-  <si>
     <t>A facet must have a type namespace prefix.</t>
   </si>
   <si>
-    <t>facet-prefix-all-invalid</t>
-  </si>
-  <si>
     <t>A facet must have a valid type namespace prefix.</t>
   </si>
   <si>
-    <t>facet-name-all-missing</t>
-  </si>
-  <si>
     <t>A facet must have a type name.</t>
   </si>
   <si>
-    <t>facet-name-all-invalid</t>
-  </si>
-  <si>
     <t>A facet must have a valid type name.</t>
   </si>
   <si>
-    <t>facet-name-all-complex</t>
-  </si>
-  <si>
     <t>A facet must belong to a simple type.</t>
   </si>
   <si>
-    <t>facet-name-code-invalid</t>
-  </si>
-  <si>
     <t>Enumerations</t>
   </si>
   <si>
-    <t>facet-value-all-missing</t>
-  </si>
-  <si>
     <t>A facet must have a value (e.g., code value, pattern value, etc).</t>
   </si>
   <si>
-    <t>facet-value-code-duplicate</t>
-  </si>
-  <si>
     <t>A facet value should probably be unique within its type.</t>
   </si>
   <si>
-    <t>facet-def-code-missing</t>
-  </si>
-  <si>
     <t>An enumeration must have a definition.</t>
   </si>
   <si>
     <t>9-14</t>
   </si>
   <si>
-    <t>facet-def-pattern-missing</t>
-  </si>
-  <si>
     <t>Patterns</t>
   </si>
   <si>
     <t>info</t>
   </si>
   <si>
-    <t>facet-kind-all-invalid</t>
-  </si>
-  <si>
     <t>A facet must have a valid style (e.g., enumeration, pattern, etc.).</t>
   </si>
   <si>
@@ -702,13 +669,124 @@
   </si>
   <si>
     <t>Type PersonType cannot extend type structures:BogusType (this type does not exist).</t>
+  </si>
+  <si>
+    <t>type_prefix_missing</t>
+  </si>
+  <si>
+    <t>Types must have a namespace prefix.</t>
+  </si>
+  <si>
+    <t>facet_prefix_missing</t>
+  </si>
+  <si>
+    <t>facet_prefix_unknown</t>
+  </si>
+  <si>
+    <t>facet_type_missing</t>
+  </si>
+  <si>
+    <t>facet_type_unknown</t>
+  </si>
+  <si>
+    <t>facet_type_complex</t>
+  </si>
+  <si>
+    <t>facet_type_repTerm</t>
+  </si>
+  <si>
+    <t>facet_value_missing</t>
+  </si>
+  <si>
+    <t>facet_value_duplicate</t>
+  </si>
+  <si>
+    <t>facet_def_missing_code</t>
+  </si>
+  <si>
+    <t>facet_def_missing_pattern</t>
+  </si>
+  <si>
+    <t>facet_kind_invalid</t>
+  </si>
+  <si>
+    <t>property_name_duplicate</t>
+  </si>
+  <si>
+    <t>property_name_camelCase_element</t>
+  </si>
+  <si>
+    <t>property_name_camelCase_attribute</t>
+  </si>
+  <si>
+    <t>property_name_spellcheck</t>
+  </si>
+  <si>
+    <t>property_type_abstract</t>
+  </si>
+  <si>
+    <t>property_type_element</t>
+  </si>
+  <si>
+    <t>property_type_attribute</t>
+  </si>
+  <si>
+    <t>property_type_unknown</t>
+  </si>
+  <si>
+    <t>property_group_unknown</t>
+  </si>
+  <si>
+    <t>property_type_missing</t>
+  </si>
+  <si>
+    <t>A property that is not abstract must have a data type.</t>
+  </si>
+  <si>
+    <t>Concrete elements and attributes</t>
+  </si>
+  <si>
+    <t>property_def_spellcheck</t>
+  </si>
+  <si>
+    <t>property_group_invalid</t>
+  </si>
+  <si>
+    <t>property_style_abstract</t>
+  </si>
+  <si>
+    <t>property_style_substitution</t>
+  </si>
+  <si>
+    <t>Type PersonType can be associated with a namespace prefix like 'nc'.</t>
+  </si>
+  <si>
+    <t>Type PersonType should not have a missing namespace prefix.</t>
+  </si>
+  <si>
+    <t>Type PersonType can have namespace prefix 'nc' if that prefix is declared.</t>
+  </si>
+  <si>
+    <t>Type PersonType cannot have namespace prefix 'unk' if there is no declaration of what 'unk' is.</t>
+  </si>
+  <si>
+    <t>Type PersonType has style 'object'.</t>
+  </si>
+  <si>
+    <t>Type PersonType cannot have a missing style.</t>
+  </si>
+  <si>
+    <t>Type PersonType cannot have unknown style 'myCustomObject'.</t>
+  </si>
+  <si>
+    <t>Type PersonType has permitted style 'object'.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,6 +812,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -775,7 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -800,9 +883,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -811,26 +900,33 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -878,19 +974,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -941,35 +1024,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O61" totalsRowShown="0">
-  <autoFilter ref="A1:O61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O63" totalsRowShown="0">
+  <autoFilter ref="A1:O63">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="Type"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Base"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
+  <sortState ref="A2:O63">
+    <sortCondition ref="A1:A63"/>
+  </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="14"/>
-    <tableColumn id="17" name="Category" dataDxfId="13"/>
+    <tableColumn id="1" name="ID" dataDxfId="16" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="15"/>
+    <tableColumn id="17" name="Category" dataDxfId="14"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="12"/>
+    <tableColumn id="14" name="Scope" dataDxfId="13"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="11"/>
-    <tableColumn id="18" name="Rules" dataDxfId="10"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="1"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="0"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="9"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="8"/>
-    <tableColumn id="19" name="Notes" dataDxfId="7"/>
+    <tableColumn id="21" name="Spec" dataDxfId="12"/>
+    <tableColumn id="18" name="Rules" dataDxfId="4"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="6"/>
+    <tableColumn id="19" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1238,16 +1322,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="30" style="8" customWidth="1"/>
     <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
@@ -1257,14 +1341,14 @@
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="9" width="11.88671875" customWidth="1"/>
     <col min="10" max="10" width="10.77734375" style="7" customWidth="1"/>
-    <col min="11" max="12" width="34.77734375" style="7" customWidth="1"/>
-    <col min="13" max="14" width="26.77734375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="27.21875" style="9" customWidth="1"/>
+    <col min="11" max="12" width="34.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="26.77734375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" style="10" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" style="1"/>
     <col min="17" max="17" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1295,38 +1379,41 @@
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>103</v>
+      <c r="O1" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" hidden="1">
+      <c r="A2" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1334,55 +1421,61 @@
       <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" hidden="1">
+      <c r="A3" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" ht="28.8" hidden="1">
+      <c r="A4" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1390,24 +1483,25 @@
       <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" hidden="1">
+      <c r="A5" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -1418,55 +1512,57 @@
       <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" hidden="1">
+      <c r="A6" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" hidden="1">
+      <c r="A7" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1474,55 +1570,57 @@
       <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" hidden="1">
+      <c r="A8" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" ht="28.8" hidden="1">
+      <c r="A9" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1530,24 +1628,29 @@
       <c r="H9" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" hidden="1">
+      <c r="A10" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -1556,57 +1659,59 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:16" hidden="1">
+      <c r="A11" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:16" ht="28.8" hidden="1">
+      <c r="A12" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1614,15 +1719,16 @@
       <c r="H12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:16" ht="28.8" hidden="1">
+      <c r="A13" s="8" t="s">
+        <v>240</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
@@ -1631,26 +1737,27 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:16" ht="28.8" hidden="1">
+      <c r="A14" s="8" t="s">
+        <v>241</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
@@ -1659,10 +1766,10 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
@@ -1672,59 +1779,55 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>170</v>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" spans="1:16" hidden="1">
+      <c r="A15" s="8" t="s">
+        <v>236</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:16" ht="28.8" hidden="1">
+      <c r="A16" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1732,33 +1835,28 @@
       <c r="H16" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>121</v>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="1:15" ht="28.8" hidden="1">
+      <c r="A17" s="8" t="s">
+        <v>229</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1766,27 +1864,22 @@
       <c r="H17" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>122</v>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" hidden="1">
+      <c r="A18" s="8" t="s">
+        <v>228</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -1800,31 +1893,22 @@
       <c r="H18" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>145</v>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:15" ht="28.8" hidden="1">
+      <c r="A19" s="8" t="s">
+        <v>231</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
@@ -1838,37 +1922,28 @@
       <c r="H19" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>123</v>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15" ht="28.8" hidden="1">
+      <c r="A20" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -1876,37 +1951,28 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>124</v>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15" ht="28.8" hidden="1">
+      <c r="A21" s="8" t="s">
+        <v>243</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -1914,71 +1980,57 @@
       <c r="H21" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>125</v>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:15" ht="28.8" hidden="1">
+      <c r="A22" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:15" hidden="1">
       <c r="A23" s="8" t="s">
-        <v>118</v>
+        <v>234</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -1986,165 +2038,135 @@
       <c r="H23" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" ht="28.8" hidden="1">
       <c r="A24" s="8" t="s">
-        <v>119</v>
+        <v>233</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" ht="43.2" hidden="1">
+      <c r="A25" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15" hidden="1">
+      <c r="A26" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" ht="28.8" hidden="1">
+      <c r="A27" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="3" t="s">
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>127</v>
+    </row>
+    <row r="28" spans="1:15" ht="28.8" hidden="1">
+      <c r="A28" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>20</v>
@@ -2153,44 +2175,42 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="72" hidden="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="43.2" hidden="1">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2200,19 +2220,19 @@
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="57.6" hidden="1">
       <c r="A30" s="4" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>117</v>
+        <v>210</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -2221,10 +2241,10 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2234,19 +2254,19 @@
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>129</v>
+      <c r="K30" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="28.8" hidden="1">
+      <c r="A31" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -2255,10 +2275,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -2267,24 +2287,18 @@
         <v>3</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="28.8" hidden="1">
       <c r="A32" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -2293,113 +2307,97 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" hidden="1">
+      <c r="A33" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:16" ht="43.2" hidden="1">
+      <c r="A34" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" t="s">
-        <v>3</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="G34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" hidden="1">
+      <c r="A35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B34" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" t="s">
-        <v>4</v>
-      </c>
-      <c r="H34" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" t="s">
-        <v>6</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="P34"/>
-    </row>
-    <row r="35" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -2414,30 +2412,26 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="L35" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:16" hidden="1">
       <c r="A36" s="4" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -2452,30 +2446,27 @@
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>35</v>
-      </c>
-      <c r="I36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="P36"/>
+    </row>
+    <row r="37" spans="1:16" ht="28.8" hidden="1">
       <c r="A37" s="4" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
@@ -2484,7 +2475,7 @@
         <v>24</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2492,52 +2483,63 @@
       <c r="H37" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>168</v>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="43.2" hidden="1">
+      <c r="A38" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>3</v>
-      </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>169</v>
+        <v>35</v>
+      </c>
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="57.6" hidden="1">
+      <c r="A39" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>20</v>
@@ -2546,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>19</v>
@@ -2555,20 +2557,23 @@
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>172</v>
+      <c r="K39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="43.2" hidden="1">
+      <c r="A40" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>20</v>
@@ -2577,10 +2582,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2588,30 +2593,37 @@
       <c r="H40" t="s">
         <v>3</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>173</v>
+      <c r="I40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="72" hidden="1">
+      <c r="A41" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2619,18 +2631,21 @@
       <c r="H41" t="s">
         <v>3</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>174</v>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="43.2" hidden="1">
+      <c r="A42" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>20</v>
@@ -2639,75 +2654,82 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
-      </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="O42" s="1"/>
-    </row>
-    <row r="43" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="28.8" hidden="1">
       <c r="A43" s="4" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" hidden="1">
+      <c r="A44" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G43" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2715,30 +2737,30 @@
       <c r="H44" t="s">
         <v>3</v>
       </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="1:16" hidden="1">
       <c r="A45" s="4" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>221</v>
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>50</v>
@@ -2747,35 +2769,35 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>35</v>
-      </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>171</v>
+        <v>3</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:16" ht="43.2" hidden="1">
+      <c r="A46" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>180</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2785,28 +2807,28 @@
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-      <c r="K46" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K46" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="28.8" hidden="1">
       <c r="A47" s="8" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>185</v>
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>53</v>
@@ -2818,32 +2840,36 @@
         <v>3</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>182</v>
+        <v>194</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="43.2" hidden="1">
+      <c r="A48" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>186</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2852,66 +2878,74 @@
         <v>3</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-    </row>
-    <row r="49" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>183</v>
+        <v>82</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="43.2" hidden="1">
+      <c r="A49" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>184</v>
+        <v>58</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="28.8" hidden="1">
+      <c r="A50" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -2921,27 +2955,31 @@
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="28.8" hidden="1">
       <c r="A51" s="8" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -2951,28 +2989,31 @@
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="O51" s="1"/>
-    </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K51" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="28.8" hidden="1">
       <c r="A52" s="8" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -2982,28 +3023,31 @@
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="O52" s="1"/>
-    </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>70</v>
+      <c r="K52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="28.8" hidden="1">
+      <c r="A53" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
         <v>23</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3011,24 +3055,31 @@
       <c r="H53" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="O53" s="1"/>
-    </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>72</v>
+      <c r="I53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" hidden="1">
+      <c r="A54" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
         <v>23</v>
@@ -3042,24 +3093,31 @@
       <c r="H54" t="s">
         <v>3</v>
       </c>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="O54" s="1"/>
-    </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>74</v>
+      <c r="I54" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="43.2" hidden="1">
+      <c r="A55" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
         <v>23</v>
@@ -3071,32 +3129,35 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="O55" s="1"/>
-    </row>
-    <row r="56" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>76</v>
+      <c r="K55" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="57.6" hidden="1">
+      <c r="A56" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E56" t="s">
         <v>23</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3105,30 +3166,36 @@
         <v>3</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="O56" s="1"/>
-    </row>
-    <row r="57" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
-        <v>78</v>
+        <v>198</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="28.8">
+      <c r="A57" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>79</v>
+        <v>216</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>19</v>
@@ -3141,25 +3208,29 @@
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="O57" s="1"/>
-    </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>80</v>
+      <c r="K57" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="O57" s="9"/>
+    </row>
+    <row r="58" spans="1:15" ht="43.2">
+      <c r="A58" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>19</v>
@@ -3168,32 +3239,36 @@
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="O58" s="1"/>
-    </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="O58" s="9"/>
+    </row>
+    <row r="59" spans="1:15" ht="28.8" hidden="1">
       <c r="A59" s="8" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3201,95 +3276,155 @@
       <c r="H59" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="O59" s="1"/>
-    </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="O59" s="9"/>
+    </row>
+    <row r="60" spans="1:15" ht="28.8" hidden="1">
       <c r="A60" s="8" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>87</v>
-      </c>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="O60" s="1"/>
-    </row>
-    <row r="61" spans="1:15" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="O60" s="9"/>
+    </row>
+    <row r="61" spans="1:15" ht="28.8" hidden="1">
       <c r="A61" s="8" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" t="s">
+        <v>3</v>
+      </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="O61" s="9"/>
+    </row>
+    <row r="62" spans="1:15" ht="28.8">
+      <c r="A62" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G61" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" t="s">
-        <v>3</v>
-      </c>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="O61" s="1"/>
+      <c r="G62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>3</v>
+      </c>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="O62" s="9"/>
+    </row>
+    <row r="63" spans="1:15" ht="43.2">
+      <c r="A63" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" t="s">
+        <v>3</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="O63" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M62:O1048576 P35:P1048576 P2:P33">
-    <cfRule type="cellIs" dxfId="6" priority="50" operator="equal">
+  <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
+    <cfRule type="cellIs" dxfId="11" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M62:O1048576 P35:P1048576 P2:P33">
-    <cfRule type="cellIs" dxfId="2" priority="25" operator="equal">
+  <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
+    <cfRule type="cellIs" dxfId="7" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Type style tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -900,15 +900,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1025,35 +1017,26 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O63" totalsRowShown="0">
-  <autoFilter ref="A1:O63">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Type"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O63"/>
   <sortState ref="A2:O63">
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="16" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="15"/>
-    <tableColumn id="17" name="Category" dataDxfId="14"/>
+    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="14"/>
+    <tableColumn id="17" name="Category" dataDxfId="13"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="13"/>
+    <tableColumn id="14" name="Scope" dataDxfId="12"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="12"/>
-    <tableColumn id="18" name="Rules" dataDxfId="4"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="6"/>
-    <tableColumn id="19" name="Notes" dataDxfId="5"/>
+    <tableColumn id="21" name="Spec" dataDxfId="11"/>
+    <tableColumn id="18" name="Rules" dataDxfId="3"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="1"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="5"/>
+    <tableColumn id="19" name="Notes" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1325,10 +1308,10 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1396,7 +1379,7 @@
       </c>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16" hidden="1">
+    <row r="2" spans="1:16">
       <c r="A2" s="5" t="s">
         <v>225</v>
       </c>
@@ -1429,7 +1412,7 @@
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:16" hidden="1">
+    <row r="3" spans="1:16">
       <c r="A3" s="5" t="s">
         <v>226</v>
       </c>
@@ -1458,7 +1441,7 @@
       <c r="J3" s="6"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:16" ht="28.8" hidden="1">
+    <row r="4" spans="1:16" ht="28.8">
       <c r="A4" s="5" t="s">
         <v>227</v>
       </c>
@@ -1487,7 +1470,7 @@
       <c r="J4" s="6"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:16" hidden="1">
+    <row r="5" spans="1:16">
       <c r="A5" s="5" t="s">
         <v>217</v>
       </c>
@@ -1516,7 +1499,7 @@
       <c r="J5" s="6"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:16" hidden="1">
+    <row r="6" spans="1:16">
       <c r="A6" s="5" t="s">
         <v>218</v>
       </c>
@@ -1545,7 +1528,7 @@
       <c r="J6" s="6"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:16" hidden="1">
+    <row r="7" spans="1:16">
       <c r="A7" s="5" t="s">
         <v>221</v>
       </c>
@@ -1574,7 +1557,7 @@
       <c r="J7" s="6"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:16" hidden="1">
+    <row r="8" spans="1:16">
       <c r="A8" s="5" t="s">
         <v>219</v>
       </c>
@@ -1603,7 +1586,7 @@
       <c r="J8" s="6"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:16" ht="28.8" hidden="1">
+    <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="5" t="s">
         <v>222</v>
       </c>
@@ -1636,7 +1619,7 @@
       </c>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:16" hidden="1">
+    <row r="10" spans="1:16">
       <c r="A10" s="5" t="s">
         <v>220</v>
       </c>
@@ -1665,7 +1648,7 @@
       <c r="J10" s="6"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:16" hidden="1">
+    <row r="11" spans="1:16">
       <c r="A11" s="5" t="s">
         <v>224</v>
       </c>
@@ -1694,7 +1677,7 @@
       <c r="J11" s="6"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:16" ht="28.8" hidden="1">
+    <row r="12" spans="1:16" ht="28.8">
       <c r="A12" s="5" t="s">
         <v>223</v>
       </c>
@@ -1723,7 +1706,7 @@
       <c r="J12" s="6"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:16" ht="28.8" hidden="1">
+    <row r="13" spans="1:16" ht="28.8">
       <c r="A13" s="8" t="s">
         <v>240</v>
       </c>
@@ -1752,7 +1735,7 @@
       <c r="J13" s="3"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:16" ht="28.8" hidden="1">
+    <row r="14" spans="1:16" ht="28.8">
       <c r="A14" s="8" t="s">
         <v>241</v>
       </c>
@@ -1781,7 +1764,7 @@
       <c r="J14" s="3"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:16" hidden="1">
+    <row r="15" spans="1:16">
       <c r="A15" s="8" t="s">
         <v>236</v>
       </c>
@@ -1810,7 +1793,7 @@
       <c r="J15" s="3"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:16" ht="28.8" hidden="1">
+    <row r="16" spans="1:16" ht="28.8">
       <c r="A16" s="8" t="s">
         <v>230</v>
       </c>
@@ -1839,7 +1822,7 @@
       <c r="J16" s="3"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:15" ht="28.8" hidden="1">
+    <row r="17" spans="1:15" ht="28.8">
       <c r="A17" s="8" t="s">
         <v>229</v>
       </c>
@@ -1868,7 +1851,7 @@
       <c r="J17" s="3"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:15" hidden="1">
+    <row r="18" spans="1:15">
       <c r="A18" s="8" t="s">
         <v>228</v>
       </c>
@@ -1897,7 +1880,7 @@
       <c r="J18" s="3"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:15" ht="28.8" hidden="1">
+    <row r="19" spans="1:15" ht="28.8">
       <c r="A19" s="8" t="s">
         <v>231</v>
       </c>
@@ -1926,7 +1909,7 @@
       <c r="J19" s="3"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:15" ht="28.8" hidden="1">
+    <row r="20" spans="1:15" ht="28.8">
       <c r="A20" s="8" t="s">
         <v>242</v>
       </c>
@@ -1955,7 +1938,7 @@
       <c r="J20" s="3"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:15" ht="28.8" hidden="1">
+    <row r="21" spans="1:15" ht="28.8">
       <c r="A21" s="8" t="s">
         <v>243</v>
       </c>
@@ -1984,7 +1967,7 @@
       <c r="J21" s="3"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" ht="28.8" hidden="1">
+    <row r="22" spans="1:15" ht="28.8">
       <c r="A22" s="8" t="s">
         <v>232</v>
       </c>
@@ -2013,7 +1996,7 @@
       <c r="J22" s="3"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" hidden="1">
+    <row r="23" spans="1:15">
       <c r="A23" s="8" t="s">
         <v>234</v>
       </c>
@@ -2042,7 +2025,7 @@
       <c r="J23" s="3"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:15" ht="28.8" hidden="1">
+    <row r="24" spans="1:15" ht="28.8">
       <c r="A24" s="8" t="s">
         <v>233</v>
       </c>
@@ -2071,7 +2054,7 @@
       <c r="J24" s="3"/>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="1:15" ht="43.2" hidden="1">
+    <row r="25" spans="1:15" ht="43.2">
       <c r="A25" s="11" t="s">
         <v>237</v>
       </c>
@@ -2100,7 +2083,7 @@
       <c r="J25" s="3"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:15" hidden="1">
+    <row r="26" spans="1:15">
       <c r="A26" s="8" t="s">
         <v>235</v>
       </c>
@@ -2129,7 +2112,7 @@
       <c r="J26" s="3"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" ht="28.8" hidden="1">
+    <row r="27" spans="1:15" ht="28.8">
       <c r="A27" s="8" t="s">
         <v>171</v>
       </c>
@@ -2161,7 +2144,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="28.8" hidden="1">
+    <row r="28" spans="1:15" ht="28.8">
       <c r="A28" s="8" t="s">
         <v>170</v>
       </c>
@@ -2193,7 +2176,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="43.2" hidden="1">
+    <row r="29" spans="1:15" ht="43.2">
       <c r="A29" s="4" t="s">
         <v>166</v>
       </c>
@@ -2227,7 +2210,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="57.6" hidden="1">
+    <row r="30" spans="1:15" ht="57.6">
       <c r="A30" s="4" t="s">
         <v>168</v>
       </c>
@@ -2261,7 +2244,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="28.8" hidden="1">
+    <row r="31" spans="1:15" ht="28.8">
       <c r="A31" s="8" t="s">
         <v>172</v>
       </c>
@@ -2293,7 +2276,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="28.8" hidden="1">
+    <row r="32" spans="1:15" ht="28.8">
       <c r="A32" s="4" t="s">
         <v>164</v>
       </c>
@@ -2327,7 +2310,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1">
+    <row r="33" spans="1:16">
       <c r="A33" s="8" t="s">
         <v>173</v>
       </c>
@@ -2355,7 +2338,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:16" ht="43.2" hidden="1">
+    <row r="34" spans="1:16" ht="43.2">
       <c r="A34" s="4" t="s">
         <v>160</v>
       </c>
@@ -2389,7 +2372,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1">
+    <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
         <v>142</v>
       </c>
@@ -2423,7 +2406,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
         <v>141</v>
       </c>
@@ -2458,7 +2441,7 @@
       <c r="L36" s="6"/>
       <c r="P36"/>
     </row>
-    <row r="37" spans="1:16" ht="28.8" hidden="1">
+    <row r="37" spans="1:16" ht="28.8">
       <c r="A37" s="4" t="s">
         <v>143</v>
       </c>
@@ -2496,7 +2479,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="43.2" hidden="1">
+    <row r="38" spans="1:16" ht="43.2">
       <c r="A38" s="4" t="s">
         <v>144</v>
       </c>
@@ -2534,7 +2517,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="57.6" hidden="1">
+    <row r="39" spans="1:16" ht="57.6">
       <c r="A39" s="4" t="s">
         <v>156</v>
       </c>
@@ -2568,7 +2551,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="43.2" hidden="1">
+    <row r="40" spans="1:16" ht="43.2">
       <c r="A40" s="4" t="s">
         <v>118</v>
       </c>
@@ -2606,7 +2589,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="72" hidden="1">
+    <row r="41" spans="1:16" ht="72">
       <c r="A41" s="4" t="s">
         <v>117</v>
       </c>
@@ -2640,7 +2623,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="43.2" hidden="1">
+    <row r="42" spans="1:16" ht="43.2">
       <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
@@ -2674,7 +2657,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="28.8" hidden="1">
+    <row r="43" spans="1:16" ht="28.8">
       <c r="A43" s="4" t="s">
         <v>111</v>
       </c>
@@ -2712,7 +2695,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1">
+    <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
         <v>110</v>
       </c>
@@ -2746,7 +2729,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:16" hidden="1">
+    <row r="45" spans="1:16">
       <c r="A45" s="4" t="s">
         <v>109</v>
       </c>
@@ -2780,7 +2763,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:16" ht="43.2" hidden="1">
+    <row r="46" spans="1:16" ht="43.2">
       <c r="A46" s="8" t="s">
         <v>108</v>
       </c>
@@ -2814,7 +2797,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="28.8" hidden="1">
+    <row r="47" spans="1:16" ht="28.8">
       <c r="A47" s="8" t="s">
         <v>107</v>
       </c>
@@ -2852,7 +2835,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="43.2" hidden="1">
+    <row r="48" spans="1:16" ht="43.2">
       <c r="A48" s="4" t="s">
         <v>114</v>
       </c>
@@ -2890,7 +2873,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="43.2" hidden="1">
+    <row r="49" spans="1:15" ht="43.2">
       <c r="A49" s="4" t="s">
         <v>115</v>
       </c>
@@ -2928,7 +2911,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="28.8" hidden="1">
+    <row r="50" spans="1:15" ht="28.8">
       <c r="A50" s="4" t="s">
         <v>113</v>
       </c>
@@ -2962,7 +2945,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="28.8" hidden="1">
+    <row r="51" spans="1:15" ht="28.8">
       <c r="A51" s="8" t="s">
         <v>139</v>
       </c>
@@ -2996,7 +2979,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="28.8" hidden="1">
+    <row r="52" spans="1:15" ht="28.8">
       <c r="A52" s="8" t="s">
         <v>138</v>
       </c>
@@ -3030,7 +3013,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="28.8" hidden="1">
+    <row r="53" spans="1:15" ht="28.8">
       <c r="A53" s="4" t="s">
         <v>112</v>
       </c>
@@ -3068,7 +3051,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1">
+    <row r="54" spans="1:15">
       <c r="A54" s="4" t="s">
         <v>134</v>
       </c>
@@ -3106,7 +3089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="43.2" hidden="1">
+    <row r="55" spans="1:15" ht="43.2">
       <c r="A55" s="4" t="s">
         <v>119</v>
       </c>
@@ -3140,7 +3123,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="57.6" hidden="1">
+    <row r="56" spans="1:15" ht="57.6">
       <c r="A56" s="4" t="s">
         <v>140</v>
       </c>
@@ -3251,7 +3234,7 @@
       </c>
       <c r="O58" s="9"/>
     </row>
-    <row r="59" spans="1:15" ht="28.8" hidden="1">
+    <row r="59" spans="1:15" ht="28.8">
       <c r="A59" s="8" t="s">
         <v>162</v>
       </c>
@@ -3280,7 +3263,7 @@
       <c r="J59" s="3"/>
       <c r="O59" s="9"/>
     </row>
-    <row r="60" spans="1:15" ht="28.8" hidden="1">
+    <row r="60" spans="1:15" ht="28.8">
       <c r="A60" s="8" t="s">
         <v>161</v>
       </c>
@@ -3309,7 +3292,7 @@
       <c r="J60" s="3"/>
       <c r="O60" s="9"/>
     </row>
-    <row r="61" spans="1:15" ht="28.8" hidden="1">
+    <row r="61" spans="1:15" ht="28.8">
       <c r="A61" s="8" t="s">
         <v>163</v>
       </c>
@@ -3339,7 +3322,7 @@
       <c r="O61" s="9"/>
     </row>
     <row r="62" spans="1:15" ht="28.8">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>157</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -3374,7 +3357,7 @@
       <c r="O62" s="9"/>
     </row>
     <row r="63" spans="1:15" ht="43.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>158</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -3410,21 +3393,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
-    <cfRule type="cellIs" dxfId="11" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
-    <cfRule type="cellIs" dxfId="7" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Replaced Type "def" tests with "definition"
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -449,18 +449,6 @@
     <t>type_name_spellcheck</t>
   </si>
   <si>
-    <t>type_def_missing_simple</t>
-  </si>
-  <si>
-    <t>type_def_missing_complex</t>
-  </si>
-  <si>
-    <t>type_def_phrase_complex</t>
-  </si>
-  <si>
-    <t>type_def_phrase_simple</t>
-  </si>
-  <si>
     <t>Type namespace prefixes must be defined.</t>
   </si>
   <si>
@@ -494,9 +482,6 @@
     <t>Types with names that end with "MetadataType" must have style "metadata".</t>
   </si>
   <si>
-    <t>type_def_spellcheck</t>
-  </si>
-  <si>
     <t>type_style_missing</t>
   </si>
   <si>
@@ -701,12 +686,6 @@
     <t>facet_value_duplicate</t>
   </si>
   <si>
-    <t>facet_def_missing_code</t>
-  </si>
-  <si>
-    <t>facet_def_missing_pattern</t>
-  </si>
-  <si>
     <t>facet_kind_invalid</t>
   </si>
   <si>
@@ -722,6 +701,9 @@
     <t>property_name_spellcheck</t>
   </si>
   <si>
+    <t>property_definition_spellcheck</t>
+  </si>
+  <si>
     <t>property_type_abstract</t>
   </si>
   <si>
@@ -746,9 +728,6 @@
     <t>Concrete elements and attributes</t>
   </si>
   <si>
-    <t>property_def_spellcheck</t>
-  </si>
-  <si>
     <t>property_group_invalid</t>
   </si>
   <si>
@@ -780,6 +759,27 @@
   </si>
   <si>
     <t>Type PersonType has permitted style 'object'.</t>
+  </si>
+  <si>
+    <t>type_definition_missing_complex</t>
+  </si>
+  <si>
+    <t>type_definition_missing_simple</t>
+  </si>
+  <si>
+    <t>type_definition_phrase_complex</t>
+  </si>
+  <si>
+    <t>type_definition_phrase_simple</t>
+  </si>
+  <si>
+    <t>type_definition_spellcheck</t>
+  </si>
+  <si>
+    <t>facet_definition_missing_code</t>
+  </si>
+  <si>
+    <t>facet_definition_missing_pattern</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1311,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="5" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>74</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="5" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>90</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="4" spans="1:16" ht="28.8">
       <c r="A4" s="5" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>78</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>66</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>67</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>70</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>68</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>89</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>69</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>73</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="12" spans="1:16" ht="28.8">
       <c r="A12" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>72</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="13" spans="1:16" ht="28.8">
       <c r="A13" s="8" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>88</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="14" spans="1:16" ht="28.8">
       <c r="A14" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>41</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="16" spans="1:16" ht="28.8">
       <c r="A16" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="17" spans="1:15" ht="28.8">
       <c r="A17" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>87</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="19" spans="1:15" ht="28.8">
       <c r="A19" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>32</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="20" spans="1:15" ht="28.8">
       <c r="A20" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>42</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="21" spans="1:15" ht="28.8">
       <c r="A21" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>43</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="22" spans="1:15" ht="28.8">
       <c r="A22" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>37</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="24" spans="1:15" ht="28.8">
       <c r="A24" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="25" spans="1:15" ht="43.2">
       <c r="A25" s="11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="8" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>38</v>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="27" spans="1:15" ht="28.8">
       <c r="A27" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -2141,15 +2141,15 @@
         <v>91</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="28.8">
       <c r="A28" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>20</v>
@@ -2173,15 +2173,15 @@
         <v>91</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="43.2">
       <c r="A29" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>20</v>
@@ -2204,18 +2204,18 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="57.6">
       <c r="A30" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>20</v>
@@ -2238,18 +2238,18 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="28.8">
       <c r="A31" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>20</v>
@@ -2273,15 +2273,15 @@
         <v>91</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="28.8">
       <c r="A32" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -2304,18 +2304,18 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>20</v>
@@ -2340,10 +2340,10 @@
     </row>
     <row r="34" spans="1:16" ht="43.2">
       <c r="A34" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>39</v>
@@ -2366,18 +2366,18 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>142</v>
+        <v>245</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>18</v>
@@ -2408,10 +2408,10 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
-        <v>141</v>
+        <v>246</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>18</v>
@@ -2443,10 +2443,10 @@
     </row>
     <row r="37" spans="1:16" ht="28.8">
       <c r="A37" s="4" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>45</v>
@@ -2473,18 +2473,18 @@
         <v>85</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="43.2">
       <c r="A38" s="4" t="s">
-        <v>144</v>
+        <v>248</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>45</v>
@@ -2511,18 +2511,18 @@
         <v>86</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="57.6">
       <c r="A39" s="4" t="s">
-        <v>156</v>
+        <v>249</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>20</v>
@@ -2545,10 +2545,10 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="43.2">
@@ -2583,10 +2583,10 @@
         <v>59</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="72">
@@ -2617,10 +2617,10 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="43.2">
@@ -2791,10 +2791,10 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="28.8">
@@ -2826,13 +2826,13 @@
         <v>91</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="43.2">
@@ -2973,10 +2973,10 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="28.8">
@@ -3007,10 +3007,10 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8">
@@ -3117,10 +3117,10 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="57.6">
@@ -3152,24 +3152,24 @@
         <v>91</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="O56" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="28.8">
       <c r="A57" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
@@ -3192,19 +3192,19 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="O57" s="9"/>
     </row>
     <row r="58" spans="1:15" ht="43.2">
       <c r="A58" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>20</v>
@@ -3227,19 +3227,19 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="2" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="O58" s="9"/>
     </row>
     <row r="59" spans="1:15" ht="28.8">
       <c r="A59" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>20</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="60" spans="1:15" ht="28.8">
       <c r="A60" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>20</v>
@@ -3294,10 +3294,10 @@
     </row>
     <row r="61" spans="1:15" ht="28.8">
       <c r="A61" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>20</v>
@@ -3323,10 +3323,10 @@
     </row>
     <row r="62" spans="1:15" ht="28.8">
       <c r="A62" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>18</v>
@@ -3349,19 +3349,19 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="O62" s="9"/>
     </row>
     <row r="63" spans="1:15" ht="43.2">
       <c r="A63" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>20</v>
@@ -3384,10 +3384,10 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="O63" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added first Facet test and refactored classes
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="255">
   <si>
     <t>Field</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>Code simple types</t>
-  </si>
-  <si>
     <t>Scope</t>
   </si>
   <si>
@@ -83,54 +80,27 @@
     <t>Missing value</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Invalid value</t>
   </si>
   <si>
     <t>Property</t>
   </si>
   <si>
-    <t>Prefix</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>IsElement</t>
-  </si>
-  <si>
     <t>Duplicate</t>
   </si>
   <si>
     <t>An element name must begin with an upper case letter.</t>
   </si>
   <si>
-    <t>Elements</t>
-  </si>
-  <si>
     <t>An attribute name must begin with a lower case letter.</t>
   </si>
   <si>
-    <t>Attributes</t>
-  </si>
-  <si>
     <t>A term in a property name that does not exist in the dictionary must be defined as Local Terminology.</t>
   </si>
   <si>
     <t>An abstract element should probably not have a data type.</t>
   </si>
   <si>
-    <t>Abstract elements</t>
-  </si>
-  <si>
     <t>warning</t>
   </si>
   <si>
@@ -158,111 +128,39 @@
     <t>A property with a substitution group must be an element.</t>
   </si>
   <si>
-    <t>Substitutable elements</t>
-  </si>
-  <si>
     <t>Definition phrasing</t>
   </si>
   <si>
     <t>Style</t>
   </si>
   <si>
-    <t>Base</t>
-  </si>
-  <si>
     <t>10-45</t>
   </si>
   <si>
     <t>11-1</t>
   </si>
   <si>
-    <t>Simple types</t>
-  </si>
-  <si>
     <t>11-3</t>
   </si>
   <si>
-    <t>Complex types</t>
-  </si>
-  <si>
-    <t>Augmentation types</t>
-  </si>
-  <si>
-    <t>Association types</t>
-  </si>
-  <si>
-    <t>Metadata types</t>
-  </si>
-  <si>
-    <t>List types</t>
-  </si>
-  <si>
-    <t>Code types</t>
-  </si>
-  <si>
     <t>10-18</t>
   </si>
   <si>
     <t>10-49</t>
   </si>
   <si>
-    <t>Simple content types</t>
-  </si>
-  <si>
     <t>CSC types</t>
   </si>
   <si>
-    <t>Union types</t>
-  </si>
-  <si>
     <t>Facet</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Kind</t>
-  </si>
-  <si>
-    <t>A facet must have a type namespace prefix.</t>
-  </si>
-  <si>
-    <t>A facet must have a valid type namespace prefix.</t>
-  </si>
-  <si>
-    <t>A facet must have a type name.</t>
-  </si>
-  <si>
-    <t>A facet must have a valid type name.</t>
-  </si>
-  <si>
-    <t>A facet must belong to a simple type.</t>
-  </si>
-  <si>
-    <t>Enumerations</t>
-  </si>
-  <si>
-    <t>A facet must have a value (e.g., code value, pattern value, etc).</t>
-  </si>
-  <si>
-    <t>A facet value should probably be unique within its type.</t>
-  </si>
-  <si>
-    <t>An enumeration must have a definition.</t>
-  </si>
-  <si>
     <t>9-14</t>
   </si>
   <si>
-    <t>Patterns</t>
-  </si>
-  <si>
     <t>info</t>
   </si>
   <si>
-    <t>A facet must have a valid style (e.g., enumeration, pattern, etc.).</t>
-  </si>
-  <si>
     <t>9-25</t>
   </si>
   <si>
@@ -293,12 +191,6 @@
     <t>A term in a property definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
   </si>
   <si>
-    <t>An enumeration must belong to type with a name that ends in "CodeSimpleType"</t>
-  </si>
-  <si>
-    <t>A pattern should probably have a definition.</t>
-  </si>
-  <si>
     <t>NDR 4.0</t>
   </si>
   <si>
@@ -662,15 +554,6 @@
     <t>Types must have a namespace prefix.</t>
   </si>
   <si>
-    <t>facet_prefix_missing</t>
-  </si>
-  <si>
-    <t>facet_prefix_unknown</t>
-  </si>
-  <si>
-    <t>facet_type_missing</t>
-  </si>
-  <si>
     <t>facet_type_unknown</t>
   </si>
   <si>
@@ -725,9 +608,6 @@
     <t>A property that is not abstract must have a data type.</t>
   </si>
   <si>
-    <t>Concrete elements and attributes</t>
-  </si>
-  <si>
     <t>property_group_invalid</t>
   </si>
   <si>
@@ -780,6 +660,135 @@
   </si>
   <si>
     <t>facet_definition_missing_pattern</t>
+  </si>
+  <si>
+    <t>Codes (enumerations) must have definitions.</t>
+  </si>
+  <si>
+    <t>Pattern should probably have a definition to make it easier for other users to understand the intended values.</t>
+  </si>
+  <si>
+    <t>Facets must have a valid style (e.g., enumeration, pattern, etc.).</t>
+  </si>
+  <si>
+    <t>Facets cannot belong to a complex type.</t>
+  </si>
+  <si>
+    <t>Codes must belong to types whose names end with "CodeSimpleType"</t>
+  </si>
+  <si>
+    <t>It is recommended that codes should be unique within their type.</t>
+  </si>
+  <si>
+    <t>Facets must have a value (e.g., a code value or a pattern value, etc).</t>
+  </si>
+  <si>
+    <t>facet_definition_duplicate</t>
+  </si>
+  <si>
+    <t>Facets should probably have unique definitions within their type.</t>
+  </si>
+  <si>
+    <t>facet_definition_escaped</t>
+  </si>
+  <si>
+    <t>Facet definitions should not contain escaped apostrophes.</t>
+  </si>
+  <si>
+    <t>Facet definitions should not contain tabs, new lines, or carriage returns.</t>
+  </si>
+  <si>
+    <t>facet_definition_formatting</t>
+  </si>
+  <si>
+    <t>Facet values should not contain leading or trailing spaces.</t>
+  </si>
+  <si>
+    <t>facet_value_spaces</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>abstract elements</t>
+  </si>
+  <si>
+    <t>association types</t>
+  </si>
+  <si>
+    <t>augmentation types</t>
+  </si>
+  <si>
+    <t>code types</t>
+  </si>
+  <si>
+    <t>code simple types</t>
+  </si>
+  <si>
+    <t>complex types</t>
+  </si>
+  <si>
+    <t>substitutable elements</t>
+  </si>
+  <si>
+    <t>concrete elements and attributes</t>
+  </si>
+  <si>
+    <t>union types</t>
+  </si>
+  <si>
+    <t>enumerations</t>
+  </si>
+  <si>
+    <t>patterns</t>
+  </si>
+  <si>
+    <t>simple types</t>
+  </si>
+  <si>
+    <t>simple content types</t>
+  </si>
+  <si>
+    <t>metadata types</t>
+  </si>
+  <si>
+    <t>list types</t>
+  </si>
+  <si>
+    <t>Facets must belong to an existing type.</t>
   </si>
 </sst>
 </file>
@@ -858,7 +867,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,6 +903,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -901,25 +913,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -966,6 +959,25 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1016,8 +1028,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O63" totalsRowShown="0">
-  <autoFilter ref="A1:O63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O64" totalsRowShown="0">
+  <autoFilter ref="A1:O64"/>
   <sortState ref="A2:O63">
     <sortCondition ref="A1:A63"/>
   </sortState>
@@ -1031,12 +1043,12 @@
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
     <tableColumn id="21" name="Spec" dataDxfId="11"/>
-    <tableColumn id="18" name="Rules" dataDxfId="3"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="1"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="5"/>
-    <tableColumn id="19" name="Notes" dataDxfId="4"/>
+    <tableColumn id="18" name="Rules" dataDxfId="8"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="6"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="10"/>
+    <tableColumn id="19" name="Notes" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1305,13 +1317,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1348,117 +1360,119 @@
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="5" t="s">
-        <v>250</v>
+    <row r="2" spans="1:16" ht="28.8">
+      <c r="A2" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="O2" s="9"/>
+      <c r="P2"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="5" t="s">
-        <v>251</v>
+      <c r="A3" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>76</v>
+        <v>228</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
       <c r="O3" s="9"/>
-    </row>
-    <row r="4" spans="1:16" ht="28.8">
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="5" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>248</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1466,86 +1480,92 @@
       <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="28.8">
       <c r="A5" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>213</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>249</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="5" t="s">
-        <v>213</v>
+    <row r="6" spans="1:16" ht="28.8">
+      <c r="A6" s="8" t="s">
+        <v>224</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>223</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="28.8">
       <c r="A7" s="5" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>233</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1559,22 +1579,22 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="5" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1588,22 +1608,22 @@
     </row>
     <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="5" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1615,28 +1635,28 @@
         <v>6</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="5" t="s">
-        <v>215</v>
+      <c r="A10" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>254</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1648,30 +1668,30 @@
       <c r="J10" s="6"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" ht="28.8">
       <c r="A11" s="5" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>227</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1679,22 +1699,22 @@
     </row>
     <row r="12" spans="1:16" ht="28.8">
       <c r="A12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>227</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1706,82 +1726,84 @@
       <c r="J12" s="6"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:16" ht="28.8">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>227</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:16" ht="28.8">
       <c r="A14" s="8" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
+        <v>229</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
         <v>25</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" t="s">
-        <v>3</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" ht="28.8">
       <c r="A15" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
         <v>230</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>29</v>
+        <v>237</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1793,24 +1815,24 @@
       <c r="J15" s="3"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:16" ht="28.8">
+    <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1824,22 +1846,22 @@
     </row>
     <row r="17" spans="1:15" ht="28.8">
       <c r="A17" s="8" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1851,24 +1873,24 @@
       <c r="J17" s="3"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" ht="28.8">
       <c r="A18" s="8" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>237</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
@@ -1880,24 +1902,24 @@
       <c r="J18" s="3"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:15" ht="28.8">
+    <row r="19" spans="1:15">
       <c r="A19" s="8" t="s">
-        <v>224</v>
+        <v>182</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -1911,22 +1933,22 @@
     </row>
     <row r="20" spans="1:15" ht="28.8">
       <c r="A20" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
         <v>235</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -1940,22 +1962,22 @@
     </row>
     <row r="21" spans="1:15" ht="28.8">
       <c r="A21" s="8" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>232</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>239</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -1969,80 +1991,80 @@
     </row>
     <row r="22" spans="1:15" ht="28.8">
       <c r="A22" s="8" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>34</v>
+        <v>245</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" ht="28.8">
       <c r="A23" s="8" t="s">
-        <v>228</v>
+        <v>187</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:15" ht="28.8">
+    <row r="24" spans="1:15">
       <c r="A24" s="8" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2054,24 +2076,24 @@
       <c r="J24" s="3"/>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="1:15" ht="43.2">
-      <c r="A25" s="11" t="s">
-        <v>231</v>
+    <row r="25" spans="1:15" ht="28.8">
+      <c r="A25" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>232</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2083,24 +2105,24 @@
       <c r="J25" s="3"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="8" t="s">
-        <v>229</v>
+    <row r="26" spans="1:15" ht="43.2">
+      <c r="A26" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>19</v>
+        <v>246</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2112,24 +2134,24 @@
       <c r="J26" s="3"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" ht="28.8">
+    <row r="27" spans="1:15">
       <c r="A27" s="8" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>54</v>
+        <v>228</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2137,31 +2159,28 @@
       <c r="H27" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="O27" s="9"/>
     </row>
     <row r="28" spans="1:15" ht="28.8">
       <c r="A28" s="8" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2170,30 +2189,30 @@
         <v>3</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="43.2">
-      <c r="A29" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="28.8">
+      <c r="A29" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>61</v>
+        <v>241</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2201,87 +2220,87 @@
       <c r="H29" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="57.6">
+      <c r="I29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="43.2">
       <c r="A30" s="4" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>205</v>
+        <v>126</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="2" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="28.8">
-      <c r="A31" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="57.6">
+      <c r="A31" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>231</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>192</v>
+      <c r="L31" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="28.8">
-      <c r="A32" s="4" t="s">
-        <v>159</v>
+      <c r="A32" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -2290,10 +2309,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>60</v>
+        <v>252</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2301,33 +2320,31 @@
       <c r="H32" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="8" t="s">
-        <v>168</v>
+      <c r="I32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="28.8">
+      <c r="A33" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>62</v>
+        <v>251</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2337,25 +2354,31 @@
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" ht="43.2">
-      <c r="A34" s="4" t="s">
-        <v>155</v>
+      <c r="K33" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2365,31 +2388,25 @@
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+    </row>
+    <row r="35" spans="1:16" ht="43.2">
       <c r="A35" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B35" t="s">
-        <v>143</v>
+        <v>119</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>231</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>52</v>
+        <v>228</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2397,216 +2414,212 @@
       <c r="H35" t="s">
         <v>3</v>
       </c>
-      <c r="I35" t="s">
-        <v>6</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>142</v>
+        <v>205</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="G36" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
-      <c r="P36"/>
-    </row>
-    <row r="37" spans="1:16" ht="28.8">
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="4" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>52</v>
+        <v>250</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="43.2">
+        <v>49</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="P37"/>
+    </row>
+    <row r="38" spans="1:16" ht="28.8">
       <c r="A38" s="4" t="s">
-        <v>248</v>
+        <v>207</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>50</v>
+        <v>244</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I38" t="s">
         <v>6</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="57.6">
+        <v>51</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="43.2">
       <c r="A39" s="4" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="K39" s="2" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="43.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="57.6">
       <c r="A40" s="4" t="s">
-        <v>118</v>
+        <v>209</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
+        <v>229</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>3</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
       <c r="K40" s="2" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="72">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="43.2">
       <c r="A41" s="4" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2614,21 +2627,25 @@
       <c r="H41" t="s">
         <v>3</v>
       </c>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
+      <c r="I41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="K41" s="2" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="43.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="72">
       <c r="A42" s="4" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>20</v>
@@ -2637,70 +2654,66 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>57</v>
+        <v>228</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="2" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="28.8">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="43.2">
       <c r="A43" s="4" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>19</v>
+        <v>242</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
       <c r="K43" s="2" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="28.8">
       <c r="A44" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>18</v>
@@ -2709,10 +2722,10 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>52</v>
+        <v>228</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2721,32 +2734,36 @@
         <v>3</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="4" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>50</v>
+        <v>244</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2755,32 +2772,32 @@
         <v>3</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:16" ht="43.2">
-      <c r="A46" s="8" t="s">
-        <v>108</v>
+    <row r="46" spans="1:16">
+      <c r="A46" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2788,21 +2805,21 @@
       <c r="H46" t="s">
         <v>3</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="28.8">
+      <c r="I46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="1:16" ht="43.2">
       <c r="A47" s="8" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>7</v>
@@ -2811,10 +2828,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2822,25 +2839,21 @@
       <c r="H47" t="s">
         <v>3</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
       <c r="K47" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="43.2">
-      <c r="A48" s="4" t="s">
-        <v>114</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="28.8">
+      <c r="A48" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>7</v>
@@ -2849,10 +2862,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2861,24 +2874,24 @@
         <v>3</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="43.2">
       <c r="A49" s="4" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>7</v>
@@ -2887,36 +2900,36 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>57</v>
+        <v>243</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="I49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J49" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="28.8">
+    </row>
+    <row r="50" spans="1:15" ht="43.2">
       <c r="A50" s="4" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>7</v>
@@ -2925,32 +2938,36 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>52</v>
+        <v>242</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>3</v>
-      </c>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="K50" s="2" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="28.8">
-      <c r="A51" s="8" t="s">
-        <v>139</v>
+      <c r="A51" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>7</v>
@@ -2959,10 +2976,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>56</v>
+        <v>244</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -2973,18 +2990,18 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="2" t="s">
-        <v>179</v>
+        <v>93</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="28.8">
       <c r="A52" s="8" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>7</v>
@@ -2993,10 +3010,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>55</v>
+        <v>253</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3007,18 +3024,18 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="2" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8">
-      <c r="A53" s="4" t="s">
-        <v>112</v>
+      <c r="A53" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>7</v>
@@ -3027,10 +3044,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>50</v>
+        <v>252</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3038,25 +3055,21 @@
       <c r="H53" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
       <c r="K53" s="2" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="28.8">
       <c r="A54" s="4" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>7</v>
@@ -3065,10 +3078,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3077,58 +3090,62 @@
         <v>3</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="43.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="4" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>35</v>
-      </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="K55" s="2" t="s">
-        <v>183</v>
+        <v>96</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="57.6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="43.2">
       <c r="A56" s="4" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>18</v>
@@ -3137,51 +3154,44 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>3</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>193</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
       <c r="K56" s="2" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="O56" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="28.8">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="57.6">
       <c r="A57" s="4" t="s">
-        <v>210</v>
+        <v>104</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>211</v>
+        <v>85</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>22</v>
+        <v>235</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3189,34 +3199,40 @@
       <c r="H57" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
+      <c r="I57" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="K57" s="2" t="s">
-        <v>237</v>
+        <v>151</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="O57" s="9"/>
-    </row>
-    <row r="58" spans="1:15" ht="43.2">
+        <v>152</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="28.8">
       <c r="A58" s="4" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>22</v>
+        <v>236</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3227,31 +3243,31 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="2" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="O58" s="9"/>
     </row>
-    <row r="59" spans="1:15" ht="28.8">
-      <c r="A59" s="8" t="s">
-        <v>157</v>
+    <row r="59" spans="1:15" ht="43.2">
+      <c r="A59" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
+        <v>236</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>54</v>
+        <v>228</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3259,28 +3275,34 @@
       <c r="H59" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="O59" s="9"/>
     </row>
     <row r="60" spans="1:15" ht="28.8">
       <c r="A60" s="8" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>53</v>
+        <v>240</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3294,22 +3316,22 @@
     </row>
     <row r="61" spans="1:15" ht="28.8">
       <c r="A61" s="8" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>55</v>
+        <v>241</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3322,11 +3344,11 @@
       <c r="O61" s="9"/>
     </row>
     <row r="62" spans="1:15" ht="28.8">
-      <c r="A62" s="4" t="s">
-        <v>152</v>
+      <c r="A62" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>18</v>
@@ -3335,10 +3357,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3346,34 +3368,28 @@
       <c r="H62" t="s">
         <v>3</v>
       </c>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>242</v>
-      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
       <c r="O62" s="9"/>
     </row>
-    <row r="63" spans="1:15" ht="43.2">
+    <row r="63" spans="1:15" ht="28.8">
       <c r="A63" s="4" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3384,30 +3400,65 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="2" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="O63" s="9"/>
     </row>
+    <row r="64" spans="1:15" ht="43.2">
+      <c r="A64" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" t="s">
+        <v>3</v>
+      </c>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="O64" s="9"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
-    <cfRule type="cellIs" dxfId="10" priority="50" operator="equal">
+  <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M64:O1048576 P37:P1048576 P2:P35">
-    <cfRule type="cellIs" dxfId="6" priority="25" operator="equal">
+  <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Type test examples
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -464,9 +464,6 @@
     <t>Types 'justice:CaseType' and 'logistics:CaseType' are valid because even though they use the same name, they are defined in different namespaces.</t>
   </si>
   <si>
-    <t>Type name 'CaseType' cannot be defined twice in the same namespace.</t>
-  </si>
-  <si>
     <t>Type name 'IDCategoryCodeType' is valid because the term 'Type' only appears at the end of the name.</t>
   </si>
   <si>
@@ -626,9 +623,6 @@
     <t>Type PersonType has style 'object'.</t>
   </si>
   <si>
-    <t>Type PersonType cannot have a missing style.</t>
-  </si>
-  <si>
     <t>Type PersonType cannot have unknown style 'myCustomObject'.</t>
   </si>
   <si>
@@ -816,13 +810,19 @@
   </si>
   <si>
     <t>Type 'WeekdayCodeSimpleType' with codes 'MON', 'MON', 'MON', ...</t>
+  </si>
+  <si>
+    <t>Type name 'CaseType' cannot be defined twice in the justice namespace.</t>
+  </si>
+  <si>
+    <t>Type PersonType does not have a style.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,20 +839,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -863,7 +849,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,18 +863,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -901,13 +877,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,17 +895,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -940,7 +908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -950,10 +918,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -1364,25 +1330,25 @@
   <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30" style="8" customWidth="1"/>
+    <col min="1" max="1" width="30" style="7" customWidth="1"/>
     <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
     <col min="4" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" style="6" customWidth="1"/>
     <col min="11" max="12" width="34.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="26.77734375" style="10" customWidth="1"/>
-    <col min="15" max="15" width="27.21875" style="11" customWidth="1"/>
+    <col min="13" max="14" width="26.77734375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="27.21875" style="9" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" style="1"/>
     <col min="17" max="17" width="31.5546875" customWidth="1"/>
   </cols>
@@ -1424,23 +1390,23 @@
       <c r="L1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="9" t="s">
         <v>56</v>
       </c>
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" ht="28.8">
-      <c r="A2" s="8" t="s">
-        <v>217</v>
+      <c r="A2" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -1449,10 +1415,10 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1460,19 +1426,19 @@
       <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="O2" s="10"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="O2" s="8"/>
       <c r="P2"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="8" t="s">
-        <v>219</v>
+      <c r="A3" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
@@ -1481,10 +1447,10 @@
         <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1492,19 +1458,19 @@
       <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="O3" s="10"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="O3" s="8"/>
       <c r="P3"/>
     </row>
     <row r="4" spans="1:16" ht="28.8">
       <c r="A4" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
@@ -1513,10 +1479,10 @@
         <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1530,20 +1496,20 @@
       <c r="J4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="O4" s="10"/>
+      <c r="K4" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:16" ht="57.6">
       <c r="A5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>17</v>
@@ -1552,10 +1518,10 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1563,22 +1529,22 @@
       <c r="H5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="O5" s="10"/>
+        <v>258</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="28.8">
-      <c r="A6" s="8" t="s">
-        <v>222</v>
+      <c r="A6" s="7" t="s">
+        <v>220</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1587,10 +1553,10 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1598,18 +1564,18 @@
       <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="O6" s="10"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="7" spans="1:16" ht="28.8">
       <c r="A7" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1618,10 +1584,10 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1629,16 +1595,16 @@
       <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="O7" s="10"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:16" ht="28.8">
       <c r="A8" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -1647,10 +1613,10 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1658,22 +1624,22 @@
       <c r="H8" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="O8" s="10"/>
+        <v>255</v>
+      </c>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
@@ -1682,10 +1648,10 @@
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1700,19 +1666,19 @@
         <v>47</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="O9" s="10"/>
+        <v>253</v>
+      </c>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -1721,10 +1687,10 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1732,18 +1698,18 @@
       <c r="H10" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="O10" s="10"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:16" ht="28.8">
-      <c r="A11" s="9" t="s">
-        <v>261</v>
+      <c r="A11" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -1752,10 +1718,10 @@
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1763,22 +1729,22 @@
       <c r="H11" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="O11" s="10"/>
+        <v>261</v>
+      </c>
+      <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="28.8">
-      <c r="A12" s="5" t="s">
-        <v>178</v>
+      <c r="A12" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>17</v>
@@ -1787,10 +1753,10 @@
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1798,16 +1764,18 @@
       <c r="H12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="O12" s="10"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="12" t="s">
-        <v>224</v>
+      <c r="A13" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
@@ -1816,10 +1784,10 @@
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -1827,15 +1795,15 @@
       <c r="H13" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="O13" s="10"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:16" ht="28.8">
-      <c r="A14" s="8" t="s">
-        <v>184</v>
+      <c r="A14" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>54</v>
@@ -1847,10 +1815,10 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
@@ -1860,11 +1828,11 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="O14" s="10"/>
+      <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="28.8">
-      <c r="A15" s="8" t="s">
-        <v>192</v>
+      <c r="A15" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>31</v>
@@ -1876,10 +1844,10 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1889,11 +1857,11 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="O15" s="10"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="8" t="s">
-        <v>189</v>
+      <c r="A16" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -1905,10 +1873,10 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1918,11 +1886,11 @@
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="O16" s="10"/>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15" ht="28.8">
-      <c r="A17" s="8" t="s">
-        <v>182</v>
+      <c r="A17" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -1934,10 +1902,10 @@
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1947,11 +1915,11 @@
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" ht="28.8">
-      <c r="A18" s="8" t="s">
-        <v>181</v>
+      <c r="A18" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
@@ -1963,10 +1931,10 @@
         <v>19</v>
       </c>
       <c r="E18" t="s">
+        <v>231</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
@@ -1976,11 +1944,11 @@
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="8" t="s">
-        <v>180</v>
+      <c r="A19" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>53</v>
@@ -1992,10 +1960,10 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -2005,11 +1973,11 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" ht="28.8">
-      <c r="A20" s="8" t="s">
-        <v>183</v>
+      <c r="A20" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -2021,10 +1989,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2034,11 +2002,11 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="O20" s="10"/>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" ht="28.8">
-      <c r="A21" s="8" t="s">
-        <v>193</v>
+      <c r="A21" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>32</v>
@@ -2050,10 +2018,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2063,11 +2031,11 @@
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="O21" s="10"/>
+      <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" ht="28.8">
-      <c r="A22" s="8" t="s">
-        <v>194</v>
+      <c r="A22" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
@@ -2079,10 +2047,10 @@
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2092,11 +2060,11 @@
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="O22" s="10"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" ht="28.8">
-      <c r="A23" s="8" t="s">
-        <v>185</v>
+      <c r="A23" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -2108,10 +2076,10 @@
         <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -2121,11 +2089,11 @@
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="O23" s="10"/>
+      <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="8" t="s">
-        <v>187</v>
+      <c r="A24" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>27</v>
@@ -2137,10 +2105,10 @@
         <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2150,11 +2118,11 @@
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="O24" s="10"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" ht="28.8">
-      <c r="A25" s="8" t="s">
-        <v>186</v>
+      <c r="A25" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
@@ -2166,10 +2134,10 @@
         <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2179,14 +2147,14 @@
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="O25" s="10"/>
+      <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15" ht="43.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
@@ -2195,10 +2163,10 @@
         <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2208,11 +2176,11 @@
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="O26" s="10"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="8" t="s">
-        <v>188</v>
+      <c r="A27" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>28</v>
@@ -2224,10 +2192,10 @@
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2237,10 +2205,10 @@
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="O27" s="10"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" ht="28.8">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2253,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2268,11 +2236,11 @@
         <v>55</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="28.8">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2285,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2300,7 +2268,7 @@
         <v>55</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="43.2">
@@ -2317,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>41</v>
@@ -2328,13 +2296,13 @@
       <c r="H30" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="57.6">
@@ -2342,7 +2310,7 @@
         <v>127</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>18</v>
@@ -2351,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -2362,17 +2330,17 @@
       <c r="H31" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="28.8">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2385,10 +2353,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2400,7 +2368,7 @@
         <v>55</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="28.8">
@@ -2417,10 +2385,10 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2428,17 +2396,17 @@
       <c r="H33" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2451,10 +2419,10 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2462,8 +2430,8 @@
       <c r="H34" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:16" ht="43.2">
       <c r="A35" s="4" t="s">
@@ -2479,10 +2447,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2490,18 +2458,18 @@
       <c r="H35" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
       <c r="K35" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B36" t="s">
         <v>107</v>
@@ -2513,10 +2481,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2527,15 +2495,15 @@
       <c r="I36" t="s">
         <v>6</v>
       </c>
-      <c r="J36" s="7" t="s">
+      <c r="J36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>106</v>
@@ -2547,10 +2515,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2564,13 +2532,13 @@
       <c r="J37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
       <c r="P37"/>
     </row>
     <row r="38" spans="1:16" ht="28.8">
       <c r="A38" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>108</v>
@@ -2582,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -2599,16 +2567,16 @@
       <c r="J38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K38" s="13" t="s">
+      <c r="K38" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="L38" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="43.2">
       <c r="A39" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>109</v>
@@ -2620,10 +2588,10 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -2638,15 +2606,15 @@
         <v>52</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="57.6">
       <c r="A40" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>110</v>
@@ -2658,10 +2626,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2669,13 +2637,13 @@
       <c r="H40" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
       <c r="K40" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="43.2">
@@ -2692,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2710,10 +2678,10 @@
         <v>40</v>
       </c>
       <c r="K41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="72">
@@ -2730,10 +2698,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2741,13 +2709,13 @@
       <c r="H42" t="s">
         <v>3</v>
       </c>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
       <c r="K42" s="2" t="s">
         <v>145</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>146</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="43.2">
@@ -2764,10 +2732,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -2775,8 +2743,8 @@
       <c r="H43" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
       <c r="K43" s="2" t="s">
         <v>86</v>
       </c>
@@ -2798,10 +2766,10 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2836,10 +2804,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2853,8 +2821,8 @@
       <c r="J45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="4" t="s">
@@ -2870,10 +2838,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2887,11 +2855,11 @@
       <c r="J46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:16" ht="43.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2904,10 +2872,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2915,8 +2883,8 @@
       <c r="H47" t="s">
         <v>3</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
       <c r="K47" s="2" t="s">
         <v>139</v>
       </c>
@@ -2925,7 +2893,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" ht="28.8">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2938,10 +2906,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2953,7 +2921,7 @@
         <v>55</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>137</v>
@@ -2976,10 +2944,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3014,10 +2982,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3052,10 +3020,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3063,8 +3031,8 @@
       <c r="H51" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
       <c r="K51" s="2" t="s">
         <v>93</v>
       </c>
@@ -3073,7 +3041,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="28.8">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3086,10 +3054,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3097,8 +3065,8 @@
       <c r="H52" t="s">
         <v>3</v>
       </c>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
       <c r="K52" s="2" t="s">
         <v>143</v>
       </c>
@@ -3107,7 +3075,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -3120,10 +3088,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3131,8 +3099,8 @@
       <c r="H53" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
       <c r="K53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3154,10 +3122,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3192,10 +3160,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3230,10 +3198,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3241,13 +3209,13 @@
       <c r="H56" t="s">
         <v>25</v>
       </c>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
       <c r="K56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="L56" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="57.6">
@@ -3264,10 +3232,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3279,24 +3247,24 @@
         <v>55</v>
       </c>
       <c r="J57" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O57" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="O57" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="28.8">
       <c r="A58" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>17</v>
@@ -3305,10 +3273,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3316,15 +3284,15 @@
       <c r="H58" t="s">
         <v>3</v>
       </c>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
       <c r="K58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L58" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O58" s="10"/>
+      <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:15" ht="43.2">
       <c r="A59" s="4" t="s">
@@ -3340,10 +3308,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3351,18 +3319,18 @@
       <c r="H59" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
       <c r="K59" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L59" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="O59" s="10"/>
+      <c r="O59" s="8"/>
     </row>
     <row r="60" spans="1:15" ht="28.8">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -3378,7 +3346,7 @@
         <v>35</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3388,10 +3356,10 @@
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="O60" s="10"/>
+      <c r="O60" s="8"/>
     </row>
     <row r="61" spans="1:15" ht="28.8">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -3407,7 +3375,7 @@
         <v>35</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3417,10 +3385,10 @@
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="O61" s="10"/>
+      <c r="O61" s="8"/>
     </row>
     <row r="62" spans="1:15" ht="28.8">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -3436,7 +3404,7 @@
         <v>35</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3446,9 +3414,9 @@
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="O62" s="10"/>
-    </row>
-    <row r="63" spans="1:15" ht="28.8">
+      <c r="O62" s="8"/>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="4" t="s">
         <v>116</v>
       </c>
@@ -3465,7 +3433,7 @@
         <v>35</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3473,15 +3441,15 @@
       <c r="H63" t="s">
         <v>3</v>
       </c>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
       <c r="K63" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="O63" s="10"/>
+        <v>263</v>
+      </c>
+      <c r="O63" s="8"/>
     </row>
     <row r="64" spans="1:15" ht="43.2">
       <c r="A64" s="4" t="s">
@@ -3500,7 +3468,7 @@
         <v>35</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3508,15 +3476,15 @@
       <c r="H64" t="s">
         <v>3</v>
       </c>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
       <c r="K64" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="O64" s="10"/>
+        <v>199</v>
+      </c>
+      <c r="O64" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">

</xml_diff>

<commit_message>
Updated for refactored niem-model
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="263">
   <si>
     <t>Field</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Exceptions</t>
-  </si>
-  <si>
-    <t>NDR</t>
   </si>
   <si>
     <t>Rep term</t>
@@ -924,6 +921,60 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C6500"/>
       </font>
@@ -970,60 +1021,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1044,21 +1041,21 @@
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="14"/>
-    <tableColumn id="17" name="Category" dataDxfId="13"/>
+    <tableColumn id="1" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" name="Category" dataDxfId="8"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="12"/>
+    <tableColumn id="14" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="11"/>
-    <tableColumn id="18" name="Rules" dataDxfId="8"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="6"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="10"/>
-    <tableColumn id="19" name="Notes" dataDxfId="9"/>
+    <tableColumn id="21" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" name="Rules" dataDxfId="5"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1333,7 +1330,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1355,76 +1352,76 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" ht="28.8">
       <c r="A2" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1435,22 +1432,22 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1467,102 +1464,102 @@
     </row>
     <row r="4" spans="1:16" ht="28.8">
       <c r="A4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
-        <v>225</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="K4" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:16" ht="57.6">
       <c r="A5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="28.8">
       <c r="A6" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1572,22 +1569,22 @@
     </row>
     <row r="7" spans="1:16" ht="28.8">
       <c r="A7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1601,22 +1598,22 @@
     </row>
     <row r="8" spans="1:16" ht="28.8">
       <c r="A8" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1627,70 +1624,70 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1706,57 +1703,57 @@
     </row>
     <row r="11" spans="1:16" ht="28.8">
       <c r="A11" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="28.8">
       <c r="A12" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1772,28 +1769,28 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
         <v>222</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1803,28 +1800,28 @@
     </row>
     <row r="14" spans="1:16" ht="28.8">
       <c r="A14" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
       <c r="E14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1832,22 +1829,22 @@
     </row>
     <row r="15" spans="1:16" ht="28.8">
       <c r="A15" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
       <c r="E15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1861,22 +1858,22 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1890,22 +1887,22 @@
     </row>
     <row r="17" spans="1:15" ht="28.8">
       <c r="A17" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1919,22 +1916,22 @@
     </row>
     <row r="18" spans="1:15" ht="28.8">
       <c r="A18" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
       <c r="E18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
@@ -1948,22 +1945,22 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -1977,22 +1974,22 @@
     </row>
     <row r="20" spans="1:15" ht="28.8">
       <c r="A20" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
       <c r="E20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2006,22 +2003,22 @@
     </row>
     <row r="21" spans="1:15" ht="28.8">
       <c r="A21" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2035,22 +2032,22 @@
     </row>
     <row r="22" spans="1:15" ht="28.8">
       <c r="A22" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2064,28 +2061,28 @@
     </row>
     <row r="23" spans="1:15" ht="28.8">
       <c r="A23" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>229</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
         <v>24</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" t="s">
-        <v>230</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" t="s">
-        <v>25</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2093,22 +2090,22 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
       <c r="E24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2122,22 +2119,22 @@
     </row>
     <row r="25" spans="1:15" ht="28.8">
       <c r="A25" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
       <c r="E25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2151,22 +2148,22 @@
     </row>
     <row r="26" spans="1:15" ht="43.2">
       <c r="A26" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2180,22 +2177,22 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2209,22 +2206,22 @@
     </row>
     <row r="28" spans="1:15" ht="28.8">
       <c r="A28" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2233,30 +2230,30 @@
         <v>3</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="28.8">
       <c r="A29" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2265,30 +2262,30 @@
         <v>3</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="43.2">
       <c r="A30" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2299,64 +2296,64 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="57.6">
       <c r="A31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="28.8">
       <c r="A32" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2365,30 +2362,30 @@
         <v>3</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="28.8">
       <c r="A33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2399,30 +2396,30 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2435,22 +2432,22 @@
     </row>
     <row r="35" spans="1:16" ht="43.2">
       <c r="A35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2461,30 +2458,30 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2492,33 +2489,33 @@
       <c r="H36" t="s">
         <v>3</v>
       </c>
-      <c r="I36" t="s">
-        <v>6</v>
+      <c r="I36" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2527,10 +2524,10 @@
         <v>3</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -2538,132 +2535,132 @@
     </row>
     <row r="38" spans="1:16" ht="28.8">
       <c r="A38" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K38" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="L38" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="43.2">
       <c r="A39" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="57.6">
       <c r="A40" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="43.2">
       <c r="A41" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2672,36 +2669,36 @@
         <v>3</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="72">
       <c r="A42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2712,64 +2709,64 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="43.2">
       <c r="A43" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="28.8">
       <c r="A44" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -2778,36 +2775,36 @@
         <v>3</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2816,32 +2813,32 @@
         <v>3</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2850,32 +2847,32 @@
         <v>3</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:16" ht="43.2">
       <c r="A47" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -2886,30 +2883,30 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="28.8">
       <c r="A48" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2918,36 +2915,36 @@
         <v>3</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K48" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L48" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="43.2">
       <c r="A49" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -2956,74 +2953,74 @@
         <v>3</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="43.2">
       <c r="A50" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L50" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="28.8">
       <c r="A51" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3034,30 +3031,30 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="28.8">
       <c r="A52" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3068,30 +3065,30 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8">
       <c r="A53" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3102,30 +3099,30 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="28.8">
       <c r="A54" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3134,36 +3131,36 @@
         <v>3</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3172,70 +3169,70 @@
         <v>3</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L55" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="43.2">
       <c r="A56" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L56" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="57.6">
       <c r="A57" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3244,39 +3241,39 @@
         <v>3</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J57" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O57" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="O57" s="9" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="28.8">
       <c r="A58" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3287,31 +3284,31 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
       <c r="K58" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:15" ht="43.2">
       <c r="A59" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3322,31 +3319,31 @@
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="K59" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="O59" s="8"/>
     </row>
     <row r="60" spans="1:15" ht="28.8">
       <c r="A60" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3360,22 +3357,22 @@
     </row>
     <row r="61" spans="1:15" ht="28.8">
       <c r="A61" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3389,22 +3386,22 @@
     </row>
     <row r="62" spans="1:15" ht="28.8">
       <c r="A62" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3418,22 +3415,22 @@
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3444,31 +3441,31 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O63" s="8"/>
     </row>
     <row r="64" spans="1:15" ht="43.2">
       <c r="A64" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3479,30 +3476,30 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
       <c r="K64" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O64" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
-    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added initial property tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="282">
   <si>
     <t>Field</t>
   </si>
@@ -86,15 +86,6 @@
     <t>Duplicate</t>
   </si>
   <si>
-    <t>An element name must begin with an upper case letter.</t>
-  </si>
-  <si>
-    <t>An attribute name must begin with a lower case letter.</t>
-  </si>
-  <si>
-    <t>A term in a property name that does not exist in the dictionary must be defined as Local Terminology.</t>
-  </si>
-  <si>
     <t>An abstract element should probably not have a data type.</t>
   </si>
   <si>
@@ -113,12 +104,6 @@
     <t>Bad reference</t>
   </si>
   <si>
-    <t>A property's substitution group must exist.</t>
-  </si>
-  <si>
-    <t>A property's substitution group must be valid (element and has a compatible type).</t>
-  </si>
-  <si>
     <t>An abstract property must be an element.</t>
   </si>
   <si>
@@ -182,12 +167,6 @@
     <t>11-45</t>
   </si>
   <si>
-    <t>A property must have a unique name in its namespace.</t>
-  </si>
-  <si>
-    <t>A term in a property definition that does not exist in the dictionary should be defined as "Local Terminology".</t>
-  </si>
-  <si>
     <t>NDR 4.0</t>
   </si>
   <si>
@@ -813,6 +792,84 @@
   </si>
   <si>
     <t>Type PersonType does not have a style.</t>
+  </si>
+  <si>
+    <t>Property definitions should use words and terms that are either defined in the dictionary or as "Local Terminology".</t>
+  </si>
+  <si>
+    <t>Definition 'A FIPS state codes" is valid if the term 'FIPS' is defined as Local Terminology in that namespace.</t>
+  </si>
+  <si>
+    <t>A FIPS state codes" is not recommended if the term 'FIPS' is not defined as Local Terminology in that namespace.</t>
+  </si>
+  <si>
+    <t>Attribute name 'sequenceID' is valid because it begins with a lower case letter.</t>
+  </si>
+  <si>
+    <t>Attribute name 'SequenceID' is not valid because it begins with an upper case letter.</t>
+  </si>
+  <si>
+    <t>10-48</t>
+  </si>
+  <si>
+    <t>Element name 'Person' is valid because it begins with an upper case letter.</t>
+  </si>
+  <si>
+    <t>Element name 'person' is not valid because it begins with a lower case letter.</t>
+  </si>
+  <si>
+    <t>property_name_invalidChar</t>
+  </si>
+  <si>
+    <t>Property substitution groups must be valid (element and has a compatible type).</t>
+  </si>
+  <si>
+    <t>Property substitution groups must exist.</t>
+  </si>
+  <si>
+    <t>Attribute names must begin with a lower case letter.</t>
+  </si>
+  <si>
+    <t>Element names must begin with an upper case letter.</t>
+  </si>
+  <si>
+    <t>Properties must have unique names within their namespaces.</t>
+  </si>
+  <si>
+    <t>Property names must use valid characters.</t>
+  </si>
+  <si>
+    <t>Property names must use terms that either have standard dictionary entries or are custom defined as Local Terminology.</t>
+  </si>
+  <si>
+    <t>Property name 'Person' uses valid characters.</t>
+  </si>
+  <si>
+    <t>Property name 'PersonIsCitizen?' does not use valid characters.</t>
+  </si>
+  <si>
+    <t>property_name_missing</t>
+  </si>
+  <si>
+    <t>property_prefix_unknown</t>
+  </si>
+  <si>
+    <t>Property name 'nc:StateFIPSCode' is valid if the nc namespace defines the meaning of 'FIPS' in its Local Terminology section.</t>
+  </si>
+  <si>
+    <t>Property name 'nc:StateFIPSCode' is not valid if the nc namespace does not define 'FIPS' in its Local Terminology section.</t>
+  </si>
+  <si>
+    <t>Properties must have names.</t>
+  </si>
+  <si>
+    <t>Property namespace prefixes must be defined.</t>
+  </si>
+  <si>
+    <t>property_prefix_missing</t>
+  </si>
+  <si>
+    <t>Properties must have a namespace prefix.</t>
   </si>
 </sst>
 </file>
@@ -921,6 +978,53 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -974,53 +1078,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1035,27 +1092,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O64" totalsRowShown="0">
-  <autoFilter ref="A1:O64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O68" totalsRowShown="0">
+  <autoFilter ref="A1:O68"/>
   <sortState ref="A2:O63">
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="10" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="9"/>
-    <tableColumn id="17" name="Category" dataDxfId="8"/>
+    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="14"/>
+    <tableColumn id="17" name="Category" dataDxfId="13"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="7"/>
+    <tableColumn id="14" name="Scope" dataDxfId="12"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" name="Rules" dataDxfId="5"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" name="Notes" dataDxfId="0"/>
+    <tableColumn id="21" name="Spec" dataDxfId="11"/>
+    <tableColumn id="18" name="Rules" dataDxfId="10"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="7"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="6"/>
+    <tableColumn id="19" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1324,13 +1381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1382,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>5</v>
@@ -1394,34 +1451,34 @@
         <v>12</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" ht="28.8">
       <c r="A2" s="7" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1432,22 +1489,22 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1464,22 +1521,22 @@
     </row>
     <row r="4" spans="1:16" ht="28.8">
       <c r="A4" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1488,78 +1545,78 @@
         <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:16" ht="57.6">
       <c r="A5" s="4" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="28.8">
       <c r="A6" s="7" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1569,22 +1626,22 @@
     </row>
     <row r="7" spans="1:16" ht="28.8">
       <c r="A7" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1598,22 +1655,22 @@
     </row>
     <row r="8" spans="1:16" ht="28.8">
       <c r="A8" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1624,70 +1681,70 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="28.8">
       <c r="A9" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1703,57 +1760,57 @@
     </row>
     <row r="11" spans="1:16" ht="28.8">
       <c r="A11" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="28.8">
       <c r="A12" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1769,28 +1826,28 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="10" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1798,12 +1855,12 @@
       <c r="L13" s="12"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="28.8">
-      <c r="A14" s="7" t="s">
-        <v>182</v>
+    <row r="14" spans="1:16" ht="43.2">
+      <c r="A14" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>17</v>
@@ -1812,27 +1869,33 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="28.8">
       <c r="A15" s="7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
@@ -1841,10 +1904,10 @@
         <v>18</v>
       </c>
       <c r="E15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1858,22 +1921,22 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>266</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
       </c>
       <c r="E16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -1885,12 +1948,12 @@
       <c r="J16" s="3"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" ht="28.8">
-      <c r="A17" s="7" t="s">
-        <v>180</v>
+    <row r="17" spans="1:15" ht="43.2">
+      <c r="A17" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>267</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
@@ -1899,10 +1962,10 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1910,16 +1973,26 @@
       <c r="H17" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" ht="28.8">
-      <c r="A18" s="7" t="s">
-        <v>179</v>
+    <row r="18" spans="1:15" ht="43.2">
+      <c r="A18" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>268</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1928,10 +2001,10 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
@@ -1939,16 +2012,26 @@
       <c r="H18" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="7" t="s">
-        <v>178</v>
+    <row r="19" spans="1:15" ht="28.8">
+      <c r="A19" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>269</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>19</v>
@@ -1957,10 +2040,10 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -1968,16 +2051,18 @@
       <c r="H19" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
       <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" ht="28.8">
-      <c r="A20" s="7" t="s">
-        <v>181</v>
+      <c r="A20" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>270</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
@@ -1986,10 +2071,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -1997,16 +2082,26 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>273</v>
+      </c>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" ht="28.8">
-      <c r="A21" s="7" t="s">
-        <v>191</v>
+    <row r="21" spans="1:15">
+      <c r="A21" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>278</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>17</v>
@@ -2015,10 +2110,10 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2026,16 +2121,18 @@
       <c r="H21" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="28.8">
-      <c r="A22" s="7" t="s">
-        <v>192</v>
+    <row r="22" spans="1:15" ht="57.6">
+      <c r="A22" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>271</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>17</v>
@@ -2044,10 +2141,10 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2055,45 +2152,57 @@
       <c r="H22" t="s">
         <v>3</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="28.8">
-      <c r="A23" s="7" t="s">
-        <v>183</v>
+    <row r="23" spans="1:15">
+      <c r="A23" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>281</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="7" t="s">
-        <v>185</v>
+      <c r="A24" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>279</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>17</v>
@@ -2102,10 +2211,10 @@
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2113,8 +2222,10 @@
       <c r="H24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" ht="28.8">
@@ -2122,7 +2233,7 @@
         <v>184</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
@@ -2131,10 +2242,10 @@
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2146,24 +2257,24 @@
       <c r="J25" s="3"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="43.2">
-      <c r="A26" s="10" t="s">
-        <v>188</v>
+    <row r="26" spans="1:15" ht="28.8">
+      <c r="A26" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>189</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
         <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2175,85 +2286,82 @@
       <c r="J26" s="3"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" ht="28.8">
       <c r="A27" s="7" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" ht="28.8">
+    <row r="28" spans="1:15">
       <c r="A28" s="7" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>133</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
+        <v>222</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="G28" t="s">
         <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15" ht="28.8">
       <c r="A29" s="7" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2261,31 +2369,28 @@
       <c r="H29" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" ht="43.2">
-      <c r="A30" s="4" t="s">
-        <v>124</v>
+      <c r="A30" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>40</v>
+        <v>234</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2293,55 +2398,45 @@
       <c r="H30" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="57.6">
-      <c r="A31" s="4" t="s">
-        <v>126</v>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="O30" s="8"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>167</v>
+        <v>24</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>168</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:15" ht="28.8">
       <c r="A32" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>17</v>
@@ -2350,10 +2445,10 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2362,30 +2457,30 @@
         <v>3</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="28.8">
-      <c r="A33" s="4" t="s">
-        <v>122</v>
+      <c r="A33" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2393,21 +2488,19 @@
       <c r="H33" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="7" t="s">
-        <v>131</v>
+      <c r="I33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="43.2">
+      <c r="A34" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>17</v>
@@ -2416,10 +2509,10 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>242</v>
+        <v>35</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2429,59 +2522,65 @@
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:16" ht="43.2">
+      <c r="K34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="57.6">
       <c r="A35" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B36" t="s">
-        <v>106</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="28.8">
+      <c r="A36" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2490,20 +2589,18 @@
         <v>3</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="1:16">
+        <v>47</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="28.8">
       <c r="A37" s="4" t="s">
-        <v>201</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
@@ -2512,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2523,144 +2620,129 @@
       <c r="H37" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="P37"/>
-    </row>
-    <row r="38" spans="1:16" ht="28.8">
-      <c r="A38" s="4" t="s">
-        <v>202</v>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>158</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:16" ht="43.2">
       <c r="A39" s="4" t="s">
-        <v>203</v>
+        <v>111</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
       <c r="K39" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="57.6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>109</v>
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="43.2">
+        <v>3</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2669,92 +2751,97 @@
         <v>3</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="72">
+        <v>43</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="P41"/>
+    </row>
+    <row r="42" spans="1:16" ht="28.8">
       <c r="A42" s="4" t="s">
-        <v>80</v>
+        <v>195</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
-      </c>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>261</v>
+        <v>21</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L42" s="11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="43.2">
       <c r="A43" s="4" t="s">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>24</v>
-      </c>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="K43" s="2" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="28.8">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="57.6">
       <c r="A44" s="4" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>17</v>
@@ -2763,48 +2850,44 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
       <c r="K44" s="2" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="43.2">
       <c r="A45" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -2813,32 +2896,36 @@
         <v>3</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="1:16">
+        <v>34</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="72">
       <c r="A46" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -2846,67 +2933,67 @@
       <c r="H46" t="s">
         <v>3</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="47" spans="1:16" ht="43.2">
-      <c r="A47" s="7" t="s">
-        <v>71</v>
+      <c r="A47" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="G47" t="s">
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="2" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="28.8">
-      <c r="A48" s="7" t="s">
-        <v>70</v>
+      <c r="A48" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -2915,36 +3002,36 @@
         <v>3</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>151</v>
+        <v>30</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="43.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -2953,62 +3040,54 @@
         <v>3</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="43.2">
+        <v>39</v>
+      </c>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="28.8">
-      <c r="A51" s="4" t="s">
-        <v>76</v>
+        <v>40</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="1:15" ht="43.2">
+      <c r="A51" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
@@ -3017,10 +3096,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3031,18 +3110,18 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="2" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="28.8">
       <c r="A52" s="7" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>6</v>
@@ -3051,10 +3130,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3062,21 +3141,25 @@
       <c r="H52" t="s">
         <v>3</v>
       </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
+      <c r="I52" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="K52" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="28.8">
-      <c r="A53" s="7" t="s">
-        <v>101</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="43.2">
+      <c r="A53" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>6</v>
@@ -3085,10 +3168,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3096,18 +3179,22 @@
       <c r="H53" t="s">
         <v>3</v>
       </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
+      <c r="I53" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K53" s="2" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="28.8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="43.2">
       <c r="A54" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>60</v>
@@ -3119,36 +3206,36 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
+        <v>223</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="G54" t="s">
         <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I54" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="28.8">
+      <c r="A55" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>6</v>
@@ -3157,10 +3244,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3168,71 +3255,67 @@
       <c r="H55" t="s">
         <v>3</v>
       </c>
-      <c r="I55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
       <c r="K55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="28.8">
+      <c r="A56" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L55" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="43.2">
-      <c r="A56" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="B56" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="57.6">
-      <c r="A57" s="4" t="s">
-        <v>103</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="28.8">
+      <c r="A57" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3240,40 +3323,33 @@
       <c r="H57" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>155</v>
-      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
       <c r="K57" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="O57" s="9" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="28.8">
       <c r="A58" s="4" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3281,34 +3357,37 @@
       <c r="H58" t="s">
         <v>3</v>
       </c>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
+      <c r="I58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="K58" s="2" t="s">
-        <v>193</v>
+        <v>85</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="O58" s="8"/>
-    </row>
-    <row r="59" spans="1:15" ht="43.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="4" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3316,22 +3395,25 @@
       <c r="H59" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
+      <c r="I59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="K59" s="2" t="s">
-        <v>195</v>
+        <v>88</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O59" s="8"/>
-    </row>
-    <row r="60" spans="1:15" ht="28.8">
-      <c r="A60" s="7" t="s">
-        <v>120</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="43.2">
+      <c r="A60" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>17</v>
@@ -3340,27 +3422,32 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>34</v>
+        <v>223</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>3</v>
-      </c>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="O60" s="8"/>
-    </row>
-    <row r="61" spans="1:15" ht="28.8">
-      <c r="A61" s="7" t="s">
-        <v>119</v>
+        <v>21</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="57.6">
+      <c r="A61" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>17</v>
@@ -3369,10 +3456,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>223</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3380,28 +3467,40 @@
       <c r="H61" t="s">
         <v>3</v>
       </c>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="O61" s="8"/>
+      <c r="I61" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O61" s="9" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="62" spans="1:15" ht="28.8">
-      <c r="A62" s="7" t="s">
-        <v>121</v>
+      <c r="A62" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>34</v>
+        <v>224</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3409,28 +3508,34 @@
       <c r="H62" t="s">
         <v>3</v>
       </c>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="O62" s="8"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" ht="43.2">
       <c r="A63" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>34</v>
+        <v>224</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3441,19 +3546,19 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>262</v>
+        <v>189</v>
       </c>
       <c r="O63" s="8"/>
     </row>
-    <row r="64" spans="1:15" ht="43.2">
-      <c r="A64" s="4" t="s">
-        <v>116</v>
+    <row r="64" spans="1:15" ht="28.8">
+      <c r="A64" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>17</v>
@@ -3462,10 +3567,10 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3473,33 +3578,155 @@
       <c r="H64" t="s">
         <v>3</v>
       </c>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>198</v>
-      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
       <c r="O64" s="8"/>
     </row>
+    <row r="65" spans="1:15" ht="28.8">
+      <c r="A65" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>3</v>
+      </c>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="O65" s="8"/>
+    </row>
+    <row r="66" spans="1:15" ht="28.8">
+      <c r="A66" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G66" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" t="s">
+        <v>3</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="O66" s="8"/>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="A67" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G67" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="O67" s="8"/>
+    </row>
+    <row r="68" spans="1:15" ht="43.2">
+      <c r="A68" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G68" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" t="s">
+        <v>3</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O68" s="8"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
-    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
+  <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M65:O1048576 P38:P1048576 P4:P36">
-    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
+  <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Refactored unit and field tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -978,53 +978,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1078,6 +1031,53 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1098,21 +1098,21 @@
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="15" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="14"/>
-    <tableColumn id="17" name="Category" dataDxfId="13"/>
+    <tableColumn id="1" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" name="Category" dataDxfId="8"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="12"/>
+    <tableColumn id="14" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" name="Source"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="11"/>
-    <tableColumn id="18" name="Rules" dataDxfId="10"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="7"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="6"/>
-    <tableColumn id="19" name="Notes" dataDxfId="5"/>
+    <tableColumn id="21" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" name="Rules" dataDxfId="5"/>
+    <tableColumn id="4" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1384,10 +1384,10 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3712,21 +3712,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
-    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added issue exception handling
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cdmgtri\niem-model-qa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A955846E-AD16-40A8-BC92-7E6B78811A64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="284">
   <si>
     <t>Field</t>
   </si>
@@ -870,12 +871,18 @@
   </si>
   <si>
     <t>Properties must have a namespace prefix.</t>
+  </si>
+  <si>
+    <t>nc:CodeType</t>
+  </si>
+  <si>
+    <t>biom:Type2CrossReferenceListType, j:PersonBloodTypeCodeSimpleType, j:PersonBloodTypeCodeType, jp3-52:AirspaceCoordinatingMeasureTypeAndUsageType, jp3-52:AirspaceCoordinatingMeasureTypeCodeSimpleType, jp3-52:AirspaceCoordinatingMeasureTypeCodeType, mo:UnitTypeCodeTextSimpleType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -978,6 +985,53 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1031,53 +1085,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1092,27 +1099,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O68" totalsRowShown="0">
-  <autoFilter ref="A1:O68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O68" totalsRowShown="0">
+  <autoFilter ref="A1:O68" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:O63">
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="10" dataCellStyle="Good"/>
-    <tableColumn id="10" name="Description" dataDxfId="9"/>
-    <tableColumn id="17" name="Category" dataDxfId="8"/>
-    <tableColumn id="2" name="Component"/>
-    <tableColumn id="3" name="Field"/>
-    <tableColumn id="14" name="Scope" dataDxfId="7"/>
-    <tableColumn id="11" name="Source"/>
-    <tableColumn id="9" name="Severity"/>
-    <tableColumn id="21" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" name="Rules" dataDxfId="5"/>
-    <tableColumn id="4" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="15" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rules" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1380,31 +1387,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30" style="7" customWidth="1"/>
-    <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
-    <col min="8" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="6" customWidth="1"/>
-    <col min="11" max="12" width="34.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="26.77734375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="27.21875" style="9" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1"/>
-    <col min="17" max="17" width="31.5546875" customWidth="1"/>
+    <col min="4" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
+    <col min="11" max="12" width="34.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="26.7109375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1455,7 +1461,7 @@
       </c>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16" ht="28.8">
+    <row r="2" spans="1:16" ht="30">
       <c r="A2" s="7" t="s">
         <v>207</v>
       </c>
@@ -1487,7 +1493,7 @@
       <c r="O2" s="8"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" ht="30">
       <c r="A3" s="7" t="s">
         <v>209</v>
       </c>
@@ -1519,7 +1525,7 @@
       <c r="O3" s="8"/>
       <c r="P3"/>
     </row>
-    <row r="4" spans="1:16" ht="28.8">
+    <row r="4" spans="1:16" ht="30">
       <c r="A4" s="4" t="s">
         <v>198</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="57.6">
+    <row r="5" spans="1:16" ht="60">
       <c r="A5" s="4" t="s">
         <v>199</v>
       </c>
@@ -1593,7 +1599,7 @@
       </c>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="28.8">
+    <row r="6" spans="1:16" ht="30">
       <c r="A6" s="7" t="s">
         <v>212</v>
       </c>
@@ -1624,7 +1630,7 @@
       <c r="L6" s="12"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="28.8">
+    <row r="7" spans="1:16" ht="30">
       <c r="A7" s="4" t="s">
         <v>170</v>
       </c>
@@ -1653,7 +1659,7 @@
       <c r="J7" s="5"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="28.8">
+    <row r="8" spans="1:16" ht="30">
       <c r="A8" s="4" t="s">
         <v>168</v>
       </c>
@@ -1688,7 +1694,7 @@
       </c>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:16" ht="28.8">
+    <row r="9" spans="1:16" ht="30">
       <c r="A9" s="4" t="s">
         <v>243</v>
       </c>
@@ -1758,7 +1764,7 @@
       <c r="L10" s="5"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="28.8">
+    <row r="11" spans="1:16" ht="30">
       <c r="A11" s="4" t="s">
         <v>251</v>
       </c>
@@ -1793,7 +1799,7 @@
       </c>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:16" ht="28.8">
+    <row r="12" spans="1:16" ht="30">
       <c r="A12" s="4" t="s">
         <v>169</v>
       </c>
@@ -1824,7 +1830,7 @@
       <c r="L12" s="5"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" ht="30">
       <c r="A13" s="10" t="s">
         <v>214</v>
       </c>
@@ -1855,7 +1861,7 @@
       <c r="L13" s="12"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="43.2">
+    <row r="14" spans="1:16" ht="60">
       <c r="A14" s="4" t="s">
         <v>175</v>
       </c>
@@ -1890,7 +1896,7 @@
       </c>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="28.8">
+    <row r="15" spans="1:16" ht="30">
       <c r="A15" s="7" t="s">
         <v>183</v>
       </c>
@@ -1948,7 +1954,7 @@
       <c r="J16" s="3"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" ht="43.2">
+    <row r="17" spans="1:15" ht="45">
       <c r="A17" s="4" t="s">
         <v>173</v>
       </c>
@@ -1987,7 +1993,7 @@
       </c>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" ht="43.2">
+    <row r="18" spans="1:15" ht="45">
       <c r="A18" s="4" t="s">
         <v>172</v>
       </c>
@@ -2026,7 +2032,7 @@
       </c>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="28.8">
+    <row r="19" spans="1:15" ht="30">
       <c r="A19" s="4" t="s">
         <v>171</v>
       </c>
@@ -2057,7 +2063,7 @@
       <c r="L19" s="5"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="28.8">
+    <row r="20" spans="1:15" ht="30">
       <c r="A20" s="4" t="s">
         <v>264</v>
       </c>
@@ -2127,7 +2133,7 @@
       <c r="L21" s="5"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="57.6">
+    <row r="22" spans="1:15" ht="60">
       <c r="A22" s="4" t="s">
         <v>174</v>
       </c>
@@ -2228,7 +2234,7 @@
       <c r="L24" s="5"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="28.8">
+    <row r="25" spans="1:15" ht="30">
       <c r="A25" s="7" t="s">
         <v>184</v>
       </c>
@@ -2257,7 +2263,7 @@
       <c r="J25" s="3"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="28.8">
+    <row r="26" spans="1:15" ht="30">
       <c r="A26" s="7" t="s">
         <v>185</v>
       </c>
@@ -2286,7 +2292,7 @@
       <c r="J26" s="3"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" ht="28.8">
+    <row r="27" spans="1:15" ht="30">
       <c r="A27" s="7" t="s">
         <v>176</v>
       </c>
@@ -2344,7 +2350,7 @@
       <c r="J28" s="3"/>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" ht="28.8">
+    <row r="29" spans="1:15" ht="30">
       <c r="A29" s="7" t="s">
         <v>177</v>
       </c>
@@ -2373,7 +2379,7 @@
       <c r="J29" s="3"/>
       <c r="O29" s="8"/>
     </row>
-    <row r="30" spans="1:15" ht="43.2">
+    <row r="30" spans="1:15" ht="45">
       <c r="A30" s="10" t="s">
         <v>181</v>
       </c>
@@ -2431,7 +2437,7 @@
       <c r="J31" s="3"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" ht="28.8">
+    <row r="32" spans="1:15" ht="30">
       <c r="A32" s="7" t="s">
         <v>122</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="28.8">
+    <row r="33" spans="1:16" ht="30">
       <c r="A33" s="7" t="s">
         <v>121</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="43.2">
+    <row r="34" spans="1:16" ht="60">
       <c r="A34" s="4" t="s">
         <v>117</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="57.6">
+    <row r="35" spans="1:16" ht="60">
       <c r="A35" s="4" t="s">
         <v>119</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="28.8">
+    <row r="36" spans="1:16" ht="30">
       <c r="A36" s="7" t="s">
         <v>123</v>
       </c>
@@ -2595,7 +2601,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="28.8">
+    <row r="37" spans="1:16" ht="45">
       <c r="A37" s="4" t="s">
         <v>115</v>
       </c>
@@ -2657,7 +2663,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:16" ht="43.2">
+    <row r="39" spans="1:16" ht="45">
       <c r="A39" s="4" t="s">
         <v>111</v>
       </c>
@@ -2691,7 +2697,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" ht="30">
       <c r="A40" s="4" t="s">
         <v>193</v>
       </c>
@@ -2725,7 +2731,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" ht="30">
       <c r="A41" s="4" t="s">
         <v>194</v>
       </c>
@@ -2760,7 +2766,7 @@
       <c r="L41" s="5"/>
       <c r="P41"/>
     </row>
-    <row r="42" spans="1:16" ht="28.8">
+    <row r="42" spans="1:16" ht="30">
       <c r="A42" s="4" t="s">
         <v>195</v>
       </c>
@@ -2798,7 +2804,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="43.2">
+    <row r="43" spans="1:16" ht="45">
       <c r="A43" s="4" t="s">
         <v>196</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="57.6">
+    <row r="44" spans="1:16" ht="60">
       <c r="A44" s="4" t="s">
         <v>197</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="43.2">
+    <row r="45" spans="1:16" ht="45">
       <c r="A45" s="4" t="s">
         <v>74</v>
       </c>
@@ -2908,7 +2914,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="72">
+    <row r="46" spans="1:16" ht="75">
       <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
@@ -2942,7 +2948,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="43.2">
+    <row r="47" spans="1:16" ht="45">
       <c r="A47" s="4" t="s">
         <v>72</v>
       </c>
@@ -2975,8 +2981,11 @@
       <c r="L47" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" ht="28.8">
+      <c r="N47" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="30">
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" ht="30">
       <c r="A49" s="4" t="s">
         <v>66</v>
       </c>
@@ -3082,7 +3091,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:15" ht="43.2">
+    <row r="51" spans="1:15" ht="45">
       <c r="A51" s="7" t="s">
         <v>64</v>
       </c>
@@ -3116,7 +3125,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="28.8">
+    <row r="52" spans="1:15" ht="45">
       <c r="A52" s="7" t="s">
         <v>63</v>
       </c>
@@ -3154,7 +3163,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="43.2">
+    <row r="53" spans="1:15" ht="60">
       <c r="A53" s="4" t="s">
         <v>70</v>
       </c>
@@ -3192,7 +3201,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="43.2">
+    <row r="54" spans="1:15" ht="60">
       <c r="A54" s="4" t="s">
         <v>71</v>
       </c>
@@ -3229,8 +3238,11 @@
       <c r="L54" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" ht="28.8">
+      <c r="N54" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="30">
       <c r="A55" s="4" t="s">
         <v>69</v>
       </c>
@@ -3264,7 +3276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="28.8">
+    <row r="56" spans="1:15" ht="45">
       <c r="A56" s="7" t="s">
         <v>95</v>
       </c>
@@ -3298,7 +3310,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="28.8">
+    <row r="57" spans="1:15" ht="30">
       <c r="A57" s="7" t="s">
         <v>94</v>
       </c>
@@ -3332,7 +3344,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="28.8">
+    <row r="58" spans="1:15" ht="30">
       <c r="A58" s="4" t="s">
         <v>68</v>
       </c>
@@ -3370,7 +3382,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" ht="30">
       <c r="A59" s="4" t="s">
         <v>90</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="43.2">
+    <row r="60" spans="1:15" ht="45">
       <c r="A60" s="4" t="s">
         <v>75</v>
       </c>
@@ -3441,8 +3453,11 @@
       <c r="L60" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" ht="57.6">
+      <c r="N60" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="60">
       <c r="A61" s="4" t="s">
         <v>96</v>
       </c>
@@ -3483,7 +3498,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="28.8">
+    <row r="62" spans="1:15" ht="30">
       <c r="A62" s="4" t="s">
         <v>165</v>
       </c>
@@ -3518,7 +3533,7 @@
       </c>
       <c r="O62" s="8"/>
     </row>
-    <row r="63" spans="1:15" ht="43.2">
+    <row r="63" spans="1:15" ht="45">
       <c r="A63" s="4" t="s">
         <v>110</v>
       </c>
@@ -3553,7 +3568,7 @@
       </c>
       <c r="O63" s="8"/>
     </row>
-    <row r="64" spans="1:15" ht="28.8">
+    <row r="64" spans="1:15" ht="30">
       <c r="A64" s="7" t="s">
         <v>113</v>
       </c>
@@ -3582,7 +3597,7 @@
       <c r="J64" s="3"/>
       <c r="O64" s="8"/>
     </row>
-    <row r="65" spans="1:15" ht="28.8">
+    <row r="65" spans="1:15" ht="30">
       <c r="A65" s="7" t="s">
         <v>112</v>
       </c>
@@ -3611,7 +3626,7 @@
       <c r="J65" s="3"/>
       <c r="O65" s="8"/>
     </row>
-    <row r="66" spans="1:15" ht="28.8">
+    <row r="66" spans="1:15" ht="30">
       <c r="A66" s="7" t="s">
         <v>114</v>
       </c>
@@ -3640,7 +3655,7 @@
       <c r="J66" s="3"/>
       <c r="O66" s="8"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" ht="30">
       <c r="A67" s="4" t="s">
         <v>108</v>
       </c>
@@ -3675,7 +3690,7 @@
       </c>
       <c r="O67" s="8"/>
     </row>
-    <row r="68" spans="1:15" ht="43.2">
+    <row r="68" spans="1:15" ht="45">
       <c r="A68" s="4" t="s">
         <v>109</v>
       </c>
@@ -3711,22 +3726,23 @@
       <c r="O68" s="8"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
-    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="51" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="52" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="53" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="54" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M69:O1048576 P42:P1048576 P4:P40">
-    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates to spellcheck to handle special terms in names
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE3174B-8713-42CB-8FCE-6B90D4403169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5FCEA2-610E-4654-8BDF-7E7B3E1D9AB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="291">
   <si>
     <t>Field</t>
   </si>
@@ -904,7 +904,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,15 +931,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,11 +950,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -972,12 +960,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1016,13 +1003,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -1438,7 +1421,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3805,7 +3788,7 @@
       <c r="O69" s="8"/>
     </row>
     <row r="70" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="4" t="s">
         <v>288</v>
       </c>
       <c r="B70" s="2" t="s">

</xml_diff>

<commit_message>
Added check for non-breaking spaces to formatting tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2770F0D9-B40D-46BD-8D6B-7AB370CCB9E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F5851A-1A20-4E8F-AC55-ABC61464E1B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,12 +660,6 @@
     <t>facet_definition_formatting</t>
   </si>
   <si>
-    <t>Facet values should not contain leading or trailing spaces.</t>
-  </si>
-  <si>
-    <t>facet_value_spaces</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -919,6 +913,12 @@
   </si>
   <si>
     <t>Namespace definitions should have consistent formatting.</t>
+  </si>
+  <si>
+    <t>facet_value_formatting</t>
+  </si>
+  <si>
+    <t>Facet values should not contain leading or trailing spaces, multiple consecutive spaces, or non-breaking spaces.</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1634,10 @@
         <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1666,10 +1666,10 @@
         <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1698,10 +1698,10 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1716,10 +1716,10 @@
         <v>36</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O4" s="8"/>
     </row>
@@ -1737,10 +1737,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1751,10 +1751,10 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O5" s="8"/>
     </row>
@@ -1772,10 +1772,10 @@
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1803,10 +1803,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1832,10 +1832,10 @@
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1846,16 +1846,16 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>202</v>
@@ -1867,10 +1867,10 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1885,10 +1885,10 @@
         <v>40</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O9" s="8"/>
     </row>
@@ -1897,7 +1897,7 @@
         <v>165</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -1906,10 +1906,10 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="11" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>203</v>
@@ -1937,10 +1937,10 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1951,13 +1951,13 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -1975,10 +1975,10 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1992,12 +1992,12 @@
       <c r="L12" s="5"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>212</v>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>296</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
@@ -2006,10 +2006,10 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -2025,22 +2025,22 @@
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
@@ -2056,22 +2056,22 @@
     </row>
     <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
         <v>287</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>289</v>
-      </c>
       <c r="E15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -2087,10 +2087,10 @@
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -2099,10 +2099,10 @@
         <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -2121,7 +2121,7 @@
         <v>173</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
@@ -2130,10 +2130,10 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -2144,10 +2144,10 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O17" s="8"/>
     </row>
@@ -2156,7 +2156,7 @@
         <v>181</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -2165,10 +2165,10 @@
         <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
@@ -2185,7 +2185,7 @@
         <v>178</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -2194,10 +2194,10 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -2214,7 +2214,7 @@
         <v>171</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
@@ -2223,10 +2223,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2238,13 +2238,13 @@
         <v>46</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O20" s="8"/>
     </row>
@@ -2253,7 +2253,7 @@
         <v>170</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>17</v>
@@ -2262,10 +2262,10 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2280,10 +2280,10 @@
         <v>33</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O21" s="8"/>
     </row>
@@ -2292,7 +2292,7 @@
         <v>169</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
@@ -2301,10 +2301,10 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2320,10 +2320,10 @@
     </row>
     <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -2332,10 +2332,10 @@
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -2350,19 +2350,19 @@
         <v>29</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>17</v>
@@ -2371,10 +2371,10 @@
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2393,7 +2393,7 @@
         <v>172</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
@@ -2402,10 +2402,10 @@
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2420,19 +2420,19 @@
         <v>146</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
@@ -2441,10 +2441,10 @@
         <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2455,19 +2455,19 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>16</v>
@@ -2476,10 +2476,10 @@
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2495,10 +2495,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
@@ -2507,10 +2507,10 @@
         <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2538,10 +2538,10 @@
         <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2567,10 +2567,10 @@
         <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2596,10 +2596,10 @@
         <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -2625,10 +2625,10 @@
         <v>18</v>
       </c>
       <c r="E32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2654,10 +2654,10 @@
         <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2683,10 +2683,10 @@
         <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2712,10 +2712,10 @@
         <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2741,10 +2741,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2773,10 +2773,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>34</v>
@@ -2839,10 +2839,10 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -2873,10 +2873,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2896,7 +2896,7 @@
         <v>114</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>16</v>
@@ -2905,10 +2905,10 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2939,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2967,10 +2967,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -2989,10 +2989,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>17</v>
@@ -3001,10 +3001,10 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -3032,10 +3032,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -3067,10 +3067,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3101,10 +3101,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -3139,10 +3139,10 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3177,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3211,10 +3211,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3249,10 +3249,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3266,7 +3266,7 @@
         <v>135</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -3283,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3303,7 +3303,7 @@
         <v>78</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3320,10 +3320,10 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3358,10 +3358,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3392,10 +3392,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3426,10 +3426,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3460,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3498,10 +3498,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3536,10 +3536,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3560,7 +3560,7 @@
         <v>83</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3577,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3611,10 +3611,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3645,10 +3645,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3679,10 +3679,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3717,10 +3717,10 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3755,10 +3755,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
@@ -3775,7 +3775,7 @@
         <v>137</v>
       </c>
       <c r="N65" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -3792,10 +3792,10 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
@@ -3833,10 +3833,10 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
@@ -3868,10 +3868,10 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G68" t="s">
         <v>4</v>
@@ -3903,10 +3903,10 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -3932,10 +3932,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
@@ -3961,10 +3961,10 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
@@ -3990,10 +3990,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4007,7 +4007,7 @@
         <v>188</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O72" s="8"/>
     </row>
@@ -4025,10 +4025,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Dictionary and test updates
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED3CB7-8FA9-445B-B374-D035E3D3AC64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE294B5-183F-4308-8B10-625503676A6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="304">
   <si>
     <t>Field</t>
   </si>
@@ -934,6 +934,10 @@
   </si>
   <si>
     <t>Sample facets from certain types with known special characters should be tested to confirm special characters have been correctly encoded.</t>
+  </si>
+  <si>
+    <t>Move to NIEM Releases-specific tests.  Doesn't apply to user input.
+Sample facets from certain types with known special characters should be tested to confirm special characters have been correctly encoded.</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1017,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1055,9 +1059,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1065,6 +1066,62 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1206,62 +1263,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1282,21 +1283,21 @@
     <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rules" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rules" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1733,12 +1734,12 @@
       <c r="L4" s="11"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>299</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>17</v>
@@ -4102,59 +4103,59 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="P47:P1048576 P45 M75:O1048576 M16:O16 P16:P43 P4:P14">
-    <cfRule type="cellIs" dxfId="14" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="61" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="62" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="63" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="64" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P47:P1048576 P45 M75:O1048576 M16:O16 P16:P43 P4:P14">
-    <cfRule type="cellIs" dxfId="10" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated spreadsheet column headers
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE294B5-183F-4308-8B10-625503676A6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1133AE-B076-49D0-9748-8EE2718138FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="303">
   <si>
     <t>Field</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Spec</t>
   </si>
   <si>
-    <t>Rules</t>
-  </si>
-  <si>
     <t>Missing value</t>
   </si>
   <si>
@@ -931,13 +928,13 @@
   </si>
   <si>
     <t>Code facet 'CIV' in genc:CountryAlpha3CodeSimpleType should have correctly-encoded definition 'CÔTE D’IVOIRE'.</t>
-  </si>
-  <si>
-    <t>Sample facets from certain types with known special characters should be tested to confirm special characters have been correctly encoded.</t>
   </si>
   <si>
     <t>Move to NIEM Releases-specific tests.  Doesn't apply to user input.
 Sample facets from certain types with known special characters should be tested to confirm special characters have been correctly encoded.</t>
+  </si>
+  <si>
+    <t>Rule</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1289,7 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rules" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
@@ -1569,10 +1566,10 @@
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,13 +1617,13 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>5</v>
@@ -1635,34 +1632,34 @@
         <v>12</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P1"/>
     </row>
     <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1673,25 +1670,25 @@
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -1705,28 +1702,28 @@
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1736,25 +1733,25 @@
     </row>
     <row r="5" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H5" t="s">
         <v>3</v>
@@ -1762,105 +1759,105 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="K6" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1874,22 +1871,22 @@
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1900,70 +1897,70 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1979,60 +1976,60 @@
     </row>
     <row r="12" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="G12" t="s">
         <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="N12" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -2048,28 +2045,28 @@
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="G14" t="s">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -2079,28 +2076,28 @@
     </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2110,28 +2107,28 @@
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
         <v>286</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>287</v>
-      </c>
       <c r="E16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -2141,28 +2138,28 @@
     </row>
     <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
       <c r="E17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2172,57 +2169,57 @@
     </row>
     <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
       <c r="E18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
       <c r="E19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
@@ -2236,22 +2233,22 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2265,22 +2262,22 @@
     </row>
     <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
       <c r="E21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2289,37 +2286,37 @@
         <v>3</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K21" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
       <c r="E22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2328,37 +2325,37 @@
         <v>3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K22" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -2374,22 +2371,22 @@
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
       <c r="E24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2398,37 +2395,37 @@
         <v>3</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K24" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="L24" s="11" t="s">
         <v>268</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>269</v>
       </c>
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
         <v>17</v>
       </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
       <c r="E25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2444,22 +2441,22 @@
     </row>
     <row r="26" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
         <v>17</v>
       </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
       <c r="E26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2468,72 +2465,72 @@
         <v>3</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K26" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" t="s">
-        <v>219</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="G27" t="s">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="L27" s="12" t="s">
         <v>283</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>284</v>
       </c>
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2549,22 +2546,22 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
         <v>17</v>
       </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
       <c r="E29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2580,22 +2577,22 @@
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
         <v>17</v>
       </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
       <c r="E30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2609,22 +2606,22 @@
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="D31" t="s">
-        <v>18</v>
-      </c>
       <c r="E31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -2638,28 +2635,28 @@
     </row>
     <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
         <v>20</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" t="s">
-        <v>218</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" t="s">
-        <v>21</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -2667,22 +2664,22 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
         <v>17</v>
       </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
       <c r="E33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2696,22 +2693,22 @@
     </row>
     <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
         <v>17</v>
       </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
       <c r="E34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2725,22 +2722,22 @@
     </row>
     <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2754,22 +2751,22 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2783,22 +2780,22 @@
     </row>
     <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2807,30 +2804,30 @@
         <v>3</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -2839,30 +2836,30 @@
         <v>3</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -2873,64 +2870,64 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L39" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2939,30 +2936,30 @@
         <v>3</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2973,30 +2970,30 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
       <c r="K42" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="L42" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -3009,22 +3006,22 @@
     </row>
     <row r="44" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -3035,36 +3032,36 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L44" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -3074,22 +3071,22 @@
     </row>
     <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3098,10 +3095,10 @@
         <v>3</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -3109,22 +3106,22 @@
     </row>
     <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -3133,142 +3130,142 @@
         <v>3</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K48" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="L48" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K49" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L49" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="L50" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3277,36 +3274,36 @@
         <v>3</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="L51" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3317,67 +3314,67 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L53" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L53" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="N53" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3386,36 +3383,36 @@
         <v>3</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L54" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3424,32 +3421,32 @@
         <v>3</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3458,20 +3455,20 @@
         <v>3</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>6</v>
@@ -3480,10 +3477,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3494,18 +3491,18 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L57" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>6</v>
@@ -3514,10 +3511,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3526,24 +3523,24 @@
         <v>3</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K58" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L58" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
@@ -3552,10 +3549,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3564,24 +3561,24 @@
         <v>3</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K59" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L59" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
@@ -3590,39 +3587,39 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K60" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L60" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L60" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="N60" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
@@ -3631,10 +3628,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3645,18 +3642,18 @@
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L61" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="L61" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
@@ -3665,10 +3662,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3679,18 +3676,18 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L62" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>6</v>
@@ -3699,10 +3696,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3713,18 +3710,18 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>6</v>
@@ -3733,10 +3730,10 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3745,24 +3742,24 @@
         <v>3</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>6</v>
@@ -3771,10 +3768,10 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
@@ -3783,73 +3780,73 @@
         <v>3</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K65" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L65" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="L65" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="L66" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L66" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="N66" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
@@ -3858,39 +3855,39 @@
         <v>3</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J67" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="O67" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L67" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="O67" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C68" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G68" t="s">
         <v>4</v>
@@ -3901,31 +3898,31 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L68" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="O68" s="8"/>
     </row>
     <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -3936,31 +3933,31 @@
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
       <c r="K69" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="L69" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="O69" s="8"/>
     </row>
     <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
@@ -3974,22 +3971,22 @@
     </row>
     <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
@@ -4003,22 +4000,22 @@
     </row>
     <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4032,22 +4029,22 @@
     </row>
     <row r="73" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>
@@ -4058,31 +4055,31 @@
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O73" s="8"/>
     </row>
     <row r="74" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G74" t="s">
         <v>4</v>
@@ -4093,10 +4090,10 @@
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
       <c r="K74" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O74" s="8"/>
     </row>

</xml_diff>

<commit_message>
Removed 5.0 check for special character encoding
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1133AE-B076-49D0-9748-8EE2718138FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8BAE9-583A-4D74-AE23-26F7EA6D4FD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="299">
   <si>
     <t>Field</t>
   </si>
@@ -919,19 +919,6 @@
   </si>
   <si>
     <t>db</t>
-  </si>
-  <si>
-    <t>facet_definition_formatting_specialChars</t>
-  </si>
-  <si>
-    <t>Code facet 'CIV' in genc:CountryAlpha3CodeSimpleType should not have incorrectly-encoded definition 'CÃ”TE Dâ€™IVOIRE'.</t>
-  </si>
-  <si>
-    <t>Code facet 'CIV' in genc:CountryAlpha3CodeSimpleType should have correctly-encoded definition 'CÔTE D’IVOIRE'.</t>
-  </si>
-  <si>
-    <t>Move to NIEM Releases-specific tests.  Doesn't apply to user input.
-Sample facets from certain types with known special characters should be tested to confirm special characters have been correctly encoded.</t>
   </si>
   <si>
     <t>Rule</t>
@@ -1063,62 +1050,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1260,6 +1191,62 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1274,27 +1261,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O74" totalsRowShown="0">
-  <autoFilter ref="A1:O74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:O69">
-    <sortCondition ref="A1:A69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O73" totalsRowShown="0">
+  <autoFilter ref="A1:O73" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:O68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="22"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1563,13 +1550,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1604,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>89</v>
@@ -1731,15 +1718,15 @@
       <c r="L4" s="11"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>298</v>
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>301</v>
+        <v>197</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -1751,27 +1738,31 @@
         <v>231</v>
       </c>
       <c r="G5" t="s">
-        <v>297</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="K5" s="11" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>299</v>
+        <v>244</v>
       </c>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1783,69 +1774,59 @@
         <v>212</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>243</v>
+        <v>36</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>244</v>
       </c>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1854,7 +1835,7 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>211</v>
@@ -1867,14 +1848,20 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
+      <c r="K8" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1886,7 +1873,7 @@
         <v>218</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1894,22 +1881,26 @@
       <c r="H9" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="I9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="K9" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>238</v>
+        <v>164</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1921,7 +1912,7 @@
         <v>218</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1929,26 +1920,18 @@
       <c r="H10" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>164</v>
+        <v>246</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -1957,7 +1940,7 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>211</v>
@@ -1966,23 +1949,30 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>288</v>
+      </c>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -1997,30 +1987,23 @@
         <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>288</v>
-      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>166</v>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>295</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>296</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -2035,29 +2018,29 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>286</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>211</v>
@@ -2074,12 +2057,12 @@
       <c r="L14" s="11"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>293</v>
+    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -2099,24 +2082,24 @@
       <c r="H15" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>284</v>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>289</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>286</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>212</v>
@@ -2130,18 +2113,18 @@
       <c r="H16" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>289</v>
+    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>290</v>
+        <v>251</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -2163,16 +2146,20 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="K17" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>172</v>
+    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -2181,36 +2168,30 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>253</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -2231,24 +2212,24 @@
       <c r="J19" s="3"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>177</v>
+    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2256,16 +2237,26 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -2277,7 +2268,7 @@
         <v>218</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2289,25 +2280,25 @@
         <v>45</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2316,7 +2307,7 @@
         <v>218</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -2324,29 +2315,21 @@
       <c r="H22" t="s">
         <v>3</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>258</v>
-      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>259</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -2363,18 +2346,26 @@
       <c r="H23" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="I23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>268</v>
+      </c>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -2394,26 +2385,18 @@
       <c r="H24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>268</v>
-      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>16</v>
@@ -2433,18 +2416,26 @@
       <c r="H25" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="I25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -2456,72 +2447,64 @@
         <v>218</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>211</v>
+        <v>280</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>272</v>
+        <v>20</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>280</v>
+        <v>211</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>283</v>
-      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -2544,12 +2527,12 @@
       <c r="L28" s="5"/>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>270</v>
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>274</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -2558,10 +2541,10 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -2569,18 +2552,16 @@
       <c r="H29" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>16</v>
@@ -2592,7 +2573,7 @@
         <v>215</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2606,10 +2587,10 @@
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>16</v>
@@ -2618,27 +2599,27 @@
         <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>16</v>
@@ -2650,24 +2631,24 @@
         <v>217</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="O32" s="8"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
@@ -2679,7 +2660,7 @@
         <v>217</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2691,15 +2672,15 @@
       <c r="J33" s="3"/>
       <c r="O33" s="8"/>
     </row>
-    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>174</v>
+    <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
@@ -2708,7 +2689,7 @@
         <v>217</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -2720,15 +2701,15 @@
       <c r="J34" s="3"/>
       <c r="O34" s="8"/>
     </row>
-    <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>178</v>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -2737,7 +2718,7 @@
         <v>217</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2749,24 +2730,24 @@
       <c r="J35" s="3"/>
       <c r="O35" s="8"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>176</v>
+        <v>119</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2774,16 +2755,19 @@
       <c r="H36" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="O36" s="8"/>
+      <c r="I36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
@@ -2795,7 +2779,7 @@
         <v>214</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2807,15 +2791,15 @@
         <v>45</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>118</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>16</v>
@@ -2827,7 +2811,7 @@
         <v>214</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -2835,19 +2819,21 @@
       <c r="H38" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>143</v>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>16</v>
@@ -2859,29 +2845,29 @@
         <v>214</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>33</v>
+        <v>233</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>116</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>16</v>
@@ -2893,32 +2879,30 @@
         <v>214</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
-      </c>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>120</v>
+        <v>3</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
@@ -2927,7 +2911,7 @@
         <v>214</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2935,22 +2919,24 @@
       <c r="H41" t="s">
         <v>3</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>113</v>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>287</v>
+        <v>125</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -2959,7 +2945,7 @@
         <v>214</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -2969,22 +2955,16 @@
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>121</v>
+    </row>
+    <row r="43" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -2993,7 +2973,7 @@
         <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -3003,22 +2983,28 @@
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>109</v>
+      <c r="K43" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>117</v>
+        <v>292</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>211</v>
@@ -3027,26 +3013,23 @@
         <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>292</v>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="O44" s="8"/>
+    </row>
+    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
@@ -3055,26 +3038,30 @@
         <v>212</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>20</v>
-      </c>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="O45" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="P45"/>
     </row>
     <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B46" t="s">
-        <v>97</v>
+        <v>191</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>15</v>
@@ -3086,7 +3073,7 @@
         <v>212</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3097,22 +3084,21 @@
       <c r="I46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J46" s="6" t="s">
-        <v>42</v>
+      <c r="J46" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="P46"/>
     </row>
     <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
@@ -3121,29 +3107,33 @@
         <v>212</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-    </row>
-    <row r="48" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>27</v>
@@ -3155,7 +3145,7 @@
         <v>212</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3167,24 +3157,24 @@
         <v>45</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K48" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -3193,7 +3183,7 @@
         <v>212</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3201,25 +3191,21 @@
       <c r="H49" t="s">
         <v>20</v>
       </c>
-      <c r="I49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
       <c r="K49" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
@@ -3228,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>211</v>
@@ -3237,26 +3223,30 @@
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="K50" s="3" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
@@ -3273,28 +3263,24 @@
       <c r="H51" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
       <c r="K51" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
@@ -3303,29 +3289,32 @@
         <v>218</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
       </c>
       <c r="H52" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="3" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>16</v>
@@ -3337,35 +3326,36 @@
         <v>218</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
-      </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="K53" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="N53" s="8" t="s">
-        <v>277</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -3374,7 +3364,7 @@
         <v>218</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3386,21 +3376,17 @@
         <v>45</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>15</v>
@@ -3412,7 +3398,7 @@
         <v>218</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3424,20 +3410,20 @@
         <v>45</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>63</v>
+    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
@@ -3446,7 +3432,7 @@
         <v>218</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3454,21 +3440,21 @@
       <c r="H56" t="s">
         <v>3</v>
       </c>
-      <c r="I56" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>6</v>
@@ -3480,7 +3466,7 @@
         <v>218</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3488,21 +3474,25 @@
       <c r="H57" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
+      <c r="I57" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="K57" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>61</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>6</v>
@@ -3514,7 +3504,7 @@
         <v>218</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -3526,21 +3516,21 @@
         <v>45</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
@@ -3552,33 +3542,36 @@
         <v>218</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="N59" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
@@ -3590,36 +3583,29 @@
         <v>218</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
       <c r="K60" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N60" s="8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>67</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
@@ -3631,7 +3617,7 @@
         <v>218</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3642,18 +3628,18 @@
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="3" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
@@ -3665,7 +3651,7 @@
         <v>218</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3676,18 +3662,18 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>92</v>
+      <c r="A63" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>6</v>
@@ -3699,7 +3685,7 @@
         <v>218</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -3707,21 +3693,25 @@
       <c r="H63" t="s">
         <v>3</v>
       </c>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
+      <c r="I63" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="K63" s="3" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>6</v>
@@ -3733,7 +3723,7 @@
         <v>218</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
@@ -3745,24 +3735,24 @@
         <v>45</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -3777,27 +3767,26 @@
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>3</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
       <c r="K65" s="3" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>16</v>
@@ -3815,35 +3804,39 @@
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
-      </c>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="K66" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="N66" s="8" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>211</v>
@@ -3854,31 +3847,25 @@
       <c r="H67" t="s">
         <v>3</v>
       </c>
-      <c r="I67" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
       <c r="K67" s="3" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="O67" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="O67" s="8"/>
+    </row>
+    <row r="68" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
@@ -3898,19 +3885,19 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="O68" s="8"/>
     </row>
-    <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>108</v>
+    <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>16</v>
@@ -3919,10 +3906,10 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -3930,22 +3917,16 @@
       <c r="H69" t="s">
         <v>3</v>
       </c>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
       <c r="O69" s="8"/>
     </row>
     <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>16</v>
@@ -3957,7 +3938,7 @@
         <v>215</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
@@ -3971,10 +3952,10 @@
     </row>
     <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>16</v>
@@ -3986,7 +3967,7 @@
         <v>215</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
@@ -3999,14 +3980,14 @@
       <c r="O71" s="8"/>
     </row>
     <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>112</v>
+      <c r="A72" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
@@ -4015,7 +3996,7 @@
         <v>215</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4023,19 +4004,25 @@
       <c r="H72" t="s">
         <v>3</v>
       </c>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="O72" s="8"/>
     </row>
-    <row r="73" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
@@ -4055,104 +4042,69 @@
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>250</v>
+        <v>188</v>
       </c>
       <c r="O73" s="8"/>
-    </row>
-    <row r="74" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1</v>
-      </c>
-      <c r="E74" t="s">
-        <v>215</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G74" t="s">
-        <v>4</v>
-      </c>
-      <c r="H74" t="s">
-        <v>3</v>
-      </c>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="O74" s="8"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P47:P1048576 P45 M75:O1048576 M16:O16 P16:P43 P4:P14">
-    <cfRule type="cellIs" dxfId="25" priority="61" operator="equal">
+  <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
+    <cfRule type="cellIs" dxfId="14" priority="61" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="62" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="63" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="64" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P47:P1048576 P45 M75:O1048576 M16:O16 P16:P43 P4:P14">
-    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+  <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
+    <cfRule type="cellIs" dxfId="10" priority="36" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P44">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+  <conditionalFormatting sqref="P43">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P44">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+  <conditionalFormatting sqref="P43">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P15">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+  <conditionalFormatting sqref="P14">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P15">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="P14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated test exception handling
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8BAE9-583A-4D74-AE23-26F7EA6D4FD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC33011-3DD4-4583-A07B-C78335864E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="300">
   <si>
     <t>Field</t>
   </si>
@@ -922,6 +922,9 @@
   </si>
   <si>
     <t>Rule</t>
+  </si>
+  <si>
+    <t>nc:CodeType, stat:CodeType</t>
   </si>
 </sst>
 </file>
@@ -1050,6 +1053,62 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1191,62 +1250,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1267,21 +1270,21 @@
     <sortCondition ref="A1:A68"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1553,10 +1556,10 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,7 +3566,7 @@
         <v>82</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4052,59 +4055,59 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
-    <cfRule type="cellIs" dxfId="14" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="61" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="62" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="63" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="64" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
-    <cfRule type="cellIs" dxfId="10" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added test exceptions and added definition to error report for facets with duplicate codes
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC33011-3DD4-4583-A07B-C78335864E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A0B66A-D63D-4D84-BF10-3B022961783F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -861,9 +861,6 @@
     <t>nc:CodeType</t>
   </si>
   <si>
-    <t>biom:Type2CrossReferenceListType, j:PersonBloodTypeCodeSimpleType, j:PersonBloodTypeCodeType, jp3-52:AirspaceCoordinatingMeasureTypeAndUsageType, jp3-52:AirspaceCoordinatingMeasureTypeCodeSimpleType, jp3-52:AirspaceCoordinatingMeasureTypeCodeType, mo:UnitTypeCodeTextSimpleType</t>
-  </si>
-  <si>
     <t>property_name_repTerm_aug</t>
   </si>
   <si>
@@ -891,9 +888,6 @@
     <t>Types that represent a value (simple content) must declare a base type.  Note: Simple union types have member types instead of a base type.</t>
   </si>
   <si>
-    <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, ncic:VMOCodeSimpleType</t>
-  </si>
-  <si>
     <t>property_definition_formatting</t>
   </si>
   <si>
@@ -925,6 +919,12 @@
   </si>
   <si>
     <t>nc:CodeType, stat:CodeType</t>
+  </si>
+  <si>
+    <t>biom:Type2CrossReferenceListType, j:PersonBloodTypeCodeSimpleType, j:PersonBloodTypeCodeType, jp3-52:AirspaceCoordinatingMeasureTypeAndUsageType, jp3-52:AirspaceCoordinatingMeasureTypeCodeSimpleType, jp3-52:AirspaceCoordinatingMeasureTypeCodeType, mo:UnitTypeCodeTextSimpleType, mo:UnitTypeCodeTextType</t>
+  </si>
+  <si>
+    <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType</t>
   </si>
 </sst>
 </file>
@@ -1556,10 +1556,10 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N60" sqref="N60"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1573,8 @@
     <col min="8" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
     <col min="11" max="12" width="34.7109375" style="3" customWidth="1"/>
-    <col min="13" max="14" width="26.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="41.85546875" style="8" customWidth="1"/>
     <col min="15" max="15" width="27.28515625" style="9" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" style="1"/>
   </cols>
@@ -1607,7 +1608,7 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>89</v>
@@ -1678,7 +1679,7 @@
         <v>211</v>
       </c>
       <c r="G3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -1929,7 +1930,7 @@
       <c r="L10" s="5"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>246</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>248</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -1990,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -2000,10 +2001,10 @@
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
@@ -2031,16 +2032,16 @@
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E14" t="s">
         <v>212</v>
@@ -2062,16 +2063,16 @@
     </row>
     <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
         <v>285</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>286</v>
       </c>
       <c r="E15" t="s">
         <v>212</v>
@@ -2093,10 +2094,10 @@
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2435,10 +2436,10 @@
     </row>
     <row r="26" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -2450,7 +2451,7 @@
         <v>218</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
@@ -2461,10 +2462,10 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L26" s="12" t="s">
         <v>282</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>283</v>
       </c>
       <c r="O26" s="8"/>
     </row>
@@ -2902,7 +2903,7 @@
         <v>113</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>15</v>
@@ -2995,10 +2996,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>16</v>
@@ -3513,7 +3514,7 @@
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>45</v>
@@ -3566,7 +3567,7 @@
         <v>82</v>
       </c>
       <c r="N59" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -3781,7 +3782,7 @@
         <v>136</v>
       </c>
       <c r="N65" s="8" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added augmentation and role tests
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A0B66A-D63D-4D84-BF10-3B022961783F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7458D4-2660-4153-AABD-40E97D4474BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="321">
   <si>
     <t>Field</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Type names should not use the term "Type" in the name other than as the final representation term.</t>
   </si>
   <si>
-    <t>type_name_repTerm_aug</t>
-  </si>
-  <si>
     <t>type_name_repTerm_assn</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>type_base_unknown</t>
   </si>
   <si>
-    <t>type_style_aug</t>
-  </si>
-  <si>
     <t>type_style_assn</t>
   </si>
   <si>
@@ -381,9 +375,6 @@
     <t>Types must have bases that are defined.</t>
   </si>
   <si>
-    <t>type_base_aug</t>
-  </si>
-  <si>
     <t>type_base_assn</t>
   </si>
   <si>
@@ -858,12 +849,6 @@
     <t>Properties must have a namespace prefix.</t>
   </si>
   <si>
-    <t>nc:CodeType</t>
-  </si>
-  <si>
-    <t>property_name_repTerm_aug</t>
-  </si>
-  <si>
     <t>augmentation points</t>
   </si>
   <si>
@@ -925,13 +910,91 @@
   </si>
   <si>
     <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType</t>
+  </si>
+  <si>
+    <t>type_base_invalid_role</t>
+  </si>
+  <si>
+    <t>Object types that contain RoleOf elements should extend structures:ObjectType.</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>Type j:VictimType can contain nc:RoleOfPerson and extend structures:ObjectType</t>
+  </si>
+  <si>
+    <t>Type j:VictimType should not both contain nc:RoleOfPerson and extend nc:PersonType</t>
+  </si>
+  <si>
+    <t>property_name_augmentation</t>
+  </si>
+  <si>
+    <t>Augmentation element names should correspond to the name of the augmentation point element for which they substitute.</t>
+  </si>
+  <si>
+    <t>augmentations</t>
+  </si>
+  <si>
+    <t>Element name 'PersonAugmentation' is valid for an augmentation that substitutes for nc:PersonAugmentationPoint.</t>
+  </si>
+  <si>
+    <t>Element name 'ManagerAugmentation' is not valid for an augmentation that substitutes for nc:PersonAugmentationPoint.</t>
+  </si>
+  <si>
+    <t>property_name_repTerm_augmentation</t>
+  </si>
+  <si>
+    <t>type_base_augmentation</t>
+  </si>
+  <si>
+    <t>type_name_repTerm_augmentation</t>
+  </si>
+  <si>
+    <t>type_style_augmentation</t>
+  </si>
+  <si>
+    <t>property_definition_augmentation</t>
+  </si>
+  <si>
+    <t>property_definition_augmentationPoint</t>
+  </si>
+  <si>
+    <t>Augmentation definitions should follow a consistent pattern.</t>
+  </si>
+  <si>
+    <t>Augmentation point definitions should follow a consistent pattern.</t>
+  </si>
+  <si>
+    <t>hs:ActivityPersonAssociationAugmentation</t>
+  </si>
+  <si>
+    <t>Definitions 'Additional information about a person' and 'Additional information about nc:PersonType' are valid for em:PersonAugmentation.</t>
+  </si>
+  <si>
+    <t>Definitions 'Additional information about a location' and 'Additional information about nc:OrganizationType' are not valid for em:PersonAugmentation.</t>
+  </si>
+  <si>
+    <t>Definitions 'An augmentation point for PersonType' and a'An augmentation point for nc:PersonType' are valid for nc:PersonAugmentationPoint</t>
+  </si>
+  <si>
+    <t>type_definition_augmentation</t>
+  </si>
+  <si>
+    <t>Augmentation types should follow a consistent pattern</t>
+  </si>
+  <si>
+    <t>Definitions 'A data type for additional information about a location' and 'A data type for additional information about nc:OrganizationType' are not valid for em:PersonAugmentationType.</t>
+  </si>
+  <si>
+    <t>Definitions 'A data type for additional information about a person' and 'A data type for additional information about nc:PersonType' are valid for em:PersonAugmentationType.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,8 +1028,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -989,6 +1059,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -999,12 +1074,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1046,69 +1122,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1250,6 +1274,62 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1264,27 +1344,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O73" totalsRowShown="0">
-  <autoFilter ref="A1:O73" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:O68">
-    <sortCondition ref="A1:A68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O78" totalsRowShown="0">
+  <autoFilter ref="A1:O78" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:O73">
+    <sortCondition ref="A1:A73"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="22"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1553,13 +1633,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,13 +1688,13 @@
         <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>5</v>
@@ -1629,10 +1709,10 @@
     </row>
     <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -1641,10 +1721,10 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -1660,11 +1740,11 @@
       <c r="P2"/>
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>206</v>
+      <c r="A3" s="15" t="s">
+        <v>203</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -1673,13 +1753,13 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G3" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -1692,11 +1772,11 @@
       <c r="P3"/>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>209</v>
+      <c r="A4" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -1705,10 +1785,10 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -1724,10 +1804,10 @@
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1736,10 +1816,10 @@
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1754,19 +1834,19 @@
         <v>35</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1775,10 +1855,10 @@
         <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1789,19 +1869,19 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -1810,10 +1890,10 @@
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -1827,10 +1907,10 @@
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1839,10 +1919,10 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1853,19 +1933,19 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1874,10 +1954,10 @@
         <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1892,19 +1972,19 @@
         <v>39</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1913,10 +1993,10 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>
@@ -1932,10 +2012,10 @@
     </row>
     <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -1944,10 +2024,10 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -1958,22 +2038,22 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
@@ -1982,10 +2062,10 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -2000,11 +2080,11 @@
       <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>293</v>
+      <c r="A13" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
@@ -2013,10 +2093,10 @@
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -2031,23 +2111,23 @@
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>291</v>
+      <c r="A14" s="15" t="s">
+        <v>286</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E14" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G14" t="s">
         <v>4</v>
@@ -2063,22 +2143,22 @@
     </row>
     <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -2092,12 +2172,12 @@
       <c r="L15" s="11"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>287</v>
+    <row r="16" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2106,10 +2186,10 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>211</v>
+        <v>302</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -2117,18 +2197,25 @@
       <c r="H16" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>313</v>
+      </c>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>172</v>
+        <v>310</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -2137,10 +2224,10 @@
         <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>211</v>
+        <v>274</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -2148,22 +2235,20 @@
       <c r="H17" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="L17" s="11"/>
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>180</v>
+      <c r="A18" s="14" t="s">
+        <v>282</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -2172,56 +2257,64 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G18" t="s">
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>177</v>
+    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>250</v>
+      </c>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>170</v>
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>16</v>
@@ -2230,10 +2323,10 @@
         <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G20" t="s">
         <v>4</v>
@@ -2241,38 +2334,28 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>255</v>
-      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>169</v>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2280,57 +2363,51 @@
       <c r="H21" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>258</v>
-      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>300</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>211</v>
+        <v>302</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>304</v>
+      </c>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -2339,10 +2416,10 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -2354,22 +2431,22 @@
         <v>45</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>268</v>
+        <v>253</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>269</v>
+        <v>166</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -2378,10 +2455,10 @@
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2389,30 +2466,38 @@
       <c r="H24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="I24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -2420,26 +2505,18 @@
       <c r="H25" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>272</v>
-      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -2448,45 +2525,49 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>279</v>
+        <v>208</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>282</v>
+        <v>3</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G27" t="s">
         <v>4</v>
@@ -2500,12 +2581,12 @@
       <c r="L27" s="5"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>270</v>
+        <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>16</v>
@@ -2514,10 +2595,10 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2525,18 +2606,26 @@
       <c r="H28" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="I28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>269</v>
+      </c>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>181</v>
+    <row r="29" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>275</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -2548,36 +2637,42 @@
         <v>215</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="O29" s="8"/>
     </row>
-    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>182</v>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>273</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2585,16 +2680,18 @@
       <c r="H30" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
       <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>173</v>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>16</v>
@@ -2603,27 +2700,29 @@
         <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>16</v>
@@ -2632,10 +2731,10 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
@@ -2647,12 +2746,12 @@
       <c r="J32" s="3"/>
       <c r="O32" s="8"/>
     </row>
-    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
@@ -2661,10 +2760,10 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -2676,53 +2775,53 @@
       <c r="J33" s="3"/>
       <c r="O33" s="8"/>
     </row>
-    <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>178</v>
+    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>179</v>
+        <v>19</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="O34" s="8"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G35" t="s">
         <v>4</v>
@@ -2734,24 +2833,24 @@
       <c r="J35" s="3"/>
       <c r="O35" s="8"/>
     </row>
-    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E36" t="s">
         <v>214</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
@@ -2759,31 +2858,28 @@
       <c r="H36" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>118</v>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="O36" s="8"/>
+    </row>
+    <row r="37" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>214</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
@@ -2791,31 +2887,28 @@
       <c r="H37" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>114</v>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="O37" s="8"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
         <v>214</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="G38" t="s">
         <v>4</v>
@@ -2823,21 +2916,16 @@
       <c r="H38" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="O38" s="8"/>
+    </row>
+    <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>16</v>
@@ -2846,32 +2934,30 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>120</v>
+        <v>306</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>16</v>
@@ -2880,10 +2966,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -2895,27 +2981,27 @@
         <v>45</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -2926,18 +3012,18 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
       <c r="K41" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L41" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L41" s="3" t="s">
+    </row>
+    <row r="42" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>16</v>
@@ -2946,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>230</v>
@@ -2955,51 +3041,58 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="K42" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>109</v>
+        <v>295</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>117</v>
+        <v>296</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>289</v>
+      <c r="K43" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="O43" s="8"/>
+    </row>
+    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>290</v>
+        <v>121</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>16</v>
@@ -3008,29 +3101,30 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
-      </c>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="O44" s="8"/>
-    </row>
-    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
+        <v>111</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>15</v>
@@ -3039,10 +3133,10 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -3050,34 +3144,33 @@
       <c r="H45" t="s">
         <v>3</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="P45"/>
-    </row>
-    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>191</v>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3085,71 +3178,61 @@
       <c r="H46" t="s">
         <v>3</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>193</v>
+        <v>3</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>317</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>99</v>
+        <v>318</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3157,25 +3240,22 @@
       <c r="H48" t="s">
         <v>20</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>194</v>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="O48" s="8"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>284</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>100</v>
+        <v>285</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>16</v>
@@ -3184,10 +3264,10 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3197,31 +3277,28 @@
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="O49" s="8"/>
+    </row>
+    <row r="50" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>74</v>
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3232,34 +3309,31 @@
       <c r="I50" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J50" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="J50" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>71</v>
+        <v>188</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3267,33 +3341,33 @@
       <c r="H51" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="I51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>70</v>
+        <v>189</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3301,108 +3375,109 @@
       <c r="H52" t="s">
         <v>20</v>
       </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="N52" s="8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="I52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K52" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>64</v>
+        <v>191</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3414,29 +3489,33 @@
         <v>45</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-    </row>
-    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>62</v>
+        <v>32</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -3447,147 +3526,139 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>61</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
       </c>
       <c r="H57" t="s">
-        <v>3</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
       <c r="K57" s="3" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="N57" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N59" s="8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3595,21 +3666,21 @@
       <c r="H60" t="s">
         <v>3</v>
       </c>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="I60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
@@ -3618,10 +3689,10 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3632,18 +3703,18 @@
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>92</v>
+        <v>307</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
@@ -3652,10 +3723,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3663,21 +3734,25 @@
       <c r="H62" t="s">
         <v>3</v>
       </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
+      <c r="I62" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="K62" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>6</v>
@@ -3686,36 +3761,36 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>6</v>
@@ -3724,85 +3799,85 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="N64" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="3" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="N65" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
@@ -3810,40 +3885,33 @@
       <c r="H66" t="s">
         <v>3</v>
       </c>
-      <c r="I66" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
       <c r="K66" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="O66" s="9" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>162</v>
+      <c r="A67" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>163</v>
+        <v>56</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
@@ -3854,31 +3922,30 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="3" t="s">
-        <v>183</v>
+        <v>128</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="O67" s="8"/>
-    </row>
-    <row r="68" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G68" t="s">
         <v>4</v>
@@ -3886,25 +3953,28 @@
       <c r="H68" t="s">
         <v>3</v>
       </c>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
+      <c r="I68" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="K68" s="3" t="s">
-        <v>185</v>
+        <v>82</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="O68" s="8"/>
+        <v>84</v>
+      </c>
     </row>
     <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>111</v>
+      <c r="A69" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
@@ -3913,7 +3983,7 @@
         <v>215</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -3921,16 +3991,25 @@
       <c r="H69" t="s">
         <v>3</v>
       </c>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="O69" s="8"/>
-    </row>
-    <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>110</v>
+      <c r="I69" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>16</v>
@@ -3942,24 +4021,32 @@
         <v>215</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>3</v>
-      </c>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="O70" s="8"/>
-    </row>
-    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>112</v>
+        <v>20</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="N70" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>16</v>
@@ -3971,7 +4058,7 @@
         <v>215</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
@@ -3979,16 +4066,28 @@
       <c r="H71" t="s">
         <v>3</v>
       </c>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="O71" s="8"/>
+      <c r="I71" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="O71" s="9" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>15</v>
@@ -3997,10 +4096,10 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4011,10 +4110,10 @@
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
       <c r="K72" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>250</v>
+        <v>181</v>
       </c>
       <c r="O72" s="8"/>
     </row>
@@ -4023,7 +4122,7 @@
         <v>107</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>16</v>
@@ -4032,10 +4131,10 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>
@@ -4046,69 +4145,226 @@
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
       <c r="K73" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="O73" s="8"/>
+    </row>
+    <row r="74" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>212</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H74" t="s">
+        <v>3</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="O74" s="8"/>
+    </row>
+    <row r="75" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>212</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G75" t="s">
+        <v>4</v>
+      </c>
+      <c r="H75" t="s">
+        <v>3</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="O75" s="8"/>
+    </row>
+    <row r="76" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>212</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H76" t="s">
+        <v>3</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="O76" s="8"/>
+    </row>
+    <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>212</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G77" t="s">
+        <v>4</v>
+      </c>
+      <c r="H77" t="s">
+        <v>3</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="O77" s="8"/>
+    </row>
+    <row r="78" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>212</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G78" t="s">
+        <v>4</v>
+      </c>
+      <c r="H78" t="s">
+        <v>3</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="O78" s="8"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
-    <cfRule type="cellIs" dxfId="25" priority="61" operator="equal">
+  <conditionalFormatting sqref="P51:P1048576 P49 M79:O1048576 M15:O17 P15:P46 P4:P13">
+    <cfRule type="cellIs" dxfId="14" priority="61" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="62" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="63" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="64" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P46:P1048576 P44 M74:O1048576 M15:O15 P15:P42 P4:P13">
-    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+  <conditionalFormatting sqref="P51:P1048576 P49 M79:O1048576 M15:O17 P15:P46 P4:P13">
+    <cfRule type="cellIs" dxfId="10" priority="36" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P43">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+  <conditionalFormatting sqref="P47:P48">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P43">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+  <conditionalFormatting sqref="P47:P48">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the custom dictionary and added a new test exception
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACD3A89-A9B9-48FE-A50F-0327426AC9DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DF3BC2-EF18-49AA-B6E3-A574DB49AB3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,9 +855,6 @@
     <t>biom:Type2CrossReferenceListType, j:PersonBloodTypeCodeSimpleType, j:PersonBloodTypeCodeType, jp3-52:AirspaceCoordinatingMeasureTypeAndUsageType, jp3-52:AirspaceCoordinatingMeasureTypeCodeSimpleType, jp3-52:AirspaceCoordinatingMeasureTypeCodeType, mo:UnitTypeCodeTextSimpleType, mo:UnitTypeCodeTextType</t>
   </si>
   <si>
-    <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType</t>
-  </si>
-  <si>
     <t>Object types that contain RoleOf elements should extend structures:ObjectType.</t>
   </si>
   <si>
@@ -1042,6 +1039,9 @@
   </si>
   <si>
     <t>type_base_simpleContent</t>
+  </si>
+  <si>
+    <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType, can:StreetDirectionCodeSimpleType</t>
   </si>
 </sst>
 </file>
@@ -1144,6 +1144,62 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1444,62 +1500,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1520,21 +1520,21 @@
     <sortCondition ref="A1:A82"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="42" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="36" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="35" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="33"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1809,7 +1809,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,7 +1914,7 @@
         <v>197</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -1942,10 +1942,10 @@
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -1970,7 +1970,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="N4" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O4" s="8"/>
     </row>
@@ -2182,7 +2182,7 @@
       <c r="L10" s="5"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>226</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>228</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -2284,13 +2284,13 @@
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E14" t="s">
         <v>200</v>
@@ -2312,16 +2312,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" t="s">
         <v>331</v>
-      </c>
-      <c r="E15" t="s">
-        <v>332</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>199</v>
@@ -2340,16 +2340,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
+        <v>330</v>
+      </c>
+      <c r="E16" t="s">
         <v>331</v>
-      </c>
-      <c r="E16" t="s">
-        <v>332</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>199</v>
@@ -2368,16 +2368,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
         <v>330</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>331</v>
-      </c>
       <c r="E17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>199</v>
@@ -2396,16 +2396,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>199</v>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="21" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -2501,7 +2501,7 @@
         <v>200</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
@@ -2512,22 +2512,22 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="L21" s="10" t="s">
-        <v>296</v>
-      </c>
       <c r="N21" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
@@ -2550,7 +2550,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L22" s="10"/>
       <c r="O22" s="8"/>
@@ -2623,10 +2623,10 @@
     </row>
     <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>16</v>
@@ -2648,7 +2648,7 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="N25" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O25" s="8"/>
     </row>
@@ -2712,10 +2712,10 @@
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>16</v>
@@ -2727,7 +2727,7 @@
         <v>206</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -2738,13 +2738,13 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="L28" s="10" t="s">
-        <v>285</v>
-      </c>
       <c r="N28" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O28" s="8"/>
     </row>
@@ -2929,10 +2929,10 @@
     </row>
     <row r="34" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="36" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>258</v>
@@ -3111,7 +3111,7 @@
         <v>203</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -3140,7 +3140,7 @@
         <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -3169,7 +3169,7 @@
         <v>205</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -3256,7 +3256,7 @@
         <v>205</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>114</v>
@@ -3314,7 +3314,7 @@
         <v>202</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>113</v>
@@ -3346,7 +3346,7 @@
         <v>202</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="48" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>109</v>
@@ -3412,7 +3412,7 @@
         <v>202</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3429,10 +3429,10 @@
     </row>
     <row r="50" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
@@ -3444,7 +3444,7 @@
         <v>202</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3455,16 +3455,16 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="L50" s="10" t="s">
         <v>279</v>
-      </c>
-      <c r="L50" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="O50" s="8"/>
     </row>
     <row r="51" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>148</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="52" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>264</v>
@@ -3547,7 +3547,7 @@
         <v>202</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
@@ -3594,10 +3594,10 @@
     </row>
     <row r="55" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>16</v>
@@ -3609,7 +3609,7 @@
         <v>200</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3620,13 +3620,13 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="N55" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="L55" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="O55" s="8"/>
     </row>
@@ -3843,10 +3843,10 @@
     </row>
     <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>16</v>
@@ -3868,7 +3868,7 @@
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
       <c r="N62" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O62" s="8"/>
     </row>
@@ -4089,10 +4089,10 @@
     </row>
     <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>18</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="70" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>55</v>
@@ -4135,7 +4135,7 @@
         <v>206</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
@@ -4154,7 +4154,7 @@
     </row>
     <row r="71" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>54</v>
@@ -4169,7 +4169,7 @@
         <v>206</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
@@ -4320,7 +4320,7 @@
         <v>206</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G75" t="s">
         <v>4</v>
@@ -4354,7 +4354,7 @@
         <v>206</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G76" t="s">
         <v>4</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="83" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>102</v>
@@ -4612,7 +4612,7 @@
         <v>203</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G83" t="s">
         <v>4</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>101</v>
@@ -4641,7 +4641,7 @@
         <v>203</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G84" t="s">
         <v>4</v>
@@ -4670,7 +4670,7 @@
         <v>203</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G85" t="s">
         <v>4</v>
@@ -4755,126 +4755,126 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="P58:P61 P56 M88:O1048576 M20:O22 P70:P1048576 P63:P68 P3 P5:P18 P20:P53">
-    <cfRule type="cellIs" dxfId="31" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="78" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="79" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="80" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="81" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P58:P61 P56 M88:O1048576 M20:O22 P70:P1048576 P63:P68 P3 P5:P18 P20:P53">
-    <cfRule type="cellIs" dxfId="27" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="53" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54:P55">
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54:P55">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="27" priority="17">
       <formula>$A56&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="26" priority="16">
       <formula>$A55&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P69">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P69">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P62">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P62">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added definition check for representation pattern properties
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5FCB62-B984-4B47-8AD3-3802A7B62412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE902689-0A8A-485E-810F-7394A887D6CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="349">
   <si>
     <t>Field</t>
   </si>
@@ -1063,13 +1063,22 @@
   </si>
   <si>
     <t>subProperty_propertyQName_representation</t>
+  </si>
+  <si>
+    <t>property_definition_representation</t>
+  </si>
+  <si>
+    <t>Representation pattern definitions should follow a consistent pattern.</t>
+  </si>
+  <si>
+    <t>representations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,15 +1099,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1116,11 +1118,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1131,12 +1128,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1172,16 +1168,68 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1482,62 +1530,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1552,27 +1544,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O88" totalsRowShown="0">
-  <autoFilter ref="A1:O88" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:O83">
-    <sortCondition ref="A1:A83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O89" totalsRowShown="0">
+  <autoFilter ref="A1:O89" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:O84">
+    <sortCondition ref="A1:A84"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="42" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="36" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="35" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="33"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1841,13 +1833,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1848,7 @@
     <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
     <col min="4" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
@@ -2624,12 +2616,12 @@
       <c r="L23" s="10"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>163</v>
+        <v>346</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>231</v>
+        <v>347</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -2641,7 +2633,7 @@
         <v>200</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>199</v>
+        <v>348</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2651,20 +2643,16 @@
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>233</v>
-      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>310</v>
+        <v>163</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>308</v>
+        <v>231</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>16</v>
@@ -2672,6 +2660,9 @@
       <c r="D25" t="s">
         <v>17</v>
       </c>
+      <c r="E25" t="s">
+        <v>200</v>
+      </c>
       <c r="F25" s="2" t="s">
         <v>199</v>
       </c>
@@ -2679,23 +2670,24 @@
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="N25" s="8" t="s">
-        <v>339</v>
+        <v>20</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>171</v>
+    <row r="26" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>240</v>
+        <v>308</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -2703,31 +2695,33 @@
       <c r="D26" t="s">
         <v>17</v>
       </c>
-      <c r="E26" t="s">
-        <v>201</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G26" t="s">
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="N26" s="8" t="s">
+        <v>339</v>
+      </c>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -2748,50 +2742,41 @@
       <c r="J27" s="3"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>280</v>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>282</v>
+        <v>208</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>302</v>
-      </c>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>242</v>
+        <v>281</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -2803,34 +2788,33 @@
         <v>206</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>235</v>
+        <v>20</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>302</v>
       </c>
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>16</v>
@@ -2842,7 +2826,7 @@
         <v>206</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G30" t="s">
         <v>4</v>
@@ -2854,25 +2838,25 @@
         <v>45</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>32</v>
+        <v>236</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -2881,7 +2865,7 @@
         <v>206</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -2889,21 +2873,29 @@
       <c r="H31" t="s">
         <v>3</v>
       </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="I31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -2920,26 +2912,18 @@
       <c r="H32" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>248</v>
-      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
       <c r="O32" s="8"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
@@ -2959,21 +2943,29 @@
       <c r="H33" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="I33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="L33" s="10" t="s">
+        <v>248</v>
+      </c>
       <c r="O33" s="8"/>
     </row>
-    <row r="34" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>303</v>
+        <v>249</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
@@ -2988,23 +2980,23 @@
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
       <c r="O34" s="8"/>
     </row>
-    <row r="35" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>162</v>
+        <v>303</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>246</v>
+        <v>305</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
@@ -3019,28 +3011,20 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>252</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
       <c r="O35" s="8"/>
     </row>
-    <row r="36" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>285</v>
+        <v>162</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>16</v>
@@ -3052,64 +3036,72 @@
         <v>206</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>260</v>
+        <v>3</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="O36" s="8"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
       <c r="G37" t="s">
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="K37" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="O37" s="8"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -3133,11 +3125,11 @@
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>172</v>
+      <c r="A39" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>16</v>
@@ -3146,10 +3138,10 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>316</v>
+        <v>199</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -3157,16 +3149,18 @@
       <c r="H39" t="s">
         <v>3</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
       <c r="O39" s="8"/>
     </row>
-    <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>16</v>
@@ -3178,7 +3172,7 @@
         <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -3192,10 +3186,10 @@
     </row>
     <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>16</v>
@@ -3204,27 +3198,27 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="O41" s="8"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>16</v>
@@ -3236,24 +3230,24 @@
         <v>205</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>209</v>
+        <v>316</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="O42" s="8"/>
     </row>
-    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>165</v>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>16</v>
@@ -3265,7 +3259,7 @@
         <v>205</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -3277,15 +3271,15 @@
       <c r="J43" s="3"/>
       <c r="O43" s="8"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>170</v>
+        <v>21</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -3294,7 +3288,7 @@
         <v>205</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>315</v>
+        <v>208</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -3307,14 +3301,14 @@
       <c r="O44" s="8"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>167</v>
+      <c r="A45" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -3323,7 +3317,7 @@
         <v>205</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>199</v>
+        <v>315</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -3335,24 +3329,24 @@
       <c r="J45" s="3"/>
       <c r="O45" s="8"/>
     </row>
-    <row r="46" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>345</v>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>340</v>
+        <v>23</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>341</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>342</v>
+        <v>205</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>277</v>
+        <v>199</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3362,52 +3356,49 @@
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="10" t="s">
+      <c r="O46" s="8"/>
+    </row>
+    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>341</v>
+      </c>
+      <c r="E47" t="s">
+        <v>342</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>3</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="L46" s="10" t="s">
+      <c r="L47" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="O46" s="8"/>
-    </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>202</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G47" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" t="s">
-        <v>3</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="O47" s="8"/>
     </row>
     <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>16</v>
@@ -3419,7 +3410,7 @@
         <v>202</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3431,15 +3422,15 @@
         <v>45</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>16</v>
@@ -3451,7 +3442,7 @@
         <v>202</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>33</v>
+        <v>282</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3459,21 +3450,19 @@
       <c r="H49" t="s">
         <v>3</v>
       </c>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>111</v>
+        <v>334</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
@@ -3485,7 +3474,7 @@
         <v>202</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>317</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3493,19 +3482,21 @@
       <c r="H50" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>336</v>
+        <v>111</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>276</v>
+        <v>115</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>16</v>
@@ -3517,30 +3508,27 @@
         <v>202</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
       </c>
       <c r="H51" t="s">
-        <v>20</v>
-      </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="L51" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="O51" s="8"/>
-    </row>
-    <row r="52" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>148</v>
+        <v>276</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>16</v>
@@ -3552,7 +3540,7 @@
         <v>202</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3562,22 +3550,23 @@
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
-      <c r="K52" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="K52" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="O52" s="8"/>
+    </row>
+    <row r="53" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>264</v>
+        <v>148</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
@@ -3586,32 +3575,32 @@
         <v>202</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>112</v>
+        <v>337</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>116</v>
+        <v>264</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -3620,7 +3609,7 @@
         <v>202</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>318</v>
+        <v>216</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3630,16 +3619,22 @@
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="K54" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
@@ -3648,7 +3643,7 @@
         <v>202</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>199</v>
+        <v>318</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3658,57 +3653,47 @@
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
-      <c r="K55" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>297</v>
+        <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>298</v>
+        <v>110</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>282</v>
+        <v>199</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
-      <c r="K56" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="L56" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="O56" s="8"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K56" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>16</v>
@@ -3720,7 +3705,7 @@
         <v>200</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>199</v>
+        <v>282</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3730,20 +3715,26 @@
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
-      <c r="N57" s="2"/>
+      <c r="K57" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="O57" s="8"/>
     </row>
-    <row r="58" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B58" t="s">
-        <v>95</v>
+        <v>267</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
@@ -3752,30 +3743,27 @@
         <v>200</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>3</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="P58"/>
+        <v>20</v>
+      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>94</v>
+        <v>181</v>
+      </c>
+      <c r="B59" t="s">
+        <v>95</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>15</v>
@@ -3787,7 +3775,7 @@
         <v>200</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3798,21 +3786,22 @@
       <c r="I59" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J59" s="3" t="s">
-        <v>41</v>
+      <c r="J59" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
+      <c r="P59"/>
     </row>
     <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
@@ -3821,33 +3810,29 @@
         <v>200</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>27</v>
@@ -3859,7 +3844,7 @@
         <v>200</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3871,24 +3856,24 @@
         <v>45</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L61" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L61" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
@@ -3897,7 +3882,7 @@
         <v>200</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3905,21 +3890,25 @@
       <c r="H62" t="s">
         <v>20</v>
       </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
+      <c r="I62" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="K62" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>311</v>
+        <v>185</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>312</v>
+        <v>98</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>16</v>
@@ -3927,6 +3916,9 @@
       <c r="D63" t="s">
         <v>1</v>
       </c>
+      <c r="E63" t="s">
+        <v>200</v>
+      </c>
       <c r="F63" s="2" t="s">
         <v>199</v>
       </c>
@@ -3934,23 +3926,23 @@
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>36</v>
-      </c>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="N63" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="O63" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>70</v>
+        <v>311</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>72</v>
+        <v>312</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>16</v>
@@ -3958,9 +3950,6 @@
       <c r="D64" t="s">
         <v>1</v>
       </c>
-      <c r="E64" t="s">
-        <v>206</v>
-      </c>
       <c r="F64" s="2" t="s">
         <v>199</v>
       </c>
@@ -3968,30 +3957,26 @@
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>3</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="N64" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="O64" s="8"/>
+    </row>
+    <row r="65" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -4008,24 +3993,28 @@
       <c r="H65" t="s">
         <v>3</v>
       </c>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
+      <c r="I65" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="K65" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
@@ -4034,32 +4023,29 @@
         <v>206</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
       <c r="K66" s="3" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N66" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>16</v>
@@ -4071,36 +4057,35 @@
         <v>206</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
       </c>
       <c r="H67" t="s">
-        <v>3</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
       <c r="K67" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="N67" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
@@ -4109,7 +4094,7 @@
         <v>206</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G68" t="s">
         <v>4</v>
@@ -4121,17 +4106,21 @@
         <v>45</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>15</v>
@@ -4143,7 +4132,7 @@
         <v>206</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -4155,20 +4144,20 @@
         <v>45</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>304</v>
+        <v>61</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>306</v>
+        <v>47</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
@@ -4177,29 +4166,32 @@
         <v>206</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>36</v>
-      </c>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="O70" s="8"/>
-    </row>
-    <row r="71" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>325</v>
+        <v>3</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>304</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>55</v>
+        <v>306</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
@@ -4208,29 +4200,26 @@
         <v>206</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>314</v>
+        <v>199</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
-      <c r="K71" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>120</v>
-      </c>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="O71" s="8"/>
     </row>
     <row r="72" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>287</v>
+        <v>325</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>6</v>
@@ -4242,7 +4231,7 @@
         <v>206</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4250,25 +4239,21 @@
       <c r="H72" t="s">
         <v>3</v>
       </c>
-      <c r="I72" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
       <c r="K72" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>66</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>6</v>
@@ -4280,33 +4265,33 @@
         <v>206</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>211</v>
+        <v>282</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>
       </c>
       <c r="H73" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>6</v>
@@ -4318,7 +4303,7 @@
         <v>206</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G74" t="s">
         <v>4</v>
@@ -4330,24 +4315,21 @@
         <v>45</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="K74" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L74" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L74" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N74" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>6</v>
@@ -4359,29 +4341,36 @@
         <v>206</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G75" t="s">
         <v>4</v>
       </c>
       <c r="H75" t="s">
-        <v>3</v>
-      </c>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="K75" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="N75" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>6</v>
@@ -4393,7 +4382,7 @@
         <v>206</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>319</v>
+        <v>212</v>
       </c>
       <c r="G76" t="s">
         <v>4</v>
@@ -4404,18 +4393,18 @@
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="3" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>6</v>
@@ -4427,7 +4416,7 @@
         <v>206</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G77" t="s">
         <v>4</v>
@@ -4438,18 +4427,18 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>64</v>
+      <c r="A78" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>6</v>
@@ -4461,7 +4450,7 @@
         <v>206</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="G78" t="s">
         <v>4</v>
@@ -4469,25 +4458,21 @@
       <c r="H78" t="s">
         <v>3</v>
       </c>
-      <c r="I78" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
       <c r="K78" s="3" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>6</v>
@@ -4499,7 +4484,7 @@
         <v>206</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G79" t="s">
         <v>4</v>
@@ -4511,24 +4496,24 @@
         <v>45</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
@@ -4543,26 +4528,27 @@
         <v>4</v>
       </c>
       <c r="H80" t="s">
-        <v>20</v>
-      </c>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="K80" s="3" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="N80" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>16</v>
@@ -4580,39 +4566,35 @@
         <v>4</v>
       </c>
       <c r="H81" t="s">
-        <v>3</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>136</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
       <c r="K81" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="O81" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="N81" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>199</v>
@@ -4623,25 +4605,31 @@
       <c r="H82" t="s">
         <v>3</v>
       </c>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
+      <c r="I82" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="K82" s="3" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="O82" s="8"/>
-    </row>
-    <row r="83" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="O82" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
@@ -4661,19 +4649,19 @@
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
       <c r="K83" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="O83" s="8"/>
     </row>
-    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>324</v>
+    <row r="84" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>16</v>
@@ -4682,10 +4670,10 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>314</v>
+        <v>199</v>
       </c>
       <c r="G84" t="s">
         <v>4</v>
@@ -4693,16 +4681,22 @@
       <c r="H84" t="s">
         <v>3</v>
       </c>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="O84" s="8"/>
     </row>
     <row r="85" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>288</v>
+        <v>324</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>16</v>
@@ -4714,7 +4708,7 @@
         <v>203</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="G85" t="s">
         <v>4</v>
@@ -4728,10 +4722,10 @@
     </row>
     <row r="86" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>16</v>
@@ -4743,7 +4737,7 @@
         <v>203</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="G86" t="s">
         <v>4</v>
@@ -4756,14 +4750,14 @@
       <c r="O86" s="8"/>
     </row>
     <row r="87" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>104</v>
+      <c r="A87" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
@@ -4772,7 +4766,7 @@
         <v>203</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>199</v>
+        <v>317</v>
       </c>
       <c r="G87" t="s">
         <v>4</v>
@@ -4780,25 +4774,19 @@
       <c r="H87" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="5"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="L87" s="3" t="s">
-        <v>230</v>
-      </c>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
       <c r="O87" s="8"/>
     </row>
-    <row r="88" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
@@ -4818,136 +4806,171 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
       <c r="K88" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="O88" s="8"/>
+    </row>
+    <row r="89" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G89" t="s">
+        <v>4</v>
+      </c>
+      <c r="H89" t="s">
+        <v>3</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L88" s="3" t="s">
+      <c r="L89" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="O88" s="8"/>
+      <c r="O89" s="8"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P59:P62 P57 M89:O1048576 M20:O22 P71:P1048576 P64:P69 P3 P5:P18 P20:P54">
-    <cfRule type="cellIs" dxfId="31" priority="78" operator="equal">
+  <conditionalFormatting sqref="P60:P63 P58 M90:O1048576 M20:O22 P72:P1048576 P65:P70 P3 P5:P18 P20:P55">
+    <cfRule type="cellIs" dxfId="42" priority="78" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="79" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="80" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="81" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P59:P62 P57 M89:O1048576 M20:O22 P71:P1048576 P64:P69 P3 P5:P18 P20:P54">
-    <cfRule type="cellIs" dxfId="27" priority="53" operator="equal">
+  <conditionalFormatting sqref="P60:P63 P58 M90:O1048576 M20:O22 P72:P1048576 P65:P70 P3 P5:P18 P20:P55">
+    <cfRule type="cellIs" dxfId="38" priority="53" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P55:P56">
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+  <conditionalFormatting sqref="P56:P57">
+    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P55:P56">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+  <conditionalFormatting sqref="P56:P57">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N58">
+    <cfRule type="expression" dxfId="27" priority="17">
+      <formula>$A58&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="26" priority="16">
       <formula>$A57&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>$A56&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P70">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+  <conditionalFormatting sqref="P71">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P70">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+  <conditionalFormatting sqref="P71">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P63">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+  <conditionalFormatting sqref="P64">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P63">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="P64">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added to dictionary and updated test exception
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE902689-0A8A-485E-810F-7394A887D6CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FFC74-635A-4CEB-8E1B-CFCC2B5B7B66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="349">
   <si>
     <t>Field</t>
   </si>
@@ -1041,9 +1041,6 @@
     <t>type_base_simpleContent</t>
   </si>
   <si>
-    <t>dea:DrugCodeSimpleType, fips:USCountyNumericCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType, can:StreetDirectionCodeSimpleType</t>
-  </si>
-  <si>
     <t>nc:CalendarDate, nc:Chemical, nc:CommercialFacility, nc:Computer, nc:ContactAbstract, nc:CoordinatingAgency, nc:CourtCase, nc:DrugMeasure, nc:ElectronicEquipment, nc:ElectronicInstrument, nc:Email, nc:HazardousMaterial, nc:HazmatAbstract, nc:InjuryTreatment, nc:Kit, nc:Machinery, nc:OdometerReadingMeasure, nc:PersonWorkLocation, nc:ResidentialFacility, nc:RiskReductionFacility, nc:RiskReductionProgram, nc:RoleOfAbstract, nc:ServiceDeliveryNGO, nc:TowingCompany, nc:UTMCoordinateValue, j:AdmittingAgency, j:AmendedSentence, j:Attorney, j:CorrectionalCounselor, j:Corrections, j:Counselor, j:CourtCharge, j:CorrectionsOfficerAppliedForce, j:CorrectionSubjectNotification, j:DetainerNotificationRequest, j:DetainerOrder, j:Detention, j:DetentionFacility, j:DevelopmentDisability, j:DisciplinaryIncident, j:DiversionProgram, j:DriverLicenseConviction, j:Felony, j:FinalPlea, j:Holding, j:Infraction, j:Judgment, j:MentalHealthNotification, j:MentalHealthTreatment, j:Metal, j:Misdemeanor, j:NetworkAddress, j:OfferedPlea, j:Parole, j:PreciousMetal, j:PreviousSentence, j:Probation, j:Project, j:ProsecutionCharge, j:RansomMoneyCode, j:RehabilitationProgram, j:Restitution, j:SearchWarrant, j:SubExhibit, j:SubstanceTest, j:Summons, j:Suspect, j:TaskForce, j:Violation</t>
   </si>
   <si>
@@ -1072,6 +1069,9 @@
   </si>
   <si>
     <t>representations</t>
+  </si>
+  <si>
+    <t>dea:DrugCodeSimpleType, fips:USCounty3DigitCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType, can:StreetDirectionCodeSimpleType</t>
   </si>
 </sst>
 </file>
@@ -1836,10 +1836,10 @@
   <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2246,7 @@
         <v>228</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -2618,10 +2618,10 @@
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -2633,7 +2633,7 @@
         <v>200</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2709,7 +2709,7 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="N26" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O26" s="8"/>
     </row>
@@ -3360,22 +3360,22 @@
     </row>
     <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
         <v>340</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>341</v>
       </c>
-      <c r="E47" t="s">
-        <v>342</v>
-      </c>
       <c r="F47" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -3386,10 +3386,10 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="L47" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="L47" s="10" t="s">
-        <v>344</v>
       </c>
       <c r="O47" s="8"/>
     </row>

</xml_diff>

<commit_message>
Updated dictionary and added some property data type tests based on rep term
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FFC74-635A-4CEB-8E1B-CFCC2B5B7B66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7BECCA-6C22-49AA-97C8-0F6AF1147C20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="361">
   <si>
     <t>Field</t>
   </si>
@@ -1072,6 +1072,42 @@
   </si>
   <si>
     <t>dea:DrugCodeSimpleType, fips:USCounty3DigitCodeSimpleType, hazmat:HazmatCodeSimpleType, usps:StreetSuffixCodeSimpleType, can:StreetDirectionCodeSimpleType</t>
+  </si>
+  <si>
+    <t>property_type_amount</t>
+  </si>
+  <si>
+    <t>Properties with an "Amount" representation term should have type nc:AmountType.</t>
+  </si>
+  <si>
+    <t>amounts</t>
+  </si>
+  <si>
+    <t>property_type_binaryObject</t>
+  </si>
+  <si>
+    <t>Properties with a "BinaryObject" representation term should have a binary simple-value data type.</t>
+  </si>
+  <si>
+    <t>binaries</t>
+  </si>
+  <si>
+    <t>property_type_indicator</t>
+  </si>
+  <si>
+    <t>Properties with an "Indicator" representation term should have a boolean data type.</t>
+  </si>
+  <si>
+    <t>property_type_percent</t>
+  </si>
+  <si>
+    <t>Properties with an "Percent" representation term should have data type "nc:PercentType".</t>
+  </si>
+  <si>
+    <t>indicators</t>
+  </si>
+  <si>
+    <t>percents</t>
   </si>
 </sst>
 </file>
@@ -1173,62 +1209,100 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="53">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1530,6 +1604,62 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1544,27 +1674,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O89" totalsRowShown="0">
-  <autoFilter ref="A1:O89" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:O84">
-    <sortCondition ref="A1:A84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O93" totalsRowShown="0">
+  <autoFilter ref="A1:O93" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:O88">
+    <sortCondition ref="A1:A88"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="52" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="51"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="50"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="49"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="48"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="46" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="45" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="44"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="43"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1833,13 +1963,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,12 +3372,12 @@
       <c r="J42" s="3"/>
       <c r="O42" s="8"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>166</v>
+    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>349</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>22</v>
+        <v>350</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>16</v>
@@ -3259,24 +3389,25 @@
         <v>205</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>209</v>
+        <v>351</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="J43"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
       <c r="O43" s="8"/>
     </row>
-    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>165</v>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>16</v>
@@ -3288,7 +3419,7 @@
         <v>205</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
@@ -3300,15 +3431,15 @@
       <c r="J44" s="3"/>
       <c r="O44" s="8"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>169</v>
+        <v>352</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>170</v>
+        <v>353</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -3317,27 +3448,29 @@
         <v>205</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>315</v>
+        <v>354</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
       <c r="O45" s="8"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>167</v>
+    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -3346,7 +3479,7 @@
         <v>205</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
@@ -3358,59 +3491,55 @@
       <c r="J46" s="3"/>
       <c r="O46" s="8"/>
     </row>
-    <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>340</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>341</v>
+        <v>205</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="L47" s="10" t="s">
-        <v>343</v>
-      </c>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
       <c r="O47" s="8"/>
     </row>
-    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>313</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3418,63 +3547,59 @@
       <c r="H48" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="O48" s="8"/>
     </row>
     <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>286</v>
+        <v>357</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>358</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>282</v>
+        <v>360</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>3</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>334</v>
+        <v>20</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="O49" s="8"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>33</v>
+        <v>199</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -3482,33 +3607,28 @@
       <c r="H50" t="s">
         <v>3</v>
       </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="O50" s="8"/>
+    </row>
+    <row r="51" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>111</v>
+        <v>344</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>339</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="E51" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>317</v>
+        <v>347</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3516,19 +3636,22 @@
       <c r="H51" t="s">
         <v>3</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="O51" s="8"/>
+    </row>
+    <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>276</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>16</v>
@@ -3540,30 +3663,27 @@
         <v>202</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>277</v>
+        <v>314</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
       </c>
       <c r="H52" t="s">
-        <v>20</v>
-      </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="O52" s="8"/>
-    </row>
-    <row r="53" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>335</v>
+        <v>286</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>16</v>
@@ -3575,32 +3695,30 @@
         <v>202</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>215</v>
+        <v>282</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
-      </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>264</v>
+        <v>109</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
@@ -3609,7 +3727,7 @@
         <v>202</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>216</v>
+        <v>33</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
@@ -3620,18 +3738,18 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>16</v>
@@ -3643,7 +3761,7 @@
         <v>202</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3651,18 +3769,22 @@
       <c r="H55" t="s">
         <v>3</v>
       </c>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
+      <c r="I55" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="56" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>107</v>
+        <v>336</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>276</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
@@ -3671,29 +3793,30 @@
         <v>202</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>199</v>
+        <v>277</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
-      <c r="K56" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="K56" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="O56" s="8"/>
+    </row>
+    <row r="57" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>298</v>
+        <v>148</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>16</v>
@@ -3702,10 +3825,10 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>282</v>
+        <v>215</v>
       </c>
       <c r="G57" t="s">
         <v>4</v>
@@ -3715,67 +3838,65 @@
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
-      <c r="K57" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="O57" s="8"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K57" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>267</v>
+        <v>337</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="8"/>
-    </row>
-    <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="K58" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B59" t="s">
-        <v>95</v>
+        <v>112</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>212</v>
+        <v>318</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -3783,34 +3904,27 @@
       <c r="H59" t="s">
         <v>3</v>
       </c>
-      <c r="I59" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="P59"/>
-    </row>
-    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
@@ -3818,24 +3932,24 @@
       <c r="H60" t="s">
         <v>3</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-    </row>
-    <row r="61" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>183</v>
+        <v>297</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>96</v>
+        <v>298</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
@@ -3844,7 +3958,7 @@
         <v>200</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>212</v>
+        <v>282</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
@@ -3852,28 +3966,28 @@
       <c r="H61" t="s">
         <v>20</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="L61" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="O61" s="8"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>184</v>
+        <v>267</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>97</v>
+        <v>268</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
@@ -3882,7 +3996,7 @@
         <v>200</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -3890,28 +4004,22 @@
       <c r="H62" t="s">
         <v>20</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="8"/>
+    </row>
+    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>98</v>
+        <v>181</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
@@ -3920,132 +4028,140 @@
         <v>200</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>20</v>
-      </c>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="L63" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="P63"/>
+    </row>
+    <row r="64" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>311</v>
+        <v>182</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>312</v>
+        <v>94</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
+      <c r="E64" t="s">
+        <v>200</v>
+      </c>
       <c r="F64" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>36</v>
-      </c>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="N64" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="O64" s="8"/>
-    </row>
-    <row r="65" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="L65" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="K65" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L65" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>69</v>
+        <v>184</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>3</v>
-      </c>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="K66" s="3" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>16</v>
@@ -4054,10 +4170,10 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
@@ -4068,21 +4184,18 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
       <c r="K67" s="3" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N67" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>63</v>
+        <v>311</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>16</v>
@@ -4090,9 +4203,6 @@
       <c r="D68" t="s">
         <v>1</v>
       </c>
-      <c r="E68" t="s">
-        <v>206</v>
-      </c>
       <c r="F68" s="2" t="s">
         <v>199</v>
       </c>
@@ -4100,30 +4210,26 @@
         <v>4</v>
       </c>
       <c r="H68" t="s">
-        <v>3</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="N68" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="O68" s="8"/>
+    </row>
+    <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
@@ -4132,7 +4238,7 @@
         <v>206</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
@@ -4144,20 +4250,24 @@
         <v>45</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
@@ -4166,7 +4276,7 @@
         <v>206</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
@@ -4174,24 +4284,24 @@
       <c r="H70" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>304</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>306</v>
+        <v>59</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
@@ -4200,29 +4310,35 @@
         <v>206</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="G71" t="s">
         <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="O71" s="8"/>
-    </row>
-    <row r="72" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>325</v>
+      <c r="K71" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N71" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
@@ -4231,7 +4347,7 @@
         <v>206</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>314</v>
+        <v>199</v>
       </c>
       <c r="G72" t="s">
         <v>4</v>
@@ -4239,24 +4355,28 @@
       <c r="H72" t="s">
         <v>3</v>
       </c>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
+      <c r="I72" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="K72" s="3" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>287</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
@@ -4265,7 +4385,7 @@
         <v>206</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>
@@ -4277,24 +4397,20 @@
         <v>45</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
@@ -4303,36 +4419,32 @@
         <v>206</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="G74" t="s">
         <v>4</v>
       </c>
       <c r="H74" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+    </row>
+    <row r="75" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>67</v>
+        <v>304</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>58</v>
+        <v>306</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
@@ -4341,36 +4453,26 @@
         <v>206</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="G75" t="s">
         <v>4</v>
       </c>
       <c r="H75" t="s">
-        <v>20</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L75" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N75" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="O75" s="8"/>
+    </row>
+    <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>325</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>6</v>
@@ -4382,7 +4484,7 @@
         <v>206</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>212</v>
+        <v>314</v>
       </c>
       <c r="G76" t="s">
         <v>4</v>
@@ -4393,18 +4495,18 @@
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="3" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>91</v>
+        <v>287</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>6</v>
@@ -4416,7 +4518,7 @@
         <v>206</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="G77" t="s">
         <v>4</v>
@@ -4424,21 +4526,25 @@
       <c r="H77" t="s">
         <v>3</v>
       </c>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
+      <c r="I77" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="K77" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>90</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>6</v>
@@ -4450,29 +4556,33 @@
         <v>206</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>317</v>
+        <v>211</v>
       </c>
       <c r="G78" t="s">
         <v>4</v>
       </c>
       <c r="H78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="K78" s="3" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>6</v>
@@ -4484,33 +4594,36 @@
         <v>206</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G79" t="s">
         <v>4</v>
       </c>
       <c r="H79" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="N79" s="8" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>6</v>
@@ -4522,7 +4635,7 @@
         <v>206</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="G80" t="s">
         <v>4</v>
@@ -4530,28 +4643,24 @@
       <c r="H80" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
       <c r="K80" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>71</v>
+      <c r="A81" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
@@ -4560,35 +4669,32 @@
         <v>206</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>199</v>
+        <v>319</v>
       </c>
       <c r="G81" t="s">
         <v>4</v>
       </c>
       <c r="H81" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
       <c r="K81" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="N81" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>92</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
@@ -4597,7 +4703,7 @@
         <v>206</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>199</v>
+        <v>317</v>
       </c>
       <c r="G82" t="s">
         <v>4</v>
@@ -4605,40 +4711,33 @@
       <c r="H82" t="s">
         <v>3</v>
       </c>
-      <c r="I82" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
       <c r="K82" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="O82" s="9" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="G83" t="s">
         <v>4</v>
@@ -4646,31 +4745,34 @@
       <c r="H83" t="s">
         <v>3</v>
       </c>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
+      <c r="I83" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="K83" s="3" t="s">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="O83" s="8"/>
-    </row>
-    <row r="84" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>199</v>
@@ -4681,22 +4783,25 @@
       <c r="H84" t="s">
         <v>3</v>
       </c>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
+      <c r="I84" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="K84" s="3" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="O84" s="8"/>
-    </row>
-    <row r="85" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>324</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>16</v>
@@ -4705,27 +4810,35 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>314</v>
+        <v>199</v>
       </c>
       <c r="G85" t="s">
         <v>4</v>
       </c>
       <c r="H85" t="s">
-        <v>3</v>
-      </c>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="O85" s="8"/>
-    </row>
-    <row r="86" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>288</v>
+        <v>20</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="N85" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>16</v>
@@ -4734,10 +4847,10 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>282</v>
+        <v>199</v>
       </c>
       <c r="G86" t="s">
         <v>4</v>
@@ -4745,28 +4858,40 @@
       <c r="H86" t="s">
         <v>3</v>
       </c>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="O86" s="8"/>
+      <c r="I86" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="O86" s="9" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="87" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>108</v>
+      <c r="A87" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>317</v>
+        <v>199</v>
       </c>
       <c r="G87" t="s">
         <v>4</v>
@@ -4774,25 +4899,31 @@
       <c r="H87" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L87" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="O87" s="8"/>
     </row>
-    <row r="88" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>199</v>
@@ -4806,19 +4937,19 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
       <c r="K88" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="O88" s="8"/>
     </row>
-    <row r="89" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>105</v>
+    <row r="89" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>324</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>16</v>
@@ -4830,7 +4961,7 @@
         <v>203</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>199</v>
+        <v>314</v>
       </c>
       <c r="G89" t="s">
         <v>4</v>
@@ -4838,139 +4969,280 @@
       <c r="H89" t="s">
         <v>3</v>
       </c>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="3" t="s">
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="O89" s="8"/>
+    </row>
+    <row r="90" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G90" t="s">
+        <v>4</v>
+      </c>
+      <c r="H90" t="s">
+        <v>3</v>
+      </c>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="O90" s="8"/>
+    </row>
+    <row r="91" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>203</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G91" t="s">
+        <v>4</v>
+      </c>
+      <c r="H91" t="s">
+        <v>3</v>
+      </c>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="O91" s="8"/>
+    </row>
+    <row r="92" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>203</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G92" t="s">
+        <v>4</v>
+      </c>
+      <c r="H92" t="s">
+        <v>3</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="O92" s="8"/>
+    </row>
+    <row r="93" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>203</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G93" t="s">
+        <v>4</v>
+      </c>
+      <c r="H93" t="s">
+        <v>3</v>
+      </c>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L89" s="3" t="s">
+      <c r="L93" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="O89" s="8"/>
+      <c r="O93" s="8"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P60:P63 P58 M90:O1048576 M20:O22 P72:P1048576 P65:P70 P3 P5:P18 P20:P55">
-    <cfRule type="cellIs" dxfId="42" priority="78" operator="equal">
+  <conditionalFormatting sqref="P64:P67 P62 M94:O1048576 M20:O22 P76:P1048576 P69:P74 P3 P5:P18 P20:P48 P50:P59">
+    <cfRule type="cellIs" dxfId="41" priority="88" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="89" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="90" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="91" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P60:P63 P58 M90:O1048576 M20:O22 P72:P1048576 P65:P70 P3 P5:P18 P20:P55">
-    <cfRule type="cellIs" dxfId="38" priority="53" operator="equal">
+  <conditionalFormatting sqref="P64:P67 P62 M94:O1048576 M20:O22 P76:P1048576 P69:P74 P3 P5:P18 P20:P48 P50:P59">
+    <cfRule type="cellIs" dxfId="37" priority="63" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P56:P57">
-    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
+  <conditionalFormatting sqref="P60:P61">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P56:P57">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+  <conditionalFormatting sqref="P60:P61">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="27" priority="17">
-      <formula>$A58&lt;&gt;""</formula>
+  <conditionalFormatting sqref="N62">
+    <cfRule type="expression" dxfId="26" priority="27">
+      <formula>$A62&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="26" priority="16">
-      <formula>$A57&lt;&gt;""</formula>
+  <conditionalFormatting sqref="N61">
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>$A61&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P71">
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+  <conditionalFormatting sqref="P75">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P71">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+  <conditionalFormatting sqref="P75">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P64">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+  <conditionalFormatting sqref="P68">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P64">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+  <conditionalFormatting sqref="P68">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"check"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P49">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"n/a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"to do"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P49">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated dependencies, dictionary, and exceptions
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7BECCA-6C22-49AA-97C8-0F6AF1147C20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D8FE07-9D2B-447B-ACF0-CB7BE3B393FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="362">
   <si>
     <t>Field</t>
   </si>
@@ -933,9 +933,6 @@
     <t>hs:ActivityInvolvedPersonAssociationAugmentationType</t>
   </si>
   <si>
-    <t>geo:LocationFeature, geo:LocationGeometry</t>
-  </si>
-  <si>
     <t>property_name_overlap</t>
   </si>
   <si>
@@ -1108,6 +1105,12 @@
   </si>
   <si>
     <t>percents</t>
+  </si>
+  <si>
+    <t>mo:CPENamePatternSimpleType</t>
+  </si>
+  <si>
+    <t>geo:LocationFeature, geo:LocationGeometry, mo:AngularMeasureDecimalValue, mo:CommentDestinationText, mo:CommentKeywordText</t>
   </si>
 </sst>
 </file>
@@ -1209,53 +1212,62 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="48">
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1604,62 +1616,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1680,21 +1636,21 @@
     <sortCondition ref="A1:A88"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="52" dataCellStyle="Good"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="51"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10" dataCellStyle="Good"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Category" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Component"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Field"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Scope" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Source"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Severity"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="48"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="46" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="45" dataCellStyle="Normal"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="44"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="43"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Spec" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Rule" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Valid Example" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Invalid Example" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Exceptions" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Exception IDs" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1966,10 +1922,10 @@
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2030,7 @@
         <v>197</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -2102,10 +2058,10 @@
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -2130,7 +2086,7 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="N4" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O4" s="8"/>
     </row>
@@ -2376,7 +2332,7 @@
         <v>228</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -2444,13 +2400,13 @@
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E14" t="s">
         <v>200</v>
@@ -2472,16 +2428,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" t="s">
         <v>330</v>
-      </c>
-      <c r="E15" t="s">
-        <v>331</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>199</v>
@@ -2500,16 +2456,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
+        <v>329</v>
+      </c>
+      <c r="E16" t="s">
         <v>330</v>
-      </c>
-      <c r="E16" t="s">
-        <v>331</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>199</v>
@@ -2528,16 +2484,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
         <v>329</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>330</v>
-      </c>
       <c r="E17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>199</v>
@@ -2556,16 +2512,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>199</v>
@@ -2748,10 +2704,10 @@
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -2763,7 +2719,7 @@
         <v>200</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G24" t="s">
         <v>4</v>
@@ -2814,10 +2770,10 @@
     </row>
     <row r="26" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -2839,7 +2795,7 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="N26" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O26" s="8"/>
     </row>
@@ -2935,7 +2891,7 @@
         <v>284</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="O29" s="8"/>
     </row>
@@ -3120,10 +3076,10 @@
     </row>
     <row r="35" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>18</v>
@@ -3302,7 +3258,7 @@
         <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G40" t="s">
         <v>4</v>
@@ -3331,7 +3287,7 @@
         <v>203</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G41" t="s">
         <v>4</v>
@@ -3360,7 +3316,7 @@
         <v>205</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -3374,10 +3330,10 @@
     </row>
     <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>16</v>
@@ -3389,7 +3345,7 @@
         <v>205</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -3433,10 +3389,10 @@
     </row>
     <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>16</v>
@@ -3448,7 +3404,7 @@
         <v>205</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -3493,10 +3449,10 @@
     </row>
     <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>16</v>
@@ -3508,7 +3464,7 @@
         <v>205</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -3539,7 +3495,7 @@
         <v>205</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -3553,10 +3509,10 @@
     </row>
     <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>16</v>
@@ -3568,7 +3524,7 @@
         <v>205</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -3613,22 +3569,22 @@
     </row>
     <row r="51" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
         <v>339</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>340</v>
       </c>
-      <c r="E51" t="s">
-        <v>341</v>
-      </c>
       <c r="F51" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
@@ -3639,16 +3595,16 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="L51" s="10" t="s">
         <v>342</v>
-      </c>
-      <c r="L51" s="10" t="s">
-        <v>343</v>
       </c>
       <c r="O51" s="8"/>
     </row>
     <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>114</v>
@@ -3663,7 +3619,7 @@
         <v>202</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G52" t="s">
         <v>4</v>
@@ -3712,7 +3668,7 @@
     </row>
     <row r="54" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>109</v>
@@ -3761,7 +3717,7 @@
         <v>202</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
@@ -3778,7 +3734,7 @@
     </row>
     <row r="56" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>276</v>
@@ -3813,7 +3769,7 @@
     </row>
     <row r="57" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>148</v>
@@ -3844,10 +3800,13 @@
       <c r="L57" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="M57" s="8" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="58" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>264</v>
@@ -3896,7 +3855,7 @@
         <v>202</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
@@ -4192,10 +4151,10 @@
     </row>
     <row r="68" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>16</v>
@@ -4217,7 +4176,7 @@
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
       <c r="N68" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O68" s="8"/>
     </row>
@@ -4438,10 +4397,10 @@
     </row>
     <row r="75" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>18</v>
@@ -4469,7 +4428,7 @@
     </row>
     <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>55</v>
@@ -4484,7 +4443,7 @@
         <v>206</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G76" t="s">
         <v>4</v>
@@ -4669,7 +4628,7 @@
         <v>206</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G81" t="s">
         <v>4</v>
@@ -4703,7 +4662,7 @@
         <v>206</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G82" t="s">
         <v>4</v>
@@ -4946,7 +4905,7 @@
     </row>
     <row r="89" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>102</v>
@@ -4961,7 +4920,7 @@
         <v>203</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G89" t="s">
         <v>4</v>
@@ -5019,7 +4978,7 @@
         <v>203</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G91" t="s">
         <v>4</v>
@@ -5104,145 +5063,145 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="P64:P67 P62 M94:O1048576 M20:O22 P76:P1048576 P69:P74 P3 P5:P18 P20:P48 P50:P59">
-    <cfRule type="cellIs" dxfId="41" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="88" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="89" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="90" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="91" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P64:P67 P62 M94:O1048576 M20:O22 P76:P1048576 P69:P74 P3 P5:P18 P20:P48 P50:P59">
-    <cfRule type="cellIs" dxfId="37" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="63" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P60:P61">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="35" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P60:P61">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="33" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="28" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N62">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="32" priority="27">
       <formula>$A62&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N61">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="31" priority="26">
       <formula>$A61&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P75">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P75">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P68">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P68">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated to use new niem-model type defs and to fix typescript error-reporting issues
</commit_message>
<xml_diff>
--- a/niem-model-qa-tests.xlsx
+++ b/niem-model-qa-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D8FE07-9D2B-447B-ACF0-CB7BE3B393FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1E561F-314A-4792-AACB-57100EC5878D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="363">
   <si>
     <t>Field</t>
   </si>
@@ -1111,6 +1111,9 @@
   </si>
   <si>
     <t>geo:LocationFeature, geo:LocationGeometry, mo:AngularMeasureDecimalValue, mo:CommentDestinationText, mo:CommentKeywordText</t>
+  </si>
+  <si>
+    <t>NDR-4.0</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1634,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O93" totalsRowShown="0">
-  <autoFilter ref="A1:O93" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A1:O93" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Type"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:O88">
     <sortCondition ref="A1:A88"/>
   </sortState>
@@ -1922,10 +1931,10 @@
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
+      <selection pane="bottomRight" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +2002,7 @@
       </c>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>195</v>
       </c>
@@ -2025,7 +2034,7 @@
       <c r="O2" s="8"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>197</v>
       </c>
@@ -2056,7 +2065,7 @@
       <c r="L3" s="10"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>319</v>
       </c>
@@ -2090,7 +2099,7 @@
       </c>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>186</v>
       </c>
@@ -2129,7 +2138,7 @@
       </c>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>187</v>
       </c>
@@ -2164,7 +2173,7 @@
       </c>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>158</v>
       </c>
@@ -2193,7 +2202,7 @@
       <c r="J7" s="5"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -2228,7 +2237,7 @@
       </c>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>218</v>
       </c>
@@ -2267,7 +2276,7 @@
       </c>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>155</v>
       </c>
@@ -2298,7 +2307,7 @@
       <c r="L10" s="5"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>226</v>
       </c>
@@ -2336,7 +2345,7 @@
       </c>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>271</v>
       </c>
@@ -2367,7 +2376,7 @@
       <c r="L12" s="10"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>157</v>
       </c>
@@ -2398,7 +2407,7 @@
       <c r="L13" s="5"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>325</v>
       </c>
@@ -2426,7 +2435,7 @@
       <c r="L14" s="10"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>327</v>
       </c>
@@ -2454,7 +2463,7 @@
       <c r="L15" s="10"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>326</v>
       </c>
@@ -2482,7 +2491,7 @@
       <c r="L16" s="10"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>328</v>
       </c>
@@ -2510,7 +2519,7 @@
       <c r="L17" s="10"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>332</v>
       </c>
@@ -2538,7 +2547,7 @@
       <c r="L18" s="10"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>269</v>
       </c>
@@ -2569,7 +2578,7 @@
       <c r="L19" s="10"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>261</v>
       </c>
@@ -2600,7 +2609,7 @@
       <c r="L20" s="10"/>
       <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>289</v>
       </c>
@@ -2638,7 +2647,7 @@
       </c>
       <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>290</v>
       </c>
@@ -2671,7 +2680,7 @@
       <c r="L22" s="10"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>265</v>
       </c>
@@ -2702,7 +2711,7 @@
       <c r="L23" s="10"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>344</v>
       </c>
@@ -2733,7 +2742,7 @@
       <c r="L24" s="10"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>163</v>
       </c>
@@ -2768,7 +2777,7 @@
       </c>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>309</v>
       </c>
@@ -2799,7 +2808,7 @@
       </c>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>171</v>
       </c>
@@ -2828,7 +2837,7 @@
       <c r="J27" s="3"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>168</v>
       </c>
@@ -2857,7 +2866,7 @@
       <c r="J28" s="3"/>
       <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>280</v>
       </c>
@@ -2895,7 +2904,7 @@
       </c>
       <c r="O29" s="8"/>
     </row>
-    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>161</v>
       </c>
@@ -2934,7 +2943,7 @@
       </c>
       <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>160</v>
       </c>
@@ -2973,7 +2982,7 @@
       </c>
       <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>159</v>
       </c>
@@ -3004,7 +3013,7 @@
       <c r="L32" s="5"/>
       <c r="O32" s="8"/>
     </row>
-    <row r="33" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>239</v>
       </c>
@@ -3043,7 +3052,7 @@
       </c>
       <c r="O33" s="8"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>249</v>
       </c>
@@ -3074,7 +3083,7 @@
       <c r="L34" s="5"/>
       <c r="O34" s="8"/>
     </row>
-    <row r="35" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>302</v>
       </c>
@@ -3105,7 +3114,7 @@
       <c r="L35" s="10"/>
       <c r="O35" s="8"/>
     </row>
-    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>162</v>
       </c>
@@ -3144,7 +3153,7 @@
       </c>
       <c r="O36" s="8"/>
     </row>
-    <row r="37" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>285</v>
       </c>
@@ -3179,7 +3188,7 @@
       </c>
       <c r="O37" s="8"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>255</v>
       </c>
@@ -3210,7 +3219,7 @@
       <c r="L38" s="5"/>
       <c r="O38" s="8"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>250</v>
       </c>
@@ -3241,7 +3250,7 @@
       <c r="L39" s="5"/>
       <c r="O39" s="8"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>172</v>
       </c>
@@ -3270,7 +3279,7 @@
       <c r="J40" s="3"/>
       <c r="O40" s="8"/>
     </row>
-    <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>173</v>
       </c>
@@ -3299,7 +3308,7 @@
       <c r="J41" s="3"/>
       <c r="O41" s="8"/>
     </row>
-    <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>164</v>
       </c>
@@ -3328,7 +3337,7 @@
       <c r="J42" s="3"/>
       <c r="O42" s="8"/>
     </row>
-    <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>348</v>
       </c>
@@ -3358,7 +3367,7 @@
       <c r="L43" s="11"/>
       <c r="O43" s="8"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>166</v>
       </c>
@@ -3387,7 +3396,7 @@
       <c r="J44" s="3"/>
       <c r="O44" s="8"/>
     </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>351</v>
       </c>
@@ -3418,7 +3427,7 @@
       <c r="L45" s="11"/>
       <c r="O45" s="8"/>
     </row>
-    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>165</v>
       </c>
@@ -3447,7 +3456,7 @@
       <c r="J46" s="3"/>
       <c r="O46" s="8"/>
     </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>354</v>
       </c>
@@ -3478,7 +3487,7 @@
       <c r="L47" s="10"/>
       <c r="O47" s="8"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>169</v>
       </c>
@@ -3507,7 +3516,7 @@
       <c r="J48" s="3"/>
       <c r="O48" s="8"/>
     </row>
-    <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>356</v>
       </c>
@@ -3538,7 +3547,7 @@
       <c r="L49" s="10"/>
       <c r="O49" s="8"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>167</v>
       </c>
@@ -3567,7 +3576,7 @@
       <c r="J50" s="3"/>
       <c r="O50" s="8"/>
     </row>
-    <row r="51" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>343</v>
       </c>
@@ -3628,7 +3637,7 @@
         <v>3</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>133</v>
@@ -3660,7 +3669,7 @@
         <v>3</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>134</v>
@@ -3726,7 +3735,7 @@
         <v>3</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>135</v>
@@ -3800,7 +3809,7 @@
       <c r="L57" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M57" s="8" t="s">
+      <c r="N57" s="8" t="s">
         <v>360</v>
       </c>
     </row>
@@ -3996,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>42</v>
@@ -4031,7 +4040,7 @@
         <v>3</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>41</v>
@@ -4065,7 +4074,7 @@
         <v>20</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>43</v>
@@ -4103,7 +4112,7 @@
         <v>20</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>44</v>
@@ -4206,7 +4215,7 @@
         <v>3</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>32</v>
@@ -4315,7 +4324,7 @@
         <v>3</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>28</v>
@@ -4353,7 +4362,7 @@
         <v>3</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>37</v>
@@ -4387,7 +4396,7 @@
         <v>3</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>38</v>
@@ -4486,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>132</v>
@@ -4524,7 +4533,7 @@
         <v>20</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>40</v>
@@ -4562,7 +4571,7 @@
         <v>20</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>31</v>
@@ -4705,7 +4714,7 @@
         <v>3</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>30</v>
@@ -4743,7 +4752,7 @@
         <v>3</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>29</v>
@@ -4818,7 +4827,7 @@
         <v>3</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>136</v>

</xml_diff>